<commit_message>
Update funding data 2026-02-14
</commit_message>
<xml_diff>
--- a/docs/resultados_convocatorias.xlsx
+++ b/docs/resultados_convocatorias.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Recursos" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen'!$A$4:$M$75</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Seguimiento'!$A$1:$J$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen'!$A$4:$M$84</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Seguimiento'!$A$1:$J$79</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -657,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M75"/>
+  <dimension ref="A1:M84"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -691,7 +691,7 @@
     <row r="2" ht="22" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Mision Climatica - Neutralidad 2030 - Actualizado: 13/02/2026 08:13 - 69 convocatorias - 15 nuevas</t>
+          <t>Mision Climatica - Neutralidad 2030 - Actualizado: 14/02/2026 07:52 - 78 convocatorias - 24 nuevas</t>
         </is>
       </c>
     </row>
@@ -3894,7 +3894,7 @@
       </c>
       <c r="B61" s="6" t="inlineStr">
         <is>
-          <t>EUS-15293</t>
+          <t>EUS-89962</t>
         </is>
       </c>
       <c r="C61" s="6" t="inlineStr">
@@ -3949,7 +3949,7 @@
       </c>
       <c r="B62" s="6" t="inlineStr">
         <is>
-          <t>EUS-60835</t>
+          <t>EUS-51969</t>
         </is>
       </c>
       <c r="C62" s="6" t="inlineStr">
@@ -4004,7 +4004,7 @@
       </c>
       <c r="B63" s="6" t="inlineStr">
         <is>
-          <t>EUS-59232</t>
+          <t>EUS-56284</t>
         </is>
       </c>
       <c r="C63" s="6" t="inlineStr">
@@ -4059,7 +4059,7 @@
       </c>
       <c r="B64" s="6" t="inlineStr">
         <is>
-          <t>EUS-36628</t>
+          <t>EUS-28861</t>
         </is>
       </c>
       <c r="C64" s="6" t="inlineStr">
@@ -4114,7 +4114,7 @@
       </c>
       <c r="B65" s="6" t="inlineStr">
         <is>
-          <t>EUS-18488</t>
+          <t>EUS-17841</t>
         </is>
       </c>
       <c r="C65" s="6" t="inlineStr">
@@ -4169,12 +4169,12 @@
       </c>
       <c r="B66" s="6" t="inlineStr">
         <is>
-          <t>EUS-87234</t>
+          <t>EUS-27002</t>
         </is>
       </c>
       <c r="C66" s="6" t="inlineStr">
         <is>
-          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
+          <t>Asesoría Legal - Consultas tramitación de proyectos de energías renovables y, en especial, en materia medioambiental</t>
         </is>
       </c>
       <c r="D66" s="6" t="inlineStr">
@@ -4191,12 +4191,12 @@
       <c r="G66" s="6" t="inlineStr"/>
       <c r="H66" s="6" t="inlineStr">
         <is>
-          <t>Ayuda/Subvencion Euskadi</t>
-        </is>
-      </c>
-      <c r="I66" s="10" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I66" s="8" t="inlineStr">
+        <is>
+          <t>ALTA</t>
         </is>
       </c>
       <c r="J66" s="6" t="inlineStr"/>
@@ -4224,12 +4224,12 @@
       </c>
       <c r="B67" s="6" t="inlineStr">
         <is>
-          <t>EUS-73772</t>
+          <t>EUS-18210</t>
         </is>
       </c>
       <c r="C67" s="6" t="inlineStr">
         <is>
-          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
+          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
         </is>
       </c>
       <c r="D67" s="6" t="inlineStr">
@@ -4279,12 +4279,12 @@
       </c>
       <c r="B68" s="6" t="inlineStr">
         <is>
-          <t>EUS-49109</t>
+          <t>EUS-59993</t>
         </is>
       </c>
       <c r="C68" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
+          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
         </is>
       </c>
       <c r="D68" s="6" t="inlineStr">
@@ -4334,12 +4334,12 @@
       </c>
       <c r="B69" s="6" t="inlineStr">
         <is>
-          <t>EUS-72760</t>
+          <t>EUS-25797</t>
         </is>
       </c>
       <c r="C69" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
+          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
         </is>
       </c>
       <c r="D69" s="6" t="inlineStr">
@@ -4389,12 +4389,12 @@
       </c>
       <c r="B70" s="6" t="inlineStr">
         <is>
-          <t>EUS-28905</t>
+          <t>EUS-12160</t>
         </is>
       </c>
       <c r="C70" s="6" t="inlineStr">
         <is>
-          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
+          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
         </is>
       </c>
       <c r="D70" s="6" t="inlineStr">
@@ -4444,12 +4444,12 @@
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>EUS-54869</t>
+          <t>EUS-77123</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
         <is>
-          <t>Subvenciones para innovación en economía circular 2026</t>
+          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
         </is>
       </c>
       <c r="D71" s="6" t="inlineStr">
@@ -4499,12 +4499,12 @@
       </c>
       <c r="B72" s="6" t="inlineStr">
         <is>
-          <t>EUS-95967</t>
+          <t>EUS-64792</t>
         </is>
       </c>
       <c r="C72" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
+          <t>Subvenciones para innovación en economía circular 2026</t>
         </is>
       </c>
       <c r="D72" s="6" t="inlineStr">
@@ -4554,12 +4554,12 @@
       </c>
       <c r="B73" s="6" t="inlineStr">
         <is>
-          <t>EUS-17430</t>
+          <t>EUS-00130</t>
         </is>
       </c>
       <c r="C73" s="6" t="inlineStr">
         <is>
-          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
+          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
         </is>
       </c>
       <c r="D73" s="6" t="inlineStr">
@@ -4609,12 +4609,12 @@
       </c>
       <c r="B74" s="6" t="inlineStr">
         <is>
-          <t>EUS-18205</t>
+          <t>EUS-83114</t>
         </is>
       </c>
       <c r="C74" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
+          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
         </is>
       </c>
       <c r="D74" s="6" t="inlineStr">
@@ -4664,12 +4664,12 @@
       </c>
       <c r="B75" s="6" t="inlineStr">
         <is>
-          <t>EUS-12970</t>
+          <t>EUS-36808</t>
         </is>
       </c>
       <c r="C75" s="6" t="inlineStr">
         <is>
-          <t>Asignaciones individualizadas de transporte escolar para el curso 2025-2026 del alumnado de los centros docentes públicos no universitarios de la Comunidad Autónoma del País Vasco financiado por el de</t>
+          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
         </is>
       </c>
       <c r="D75" s="6" t="inlineStr">
@@ -4711,8 +4711,503 @@
         </is>
       </c>
     </row>
+    <row r="76" ht="40" customHeight="1">
+      <c r="A76" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B76" s="6" t="inlineStr">
+        <is>
+          <t>EUS-28459</t>
+        </is>
+      </c>
+      <c r="C76" s="6" t="inlineStr">
+        <is>
+          <t>Asignaciones individualizadas de transporte escolar para el curso 2025-2026 del alumnado de los centros docentes públicos no universitarios de la Comunidad Autónoma del País Vasco financiado por el de</t>
+        </is>
+      </c>
+      <c r="D76" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E76" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F76" s="6" t="inlineStr"/>
+      <c r="G76" s="6" t="inlineStr"/>
+      <c r="H76" s="6" t="inlineStr">
+        <is>
+          <t>Ayuda/Subvencion Euskadi</t>
+        </is>
+      </c>
+      <c r="I76" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J76" s="6" t="inlineStr"/>
+      <c r="K76" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L76" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M76" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="77" ht="40" customHeight="1">
+      <c r="A77" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>EUS-68968</t>
+        </is>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>Mantenimiento preventivo de 10 grúas de techo ubicadas en el edificio de hospitalización de la OSI Debagoiena</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E77" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F77" s="6" t="inlineStr"/>
+      <c r="G77" s="6" t="inlineStr"/>
+      <c r="H77" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I77" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J77" s="6" t="inlineStr"/>
+      <c r="K77" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L77" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M77" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="78" ht="40" customHeight="1">
+      <c r="A78" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B78" s="6" t="inlineStr">
+        <is>
+          <t>EUS-40629</t>
+        </is>
+      </c>
+      <c r="C78" s="6" t="inlineStr">
+        <is>
+          <t>Asesoría Legal - Asesoramiento legal contestación borofax Solaria y análisis terrenos Indarberri</t>
+        </is>
+      </c>
+      <c r="D78" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E78" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F78" s="6" t="inlineStr"/>
+      <c r="G78" s="6" t="inlineStr"/>
+      <c r="H78" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I78" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J78" s="6" t="inlineStr"/>
+      <c r="K78" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L78" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M78" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="79" ht="40" customHeight="1">
+      <c r="A79" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>EUS-35956</t>
+        </is>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>Otras Consultorías/ Servicios - Asesoramiento en la valoración de plantas fotovoltaicas</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E79" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F79" s="6" t="inlineStr"/>
+      <c r="G79" s="6" t="inlineStr"/>
+      <c r="H79" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I79" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J79" s="6" t="inlineStr"/>
+      <c r="K79" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L79" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M79" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="80" ht="40" customHeight="1">
+      <c r="A80" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B80" s="6" t="inlineStr">
+        <is>
+          <t>EUS-21012</t>
+        </is>
+      </c>
+      <c r="C80" s="6" t="inlineStr">
+        <is>
+          <t>Otras Consultorías/ Servicios - Asesoramiento en la valoración de plantas fotovoltaicas</t>
+        </is>
+      </c>
+      <c r="D80" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E80" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F80" s="6" t="inlineStr"/>
+      <c r="G80" s="6" t="inlineStr"/>
+      <c r="H80" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I80" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J80" s="6" t="inlineStr"/>
+      <c r="K80" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L80" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M80" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="81" ht="40" customHeight="1">
+      <c r="A81" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B81" s="6" t="inlineStr">
+        <is>
+          <t>EUS-80336</t>
+        </is>
+      </c>
+      <c r="C81" s="6" t="inlineStr">
+        <is>
+          <t>Asesoría Legal - Asesoramiento en negociación proyecto plantas fotovoltaicas</t>
+        </is>
+      </c>
+      <c r="D81" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E81" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F81" s="6" t="inlineStr"/>
+      <c r="G81" s="6" t="inlineStr"/>
+      <c r="H81" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J81" s="6" t="inlineStr"/>
+      <c r="K81" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L81" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M81" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="82" ht="40" customHeight="1">
+      <c r="A82" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B82" s="6" t="inlineStr">
+        <is>
+          <t>EUS-82751</t>
+        </is>
+      </c>
+      <c r="C82" s="6" t="inlineStr">
+        <is>
+          <t>Limpieza de foso ascensor san juan mekola</t>
+        </is>
+      </c>
+      <c r="D82" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E82" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F82" s="6" t="inlineStr"/>
+      <c r="G82" s="6" t="inlineStr"/>
+      <c r="H82" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I82" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J82" s="6" t="inlineStr"/>
+      <c r="K82" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L82" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M82" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="83" ht="40" customHeight="1">
+      <c r="A83" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B83" s="6" t="inlineStr">
+        <is>
+          <t>EUS-08134</t>
+        </is>
+      </c>
+      <c r="C83" s="6" t="inlineStr">
+        <is>
+          <t>Limpieza sumideros de errebal</t>
+        </is>
+      </c>
+      <c r="D83" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E83" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F83" s="6" t="inlineStr"/>
+      <c r="G83" s="6" t="inlineStr"/>
+      <c r="H83" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I83" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J83" s="6" t="inlineStr"/>
+      <c r="K83" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L83" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M83" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
+    <row r="84" ht="40" customHeight="1">
+      <c r="A84" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B84" s="6" t="inlineStr">
+        <is>
+          <t>EUS-92185</t>
+        </is>
+      </c>
+      <c r="C84" s="6" t="inlineStr">
+        <is>
+          <t>Reparación de cableados de circuitos de fuerza y alumbrado que se encuentran requemados y sin aislamiento en el fronton astelena</t>
+        </is>
+      </c>
+      <c r="D84" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E84" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F84" s="6" t="inlineStr"/>
+      <c r="G84" s="6" t="inlineStr"/>
+      <c r="H84" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I84" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J84" s="6" t="inlineStr"/>
+      <c r="K84" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L84" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M84" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:M75"/>
+  <autoFilter ref="A4:M84"/>
   <mergeCells count="4">
     <mergeCell ref="A60:M60"/>
     <mergeCell ref="A2:M2"/>
@@ -4789,6 +5284,15 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M73" r:id="rId67"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M74" r:id="rId68"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M75" r:id="rId69"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M76" r:id="rId70"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M77" r:id="rId71"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M78" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M79" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M80" r:id="rId74"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M81" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M82" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M83" r:id="rId77"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M84" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -4800,7 +5304,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1034"/>
+  <dimension ref="A1:F1169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16447,7 +16951,7 @@
     <row r="811" ht="30" customHeight="1">
       <c r="A811" s="16" t="inlineStr">
         <is>
-          <t>FICHA 55: EUS-15293</t>
+          <t>FICHA 55: EUS-89962</t>
         </is>
       </c>
       <c r="B811" s="17" t="n"/>
@@ -16496,7 +17000,7 @@
       </c>
       <c r="B814" s="19" t="inlineStr">
         <is>
-          <t>EUS-15293</t>
+          <t>EUS-89962</t>
         </is>
       </c>
       <c r="C814" s="20" t="n"/>
@@ -16659,7 +17163,7 @@
     <row r="826" ht="30" customHeight="1">
       <c r="A826" s="16" t="inlineStr">
         <is>
-          <t>FICHA 56: EUS-60835</t>
+          <t>FICHA 56: EUS-51969</t>
         </is>
       </c>
       <c r="B826" s="17" t="n"/>
@@ -16708,7 +17212,7 @@
       </c>
       <c r="B829" s="19" t="inlineStr">
         <is>
-          <t>EUS-60835</t>
+          <t>EUS-51969</t>
         </is>
       </c>
       <c r="C829" s="20" t="n"/>
@@ -16871,7 +17375,7 @@
     <row r="841" ht="30" customHeight="1">
       <c r="A841" s="16" t="inlineStr">
         <is>
-          <t>FICHA 57: EUS-59232</t>
+          <t>FICHA 57: EUS-56284</t>
         </is>
       </c>
       <c r="B841" s="17" t="n"/>
@@ -16920,7 +17424,7 @@
       </c>
       <c r="B844" s="19" t="inlineStr">
         <is>
-          <t>EUS-59232</t>
+          <t>EUS-56284</t>
         </is>
       </c>
       <c r="C844" s="20" t="n"/>
@@ -17083,7 +17587,7 @@
     <row r="856" ht="30" customHeight="1">
       <c r="A856" s="16" t="inlineStr">
         <is>
-          <t>FICHA 58: EUS-36628</t>
+          <t>FICHA 58: EUS-28861</t>
         </is>
       </c>
       <c r="B856" s="17" t="n"/>
@@ -17132,7 +17636,7 @@
       </c>
       <c r="B859" s="19" t="inlineStr">
         <is>
-          <t>EUS-36628</t>
+          <t>EUS-28861</t>
         </is>
       </c>
       <c r="C859" s="20" t="n"/>
@@ -17295,7 +17799,7 @@
     <row r="871" ht="30" customHeight="1">
       <c r="A871" s="16" t="inlineStr">
         <is>
-          <t>FICHA 59: EUS-18488</t>
+          <t>FICHA 59: EUS-17841</t>
         </is>
       </c>
       <c r="B871" s="17" t="n"/>
@@ -17344,7 +17848,7 @@
       </c>
       <c r="B874" s="19" t="inlineStr">
         <is>
-          <t>EUS-18488</t>
+          <t>EUS-17841</t>
         </is>
       </c>
       <c r="C874" s="20" t="n"/>
@@ -17507,7 +18011,7 @@
     <row r="886" ht="30" customHeight="1">
       <c r="A886" s="16" t="inlineStr">
         <is>
-          <t>FICHA 60: EUS-87234</t>
+          <t>FICHA 60: EUS-27002</t>
         </is>
       </c>
       <c r="B886" s="17" t="n"/>
@@ -17540,7 +18044,7 @@
       </c>
       <c r="B888" s="19" t="inlineStr">
         <is>
-          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
+          <t>Asesoría Legal - Consultas tramitación de proyectos de energías renovables y, en especial, en materia medioambiental</t>
         </is>
       </c>
       <c r="C888" s="20" t="n"/>
@@ -17556,7 +18060,7 @@
       </c>
       <c r="B889" s="19" t="inlineStr">
         <is>
-          <t>EUS-87234</t>
+          <t>EUS-27002</t>
         </is>
       </c>
       <c r="C889" s="20" t="n"/>
@@ -17632,7 +18136,7 @@
       </c>
       <c r="B894" s="19" t="inlineStr">
         <is>
-          <t>Ayuda/Subvencion Euskadi</t>
+          <t>Licitacion Euskadi</t>
         </is>
       </c>
       <c r="C894" s="20" t="n"/>
@@ -17690,9 +18194,9 @@
           <t>Relevancia Bilbao</t>
         </is>
       </c>
-      <c r="B898" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MEDIA — </t>
+      <c r="B898" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALTA — </t>
         </is>
       </c>
       <c r="C898" s="20" t="n"/>
@@ -17708,7 +18212,7 @@
       </c>
       <c r="B899" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260204smartcities/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/asesoria-legal-consultas-tramitacion-proyectos-energias-renovables-y-especial-materia-medioambiental/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C899" s="20" t="n"/>
@@ -17719,7 +18223,7 @@
     <row r="901" ht="30" customHeight="1">
       <c r="A901" s="16" t="inlineStr">
         <is>
-          <t>FICHA 61: EUS-73772</t>
+          <t>FICHA 61: EUS-18210</t>
         </is>
       </c>
       <c r="B901" s="17" t="n"/>
@@ -17752,7 +18256,7 @@
       </c>
       <c r="B903" s="19" t="inlineStr">
         <is>
-          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
+          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
         </is>
       </c>
       <c r="C903" s="20" t="n"/>
@@ -17768,7 +18272,7 @@
       </c>
       <c r="B904" s="19" t="inlineStr">
         <is>
-          <t>EUS-73772</t>
+          <t>EUS-18210</t>
         </is>
       </c>
       <c r="C904" s="20" t="n"/>
@@ -17920,7 +18424,7 @@
       </c>
       <c r="B914" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260119nextlanbidedigital/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260204smartcities/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C914" s="20" t="n"/>
@@ -17931,7 +18435,7 @@
     <row r="916" ht="30" customHeight="1">
       <c r="A916" s="16" t="inlineStr">
         <is>
-          <t>FICHA 62: EUS-49109</t>
+          <t>FICHA 62: EUS-59993</t>
         </is>
       </c>
       <c r="B916" s="17" t="n"/>
@@ -17964,7 +18468,7 @@
       </c>
       <c r="B918" s="19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
+          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
         </is>
       </c>
       <c r="C918" s="20" t="n"/>
@@ -17980,7 +18484,7 @@
       </c>
       <c r="B919" s="19" t="inlineStr">
         <is>
-          <t>EUS-49109</t>
+          <t>EUS-59993</t>
         </is>
       </c>
       <c r="C919" s="20" t="n"/>
@@ -18132,7 +18636,7 @@
       </c>
       <c r="B929" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/250119horizondiginduspaceklust/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260119nextlanbidedigital/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C929" s="20" t="n"/>
@@ -18143,7 +18647,7 @@
     <row r="931" ht="30" customHeight="1">
       <c r="A931" s="16" t="inlineStr">
         <is>
-          <t>FICHA 63: EUS-72760</t>
+          <t>FICHA 63: EUS-25797</t>
         </is>
       </c>
       <c r="B931" s="17" t="n"/>
@@ -18176,7 +18680,7 @@
       </c>
       <c r="B933" s="19" t="inlineStr">
         <is>
-          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
+          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
         </is>
       </c>
       <c r="C933" s="20" t="n"/>
@@ -18192,7 +18696,7 @@
       </c>
       <c r="B934" s="19" t="inlineStr">
         <is>
-          <t>EUS-72760</t>
+          <t>EUS-25797</t>
         </is>
       </c>
       <c r="C934" s="20" t="n"/>
@@ -18344,7 +18848,7 @@
       </c>
       <c r="B944" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/horizonkluster5hirimisioa/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/250119horizondiginduspaceklust/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C944" s="20" t="n"/>
@@ -18355,7 +18859,7 @@
     <row r="946" ht="30" customHeight="1">
       <c r="A946" s="16" t="inlineStr">
         <is>
-          <t>FICHA 64: EUS-28905</t>
+          <t>FICHA 64: EUS-12160</t>
         </is>
       </c>
       <c r="B946" s="17" t="n"/>
@@ -18388,7 +18892,7 @@
       </c>
       <c r="B948" s="19" t="inlineStr">
         <is>
-          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
+          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
         </is>
       </c>
       <c r="C948" s="20" t="n"/>
@@ -18404,7 +18908,7 @@
       </c>
       <c r="B949" s="19" t="inlineStr">
         <is>
-          <t>EUS-28905</t>
+          <t>EUS-12160</t>
         </is>
       </c>
       <c r="C949" s="20" t="n"/>
@@ -18556,7 +19060,7 @@
       </c>
       <c r="B959" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/azpitek-2026-programa-de-ayudas/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/horizonkluster5hirimisioa/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C959" s="20" t="n"/>
@@ -18567,7 +19071,7 @@
     <row r="961" ht="30" customHeight="1">
       <c r="A961" s="16" t="inlineStr">
         <is>
-          <t>FICHA 65: EUS-54869</t>
+          <t>FICHA 65: EUS-77123</t>
         </is>
       </c>
       <c r="B961" s="17" t="n"/>
@@ -18592,7 +19096,7 @@
       <c r="E962" s="20" t="n"/>
       <c r="F962" s="20" t="n"/>
     </row>
-    <row r="963" ht="20" customHeight="1">
+    <row r="963" ht="45" customHeight="1">
       <c r="A963" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -18600,7 +19104,7 @@
       </c>
       <c r="B963" s="19" t="inlineStr">
         <is>
-          <t>Subvenciones para innovación en economía circular 2026</t>
+          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
         </is>
       </c>
       <c r="C963" s="20" t="n"/>
@@ -18616,7 +19120,7 @@
       </c>
       <c r="B964" s="19" t="inlineStr">
         <is>
-          <t>EUS-54869</t>
+          <t>EUS-77123</t>
         </is>
       </c>
       <c r="C964" s="20" t="n"/>
@@ -18768,7 +19272,7 @@
       </c>
       <c r="B974" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/subvenciones-para-innovacion-en-economia-circular-2026/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/azpitek-2026-programa-de-ayudas/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C974" s="20" t="n"/>
@@ -18779,7 +19283,7 @@
     <row r="976" ht="30" customHeight="1">
       <c r="A976" s="16" t="inlineStr">
         <is>
-          <t>FICHA 66: EUS-95967</t>
+          <t>FICHA 66: EUS-64792</t>
         </is>
       </c>
       <c r="B976" s="17" t="n"/>
@@ -18804,7 +19308,7 @@
       <c r="E977" s="20" t="n"/>
       <c r="F977" s="20" t="n"/>
     </row>
-    <row r="978" ht="45" customHeight="1">
+    <row r="978" ht="20" customHeight="1">
       <c r="A978" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -18812,7 +19316,7 @@
       </c>
       <c r="B978" s="19" t="inlineStr">
         <is>
-          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
+          <t>Subvenciones para innovación en economía circular 2026</t>
         </is>
       </c>
       <c r="C978" s="20" t="n"/>
@@ -18828,7 +19332,7 @@
       </c>
       <c r="B979" s="19" t="inlineStr">
         <is>
-          <t>EUS-95967</t>
+          <t>EUS-64792</t>
         </is>
       </c>
       <c r="C979" s="20" t="n"/>
@@ -18980,7 +19484,7 @@
       </c>
       <c r="B989" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/251222horizon2627sprieeni/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/subvenciones-para-innovacion-en-economia-circular-2026/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C989" s="20" t="n"/>
@@ -18991,7 +19495,7 @@
     <row r="991" ht="30" customHeight="1">
       <c r="A991" s="16" t="inlineStr">
         <is>
-          <t>FICHA 67: EUS-17430</t>
+          <t>FICHA 67: EUS-00130</t>
         </is>
       </c>
       <c r="B991" s="17" t="n"/>
@@ -19024,7 +19528,7 @@
       </c>
       <c r="B993" s="19" t="inlineStr">
         <is>
-          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
+          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
         </is>
       </c>
       <c r="C993" s="20" t="n"/>
@@ -19040,7 +19544,7 @@
       </c>
       <c r="B994" s="19" t="inlineStr">
         <is>
-          <t>EUS-17430</t>
+          <t>EUS-00130</t>
         </is>
       </c>
       <c r="C994" s="20" t="n"/>
@@ -19192,7 +19696,7 @@
       </c>
       <c r="B1004" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/demokraziaezkutua251218/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/251222horizon2627sprieeni/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1004" s="20" t="n"/>
@@ -19203,7 +19707,7 @@
     <row r="1006" ht="30" customHeight="1">
       <c r="A1006" s="16" t="inlineStr">
         <is>
-          <t>FICHA 68: EUS-18205</t>
+          <t>FICHA 68: EUS-83114</t>
         </is>
       </c>
       <c r="B1006" s="17" t="n"/>
@@ -19236,7 +19740,7 @@
       </c>
       <c r="B1008" s="19" t="inlineStr">
         <is>
-          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
+          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
         </is>
       </c>
       <c r="C1008" s="20" t="n"/>
@@ -19252,7 +19756,7 @@
       </c>
       <c r="B1009" s="19" t="inlineStr">
         <is>
-          <t>EUS-18205</t>
+          <t>EUS-83114</t>
         </is>
       </c>
       <c r="C1009" s="20" t="n"/>
@@ -19404,7 +19908,7 @@
       </c>
       <c r="B1019" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/ksiberritzalieplus251218/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/demokraziaezkutua251218/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1019" s="20" t="n"/>
@@ -19415,7 +19919,7 @@
     <row r="1021" ht="30" customHeight="1">
       <c r="A1021" s="16" t="inlineStr">
         <is>
-          <t>FICHA 69: EUS-12970</t>
+          <t>FICHA 69: EUS-36808</t>
         </is>
       </c>
       <c r="B1021" s="17" t="n"/>
@@ -19448,7 +19952,7 @@
       </c>
       <c r="B1023" s="19" t="inlineStr">
         <is>
-          <t>Asignaciones individualizadas de transporte escolar para el curso 2025-2026 del alumnado de los centros docentes públicos no universitarios de la Comunidad Autónoma del País Vasco financiado por el de</t>
+          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
         </is>
       </c>
       <c r="C1023" s="20" t="n"/>
@@ -19464,7 +19968,7 @@
       </c>
       <c r="B1024" s="19" t="inlineStr">
         <is>
-          <t>EUS-12970</t>
+          <t>EUS-36808</t>
         </is>
       </c>
       <c r="C1024" s="20" t="n"/>
@@ -19616,7 +20120,7 @@
       </c>
       <c r="B1034" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/transp-escolar-25-26/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/ksiberritzalieplus251218/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1034" s="20" t="n"/>
@@ -19624,8 +20128,1916 @@
       <c r="E1034" s="20" t="n"/>
       <c r="F1034" s="20" t="n"/>
     </row>
+    <row r="1036" ht="30" customHeight="1">
+      <c r="A1036" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 70: EUS-28459</t>
+        </is>
+      </c>
+      <c r="B1036" s="17" t="n"/>
+      <c r="C1036" s="17" t="n"/>
+      <c r="D1036" s="17" t="n"/>
+      <c r="E1036" s="17" t="n"/>
+      <c r="F1036" s="17" t="n"/>
+    </row>
+    <row r="1037" ht="20" customHeight="1">
+      <c r="A1037" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1037" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1037" s="20" t="n"/>
+      <c r="D1037" s="20" t="n"/>
+      <c r="E1037" s="20" t="n"/>
+      <c r="F1037" s="20" t="n"/>
+    </row>
+    <row r="1038" ht="45" customHeight="1">
+      <c r="A1038" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1038" s="19" t="inlineStr">
+        <is>
+          <t>Asignaciones individualizadas de transporte escolar para el curso 2025-2026 del alumnado de los centros docentes públicos no universitarios de la Comunidad Autónoma del País Vasco financiado por el de</t>
+        </is>
+      </c>
+      <c r="C1038" s="20" t="n"/>
+      <c r="D1038" s="20" t="n"/>
+      <c r="E1038" s="20" t="n"/>
+      <c r="F1038" s="20" t="n"/>
+    </row>
+    <row r="1039" ht="20" customHeight="1">
+      <c r="A1039" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1039" s="19" t="inlineStr">
+        <is>
+          <t>EUS-28459</t>
+        </is>
+      </c>
+      <c r="C1039" s="20" t="n"/>
+      <c r="D1039" s="20" t="n"/>
+      <c r="E1039" s="20" t="n"/>
+      <c r="F1039" s="20" t="n"/>
+    </row>
+    <row r="1040" ht="20" customHeight="1">
+      <c r="A1040" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1040" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1040" s="20" t="n"/>
+      <c r="D1040" s="20" t="n"/>
+      <c r="E1040" s="20" t="n"/>
+      <c r="F1040" s="20" t="n"/>
+    </row>
+    <row r="1041" ht="20" customHeight="1">
+      <c r="A1041" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1041" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1041" s="20" t="n"/>
+      <c r="D1041" s="20" t="n"/>
+      <c r="E1041" s="20" t="n"/>
+      <c r="F1041" s="20" t="n"/>
+    </row>
+    <row r="1042" ht="20" customHeight="1">
+      <c r="A1042" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1042" s="19" t="inlineStr"/>
+      <c r="C1042" s="20" t="n"/>
+      <c r="D1042" s="20" t="n"/>
+      <c r="E1042" s="20" t="n"/>
+      <c r="F1042" s="20" t="n"/>
+    </row>
+    <row r="1043" ht="20" customHeight="1">
+      <c r="A1043" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1043" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1043" s="20" t="n"/>
+      <c r="D1043" s="20" t="n"/>
+      <c r="E1043" s="20" t="n"/>
+      <c r="F1043" s="20" t="n"/>
+    </row>
+    <row r="1044" ht="20" customHeight="1">
+      <c r="A1044" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1044" s="19" t="inlineStr">
+        <is>
+          <t>Ayuda/Subvencion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1044" s="20" t="n"/>
+      <c r="D1044" s="20" t="n"/>
+      <c r="E1044" s="20" t="n"/>
+      <c r="F1044" s="20" t="n"/>
+    </row>
+    <row r="1045" ht="20" customHeight="1">
+      <c r="A1045" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1045" s="19" t="inlineStr"/>
+      <c r="C1045" s="20" t="n"/>
+      <c r="D1045" s="20" t="n"/>
+      <c r="E1045" s="20" t="n"/>
+      <c r="F1045" s="20" t="n"/>
+    </row>
+    <row r="1046" ht="20" customHeight="1">
+      <c r="A1046" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1046" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1046" s="20" t="n"/>
+      <c r="D1046" s="20" t="n"/>
+      <c r="E1046" s="20" t="n"/>
+      <c r="F1046" s="20" t="n"/>
+    </row>
+    <row r="1047" ht="20" customHeight="1">
+      <c r="A1047" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1047" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1047" s="20" t="n"/>
+      <c r="D1047" s="20" t="n"/>
+      <c r="E1047" s="20" t="n"/>
+      <c r="F1047" s="20" t="n"/>
+    </row>
+    <row r="1048" ht="20" customHeight="1">
+      <c r="A1048" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1048" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1048" s="20" t="n"/>
+      <c r="D1048" s="20" t="n"/>
+      <c r="E1048" s="20" t="n"/>
+      <c r="F1048" s="20" t="n"/>
+    </row>
+    <row r="1049" ht="45" customHeight="1">
+      <c r="A1049" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1049" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/transp-escolar-25-26/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1049" s="20" t="n"/>
+      <c r="D1049" s="20" t="n"/>
+      <c r="E1049" s="20" t="n"/>
+      <c r="F1049" s="20" t="n"/>
+    </row>
+    <row r="1051" ht="30" customHeight="1">
+      <c r="A1051" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 71: EUS-68968</t>
+        </is>
+      </c>
+      <c r="B1051" s="17" t="n"/>
+      <c r="C1051" s="17" t="n"/>
+      <c r="D1051" s="17" t="n"/>
+      <c r="E1051" s="17" t="n"/>
+      <c r="F1051" s="17" t="n"/>
+    </row>
+    <row r="1052" ht="20" customHeight="1">
+      <c r="A1052" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1052" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1052" s="20" t="n"/>
+      <c r="D1052" s="20" t="n"/>
+      <c r="E1052" s="20" t="n"/>
+      <c r="F1052" s="20" t="n"/>
+    </row>
+    <row r="1053" ht="45" customHeight="1">
+      <c r="A1053" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1053" s="19" t="inlineStr">
+        <is>
+          <t>Mantenimiento preventivo de 10 grúas de techo ubicadas en el edificio de hospitalización de la OSI Debagoiena</t>
+        </is>
+      </c>
+      <c r="C1053" s="20" t="n"/>
+      <c r="D1053" s="20" t="n"/>
+      <c r="E1053" s="20" t="n"/>
+      <c r="F1053" s="20" t="n"/>
+    </row>
+    <row r="1054" ht="20" customHeight="1">
+      <c r="A1054" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1054" s="19" t="inlineStr">
+        <is>
+          <t>EUS-68968</t>
+        </is>
+      </c>
+      <c r="C1054" s="20" t="n"/>
+      <c r="D1054" s="20" t="n"/>
+      <c r="E1054" s="20" t="n"/>
+      <c r="F1054" s="20" t="n"/>
+    </row>
+    <row r="1055" ht="20" customHeight="1">
+      <c r="A1055" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1055" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1055" s="20" t="n"/>
+      <c r="D1055" s="20" t="n"/>
+      <c r="E1055" s="20" t="n"/>
+      <c r="F1055" s="20" t="n"/>
+    </row>
+    <row r="1056" ht="20" customHeight="1">
+      <c r="A1056" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1056" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1056" s="20" t="n"/>
+      <c r="D1056" s="20" t="n"/>
+      <c r="E1056" s="20" t="n"/>
+      <c r="F1056" s="20" t="n"/>
+    </row>
+    <row r="1057" ht="20" customHeight="1">
+      <c r="A1057" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1057" s="19" t="inlineStr"/>
+      <c r="C1057" s="20" t="n"/>
+      <c r="D1057" s="20" t="n"/>
+      <c r="E1057" s="20" t="n"/>
+      <c r="F1057" s="20" t="n"/>
+    </row>
+    <row r="1058" ht="20" customHeight="1">
+      <c r="A1058" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1058" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1058" s="20" t="n"/>
+      <c r="D1058" s="20" t="n"/>
+      <c r="E1058" s="20" t="n"/>
+      <c r="F1058" s="20" t="n"/>
+    </row>
+    <row r="1059" ht="20" customHeight="1">
+      <c r="A1059" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1059" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1059" s="20" t="n"/>
+      <c r="D1059" s="20" t="n"/>
+      <c r="E1059" s="20" t="n"/>
+      <c r="F1059" s="20" t="n"/>
+    </row>
+    <row r="1060" ht="20" customHeight="1">
+      <c r="A1060" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1060" s="19" t="inlineStr"/>
+      <c r="C1060" s="20" t="n"/>
+      <c r="D1060" s="20" t="n"/>
+      <c r="E1060" s="20" t="n"/>
+      <c r="F1060" s="20" t="n"/>
+    </row>
+    <row r="1061" ht="20" customHeight="1">
+      <c r="A1061" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1061" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1061" s="20" t="n"/>
+      <c r="D1061" s="20" t="n"/>
+      <c r="E1061" s="20" t="n"/>
+      <c r="F1061" s="20" t="n"/>
+    </row>
+    <row r="1062" ht="20" customHeight="1">
+      <c r="A1062" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1062" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1062" s="20" t="n"/>
+      <c r="D1062" s="20" t="n"/>
+      <c r="E1062" s="20" t="n"/>
+      <c r="F1062" s="20" t="n"/>
+    </row>
+    <row r="1063" ht="20" customHeight="1">
+      <c r="A1063" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1063" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1063" s="20" t="n"/>
+      <c r="D1063" s="20" t="n"/>
+      <c r="E1063" s="20" t="n"/>
+      <c r="F1063" s="20" t="n"/>
+    </row>
+    <row r="1064" ht="45" customHeight="1">
+      <c r="A1064" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1064" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/mantenimiento-preventivo-10-gruas-techo-ubicadas-edificio-hospitalizacion-osi-debagoiena/exposakisap2026000132/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1064" s="20" t="n"/>
+      <c r="D1064" s="20" t="n"/>
+      <c r="E1064" s="20" t="n"/>
+      <c r="F1064" s="20" t="n"/>
+    </row>
+    <row r="1066" ht="30" customHeight="1">
+      <c r="A1066" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 72: EUS-40629</t>
+        </is>
+      </c>
+      <c r="B1066" s="17" t="n"/>
+      <c r="C1066" s="17" t="n"/>
+      <c r="D1066" s="17" t="n"/>
+      <c r="E1066" s="17" t="n"/>
+      <c r="F1066" s="17" t="n"/>
+    </row>
+    <row r="1067" ht="20" customHeight="1">
+      <c r="A1067" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1067" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1067" s="20" t="n"/>
+      <c r="D1067" s="20" t="n"/>
+      <c r="E1067" s="20" t="n"/>
+      <c r="F1067" s="20" t="n"/>
+    </row>
+    <row r="1068" ht="45" customHeight="1">
+      <c r="A1068" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1068" s="19" t="inlineStr">
+        <is>
+          <t>Asesoría Legal - Asesoramiento legal contestación borofax Solaria y análisis terrenos Indarberri</t>
+        </is>
+      </c>
+      <c r="C1068" s="20" t="n"/>
+      <c r="D1068" s="20" t="n"/>
+      <c r="E1068" s="20" t="n"/>
+      <c r="F1068" s="20" t="n"/>
+    </row>
+    <row r="1069" ht="20" customHeight="1">
+      <c r="A1069" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1069" s="19" t="inlineStr">
+        <is>
+          <t>EUS-40629</t>
+        </is>
+      </c>
+      <c r="C1069" s="20" t="n"/>
+      <c r="D1069" s="20" t="n"/>
+      <c r="E1069" s="20" t="n"/>
+      <c r="F1069" s="20" t="n"/>
+    </row>
+    <row r="1070" ht="20" customHeight="1">
+      <c r="A1070" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1070" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1070" s="20" t="n"/>
+      <c r="D1070" s="20" t="n"/>
+      <c r="E1070" s="20" t="n"/>
+      <c r="F1070" s="20" t="n"/>
+    </row>
+    <row r="1071" ht="20" customHeight="1">
+      <c r="A1071" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1071" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1071" s="20" t="n"/>
+      <c r="D1071" s="20" t="n"/>
+      <c r="E1071" s="20" t="n"/>
+      <c r="F1071" s="20" t="n"/>
+    </row>
+    <row r="1072" ht="20" customHeight="1">
+      <c r="A1072" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1072" s="19" t="inlineStr"/>
+      <c r="C1072" s="20" t="n"/>
+      <c r="D1072" s="20" t="n"/>
+      <c r="E1072" s="20" t="n"/>
+      <c r="F1072" s="20" t="n"/>
+    </row>
+    <row r="1073" ht="20" customHeight="1">
+      <c r="A1073" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1073" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1073" s="20" t="n"/>
+      <c r="D1073" s="20" t="n"/>
+      <c r="E1073" s="20" t="n"/>
+      <c r="F1073" s="20" t="n"/>
+    </row>
+    <row r="1074" ht="20" customHeight="1">
+      <c r="A1074" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1074" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1074" s="20" t="n"/>
+      <c r="D1074" s="20" t="n"/>
+      <c r="E1074" s="20" t="n"/>
+      <c r="F1074" s="20" t="n"/>
+    </row>
+    <row r="1075" ht="20" customHeight="1">
+      <c r="A1075" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1075" s="19" t="inlineStr"/>
+      <c r="C1075" s="20" t="n"/>
+      <c r="D1075" s="20" t="n"/>
+      <c r="E1075" s="20" t="n"/>
+      <c r="F1075" s="20" t="n"/>
+    </row>
+    <row r="1076" ht="20" customHeight="1">
+      <c r="A1076" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1076" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1076" s="20" t="n"/>
+      <c r="D1076" s="20" t="n"/>
+      <c r="E1076" s="20" t="n"/>
+      <c r="F1076" s="20" t="n"/>
+    </row>
+    <row r="1077" ht="20" customHeight="1">
+      <c r="A1077" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1077" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1077" s="20" t="n"/>
+      <c r="D1077" s="20" t="n"/>
+      <c r="E1077" s="20" t="n"/>
+      <c r="F1077" s="20" t="n"/>
+    </row>
+    <row r="1078" ht="20" customHeight="1">
+      <c r="A1078" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1078" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1078" s="20" t="n"/>
+      <c r="D1078" s="20" t="n"/>
+      <c r="E1078" s="20" t="n"/>
+      <c r="F1078" s="20" t="n"/>
+    </row>
+    <row r="1079" ht="45" customHeight="1">
+      <c r="A1079" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1079" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/asesoria-legal-asesoramiento-legal-contestacion-borofax-solaria-y-analisis-terrenos-indarberri/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1079" s="20" t="n"/>
+      <c r="D1079" s="20" t="n"/>
+      <c r="E1079" s="20" t="n"/>
+      <c r="F1079" s="20" t="n"/>
+    </row>
+    <row r="1081" ht="30" customHeight="1">
+      <c r="A1081" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 73: EUS-35956</t>
+        </is>
+      </c>
+      <c r="B1081" s="17" t="n"/>
+      <c r="C1081" s="17" t="n"/>
+      <c r="D1081" s="17" t="n"/>
+      <c r="E1081" s="17" t="n"/>
+      <c r="F1081" s="17" t="n"/>
+    </row>
+    <row r="1082" ht="20" customHeight="1">
+      <c r="A1082" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1082" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1082" s="20" t="n"/>
+      <c r="D1082" s="20" t="n"/>
+      <c r="E1082" s="20" t="n"/>
+      <c r="F1082" s="20" t="n"/>
+    </row>
+    <row r="1083" ht="45" customHeight="1">
+      <c r="A1083" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1083" s="19" t="inlineStr">
+        <is>
+          <t>Otras Consultorías/ Servicios - Asesoramiento en la valoración de plantas fotovoltaicas</t>
+        </is>
+      </c>
+      <c r="C1083" s="20" t="n"/>
+      <c r="D1083" s="20" t="n"/>
+      <c r="E1083" s="20" t="n"/>
+      <c r="F1083" s="20" t="n"/>
+    </row>
+    <row r="1084" ht="20" customHeight="1">
+      <c r="A1084" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1084" s="19" t="inlineStr">
+        <is>
+          <t>EUS-35956</t>
+        </is>
+      </c>
+      <c r="C1084" s="20" t="n"/>
+      <c r="D1084" s="20" t="n"/>
+      <c r="E1084" s="20" t="n"/>
+      <c r="F1084" s="20" t="n"/>
+    </row>
+    <row r="1085" ht="20" customHeight="1">
+      <c r="A1085" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1085" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1085" s="20" t="n"/>
+      <c r="D1085" s="20" t="n"/>
+      <c r="E1085" s="20" t="n"/>
+      <c r="F1085" s="20" t="n"/>
+    </row>
+    <row r="1086" ht="20" customHeight="1">
+      <c r="A1086" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1086" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1086" s="20" t="n"/>
+      <c r="D1086" s="20" t="n"/>
+      <c r="E1086" s="20" t="n"/>
+      <c r="F1086" s="20" t="n"/>
+    </row>
+    <row r="1087" ht="20" customHeight="1">
+      <c r="A1087" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1087" s="19" t="inlineStr"/>
+      <c r="C1087" s="20" t="n"/>
+      <c r="D1087" s="20" t="n"/>
+      <c r="E1087" s="20" t="n"/>
+      <c r="F1087" s="20" t="n"/>
+    </row>
+    <row r="1088" ht="20" customHeight="1">
+      <c r="A1088" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1088" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1088" s="20" t="n"/>
+      <c r="D1088" s="20" t="n"/>
+      <c r="E1088" s="20" t="n"/>
+      <c r="F1088" s="20" t="n"/>
+    </row>
+    <row r="1089" ht="20" customHeight="1">
+      <c r="A1089" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1089" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1089" s="20" t="n"/>
+      <c r="D1089" s="20" t="n"/>
+      <c r="E1089" s="20" t="n"/>
+      <c r="F1089" s="20" t="n"/>
+    </row>
+    <row r="1090" ht="20" customHeight="1">
+      <c r="A1090" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1090" s="19" t="inlineStr"/>
+      <c r="C1090" s="20" t="n"/>
+      <c r="D1090" s="20" t="n"/>
+      <c r="E1090" s="20" t="n"/>
+      <c r="F1090" s="20" t="n"/>
+    </row>
+    <row r="1091" ht="20" customHeight="1">
+      <c r="A1091" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1091" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1091" s="20" t="n"/>
+      <c r="D1091" s="20" t="n"/>
+      <c r="E1091" s="20" t="n"/>
+      <c r="F1091" s="20" t="n"/>
+    </row>
+    <row r="1092" ht="20" customHeight="1">
+      <c r="A1092" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1092" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1092" s="20" t="n"/>
+      <c r="D1092" s="20" t="n"/>
+      <c r="E1092" s="20" t="n"/>
+      <c r="F1092" s="20" t="n"/>
+    </row>
+    <row r="1093" ht="20" customHeight="1">
+      <c r="A1093" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1093" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1093" s="20" t="n"/>
+      <c r="D1093" s="20" t="n"/>
+      <c r="E1093" s="20" t="n"/>
+      <c r="F1093" s="20" t="n"/>
+    </row>
+    <row r="1094" ht="45" customHeight="1">
+      <c r="A1094" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1094" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/otras-consultorias-servicios-asesoramiento-valoracion-plantas-fotovoltaicas/expcm487019/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1094" s="20" t="n"/>
+      <c r="D1094" s="20" t="n"/>
+      <c r="E1094" s="20" t="n"/>
+      <c r="F1094" s="20" t="n"/>
+    </row>
+    <row r="1096" ht="30" customHeight="1">
+      <c r="A1096" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 74: EUS-21012</t>
+        </is>
+      </c>
+      <c r="B1096" s="17" t="n"/>
+      <c r="C1096" s="17" t="n"/>
+      <c r="D1096" s="17" t="n"/>
+      <c r="E1096" s="17" t="n"/>
+      <c r="F1096" s="17" t="n"/>
+    </row>
+    <row r="1097" ht="20" customHeight="1">
+      <c r="A1097" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1097" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1097" s="20" t="n"/>
+      <c r="D1097" s="20" t="n"/>
+      <c r="E1097" s="20" t="n"/>
+      <c r="F1097" s="20" t="n"/>
+    </row>
+    <row r="1098" ht="45" customHeight="1">
+      <c r="A1098" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1098" s="19" t="inlineStr">
+        <is>
+          <t>Otras Consultorías/ Servicios - Asesoramiento en la valoración de plantas fotovoltaicas</t>
+        </is>
+      </c>
+      <c r="C1098" s="20" t="n"/>
+      <c r="D1098" s="20" t="n"/>
+      <c r="E1098" s="20" t="n"/>
+      <c r="F1098" s="20" t="n"/>
+    </row>
+    <row r="1099" ht="20" customHeight="1">
+      <c r="A1099" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1099" s="19" t="inlineStr">
+        <is>
+          <t>EUS-21012</t>
+        </is>
+      </c>
+      <c r="C1099" s="20" t="n"/>
+      <c r="D1099" s="20" t="n"/>
+      <c r="E1099" s="20" t="n"/>
+      <c r="F1099" s="20" t="n"/>
+    </row>
+    <row r="1100" ht="20" customHeight="1">
+      <c r="A1100" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1100" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1100" s="20" t="n"/>
+      <c r="D1100" s="20" t="n"/>
+      <c r="E1100" s="20" t="n"/>
+      <c r="F1100" s="20" t="n"/>
+    </row>
+    <row r="1101" ht="20" customHeight="1">
+      <c r="A1101" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1101" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1101" s="20" t="n"/>
+      <c r="D1101" s="20" t="n"/>
+      <c r="E1101" s="20" t="n"/>
+      <c r="F1101" s="20" t="n"/>
+    </row>
+    <row r="1102" ht="20" customHeight="1">
+      <c r="A1102" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1102" s="19" t="inlineStr"/>
+      <c r="C1102" s="20" t="n"/>
+      <c r="D1102" s="20" t="n"/>
+      <c r="E1102" s="20" t="n"/>
+      <c r="F1102" s="20" t="n"/>
+    </row>
+    <row r="1103" ht="20" customHeight="1">
+      <c r="A1103" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1103" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1103" s="20" t="n"/>
+      <c r="D1103" s="20" t="n"/>
+      <c r="E1103" s="20" t="n"/>
+      <c r="F1103" s="20" t="n"/>
+    </row>
+    <row r="1104" ht="20" customHeight="1">
+      <c r="A1104" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1104" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1104" s="20" t="n"/>
+      <c r="D1104" s="20" t="n"/>
+      <c r="E1104" s="20" t="n"/>
+      <c r="F1104" s="20" t="n"/>
+    </row>
+    <row r="1105" ht="20" customHeight="1">
+      <c r="A1105" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1105" s="19" t="inlineStr"/>
+      <c r="C1105" s="20" t="n"/>
+      <c r="D1105" s="20" t="n"/>
+      <c r="E1105" s="20" t="n"/>
+      <c r="F1105" s="20" t="n"/>
+    </row>
+    <row r="1106" ht="20" customHeight="1">
+      <c r="A1106" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1106" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1106" s="20" t="n"/>
+      <c r="D1106" s="20" t="n"/>
+      <c r="E1106" s="20" t="n"/>
+      <c r="F1106" s="20" t="n"/>
+    </row>
+    <row r="1107" ht="20" customHeight="1">
+      <c r="A1107" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1107" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1107" s="20" t="n"/>
+      <c r="D1107" s="20" t="n"/>
+      <c r="E1107" s="20" t="n"/>
+      <c r="F1107" s="20" t="n"/>
+    </row>
+    <row r="1108" ht="20" customHeight="1">
+      <c r="A1108" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1108" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1108" s="20" t="n"/>
+      <c r="D1108" s="20" t="n"/>
+      <c r="E1108" s="20" t="n"/>
+      <c r="F1108" s="20" t="n"/>
+    </row>
+    <row r="1109" ht="45" customHeight="1">
+      <c r="A1109" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1109" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/otras-consultorias-servicios-asesoramiento-valoracion-plantas-fotovoltaicas/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1109" s="20" t="n"/>
+      <c r="D1109" s="20" t="n"/>
+      <c r="E1109" s="20" t="n"/>
+      <c r="F1109" s="20" t="n"/>
+    </row>
+    <row r="1111" ht="30" customHeight="1">
+      <c r="A1111" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 75: EUS-80336</t>
+        </is>
+      </c>
+      <c r="B1111" s="17" t="n"/>
+      <c r="C1111" s="17" t="n"/>
+      <c r="D1111" s="17" t="n"/>
+      <c r="E1111" s="17" t="n"/>
+      <c r="F1111" s="17" t="n"/>
+    </row>
+    <row r="1112" ht="20" customHeight="1">
+      <c r="A1112" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1112" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1112" s="20" t="n"/>
+      <c r="D1112" s="20" t="n"/>
+      <c r="E1112" s="20" t="n"/>
+      <c r="F1112" s="20" t="n"/>
+    </row>
+    <row r="1113" ht="20" customHeight="1">
+      <c r="A1113" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1113" s="19" t="inlineStr">
+        <is>
+          <t>Asesoría Legal - Asesoramiento en negociación proyecto plantas fotovoltaicas</t>
+        </is>
+      </c>
+      <c r="C1113" s="20" t="n"/>
+      <c r="D1113" s="20" t="n"/>
+      <c r="E1113" s="20" t="n"/>
+      <c r="F1113" s="20" t="n"/>
+    </row>
+    <row r="1114" ht="20" customHeight="1">
+      <c r="A1114" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1114" s="19" t="inlineStr">
+        <is>
+          <t>EUS-80336</t>
+        </is>
+      </c>
+      <c r="C1114" s="20" t="n"/>
+      <c r="D1114" s="20" t="n"/>
+      <c r="E1114" s="20" t="n"/>
+      <c r="F1114" s="20" t="n"/>
+    </row>
+    <row r="1115" ht="20" customHeight="1">
+      <c r="A1115" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1115" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1115" s="20" t="n"/>
+      <c r="D1115" s="20" t="n"/>
+      <c r="E1115" s="20" t="n"/>
+      <c r="F1115" s="20" t="n"/>
+    </row>
+    <row r="1116" ht="20" customHeight="1">
+      <c r="A1116" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1116" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1116" s="20" t="n"/>
+      <c r="D1116" s="20" t="n"/>
+      <c r="E1116" s="20" t="n"/>
+      <c r="F1116" s="20" t="n"/>
+    </row>
+    <row r="1117" ht="20" customHeight="1">
+      <c r="A1117" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1117" s="19" t="inlineStr"/>
+      <c r="C1117" s="20" t="n"/>
+      <c r="D1117" s="20" t="n"/>
+      <c r="E1117" s="20" t="n"/>
+      <c r="F1117" s="20" t="n"/>
+    </row>
+    <row r="1118" ht="20" customHeight="1">
+      <c r="A1118" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1118" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1118" s="20" t="n"/>
+      <c r="D1118" s="20" t="n"/>
+      <c r="E1118" s="20" t="n"/>
+      <c r="F1118" s="20" t="n"/>
+    </row>
+    <row r="1119" ht="20" customHeight="1">
+      <c r="A1119" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1119" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1119" s="20" t="n"/>
+      <c r="D1119" s="20" t="n"/>
+      <c r="E1119" s="20" t="n"/>
+      <c r="F1119" s="20" t="n"/>
+    </row>
+    <row r="1120" ht="20" customHeight="1">
+      <c r="A1120" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1120" s="19" t="inlineStr"/>
+      <c r="C1120" s="20" t="n"/>
+      <c r="D1120" s="20" t="n"/>
+      <c r="E1120" s="20" t="n"/>
+      <c r="F1120" s="20" t="n"/>
+    </row>
+    <row r="1121" ht="20" customHeight="1">
+      <c r="A1121" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1121" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1121" s="20" t="n"/>
+      <c r="D1121" s="20" t="n"/>
+      <c r="E1121" s="20" t="n"/>
+      <c r="F1121" s="20" t="n"/>
+    </row>
+    <row r="1122" ht="20" customHeight="1">
+      <c r="A1122" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1122" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1122" s="20" t="n"/>
+      <c r="D1122" s="20" t="n"/>
+      <c r="E1122" s="20" t="n"/>
+      <c r="F1122" s="20" t="n"/>
+    </row>
+    <row r="1123" ht="20" customHeight="1">
+      <c r="A1123" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1123" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1123" s="20" t="n"/>
+      <c r="D1123" s="20" t="n"/>
+      <c r="E1123" s="20" t="n"/>
+      <c r="F1123" s="20" t="n"/>
+    </row>
+    <row r="1124" ht="45" customHeight="1">
+      <c r="A1124" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1124" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/asesoria-legal-asesoramiento-negociacion-proyecto-plantas-fotovoltaicas/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1124" s="20" t="n"/>
+      <c r="D1124" s="20" t="n"/>
+      <c r="E1124" s="20" t="n"/>
+      <c r="F1124" s="20" t="n"/>
+    </row>
+    <row r="1126" ht="30" customHeight="1">
+      <c r="A1126" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 76: EUS-82751</t>
+        </is>
+      </c>
+      <c r="B1126" s="17" t="n"/>
+      <c r="C1126" s="17" t="n"/>
+      <c r="D1126" s="17" t="n"/>
+      <c r="E1126" s="17" t="n"/>
+      <c r="F1126" s="17" t="n"/>
+    </row>
+    <row r="1127" ht="20" customHeight="1">
+      <c r="A1127" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1127" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1127" s="20" t="n"/>
+      <c r="D1127" s="20" t="n"/>
+      <c r="E1127" s="20" t="n"/>
+      <c r="F1127" s="20" t="n"/>
+    </row>
+    <row r="1128" ht="20" customHeight="1">
+      <c r="A1128" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1128" s="19" t="inlineStr">
+        <is>
+          <t>Limpieza de foso ascensor san juan mekola</t>
+        </is>
+      </c>
+      <c r="C1128" s="20" t="n"/>
+      <c r="D1128" s="20" t="n"/>
+      <c r="E1128" s="20" t="n"/>
+      <c r="F1128" s="20" t="n"/>
+    </row>
+    <row r="1129" ht="20" customHeight="1">
+      <c r="A1129" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1129" s="19" t="inlineStr">
+        <is>
+          <t>EUS-82751</t>
+        </is>
+      </c>
+      <c r="C1129" s="20" t="n"/>
+      <c r="D1129" s="20" t="n"/>
+      <c r="E1129" s="20" t="n"/>
+      <c r="F1129" s="20" t="n"/>
+    </row>
+    <row r="1130" ht="20" customHeight="1">
+      <c r="A1130" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1130" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1130" s="20" t="n"/>
+      <c r="D1130" s="20" t="n"/>
+      <c r="E1130" s="20" t="n"/>
+      <c r="F1130" s="20" t="n"/>
+    </row>
+    <row r="1131" ht="20" customHeight="1">
+      <c r="A1131" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1131" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1131" s="20" t="n"/>
+      <c r="D1131" s="20" t="n"/>
+      <c r="E1131" s="20" t="n"/>
+      <c r="F1131" s="20" t="n"/>
+    </row>
+    <row r="1132" ht="20" customHeight="1">
+      <c r="A1132" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1132" s="19" t="inlineStr"/>
+      <c r="C1132" s="20" t="n"/>
+      <c r="D1132" s="20" t="n"/>
+      <c r="E1132" s="20" t="n"/>
+      <c r="F1132" s="20" t="n"/>
+    </row>
+    <row r="1133" ht="20" customHeight="1">
+      <c r="A1133" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1133" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1133" s="20" t="n"/>
+      <c r="D1133" s="20" t="n"/>
+      <c r="E1133" s="20" t="n"/>
+      <c r="F1133" s="20" t="n"/>
+    </row>
+    <row r="1134" ht="20" customHeight="1">
+      <c r="A1134" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1134" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1134" s="20" t="n"/>
+      <c r="D1134" s="20" t="n"/>
+      <c r="E1134" s="20" t="n"/>
+      <c r="F1134" s="20" t="n"/>
+    </row>
+    <row r="1135" ht="20" customHeight="1">
+      <c r="A1135" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1135" s="19" t="inlineStr"/>
+      <c r="C1135" s="20" t="n"/>
+      <c r="D1135" s="20" t="n"/>
+      <c r="E1135" s="20" t="n"/>
+      <c r="F1135" s="20" t="n"/>
+    </row>
+    <row r="1136" ht="20" customHeight="1">
+      <c r="A1136" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1136" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1136" s="20" t="n"/>
+      <c r="D1136" s="20" t="n"/>
+      <c r="E1136" s="20" t="n"/>
+      <c r="F1136" s="20" t="n"/>
+    </row>
+    <row r="1137" ht="20" customHeight="1">
+      <c r="A1137" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1137" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1137" s="20" t="n"/>
+      <c r="D1137" s="20" t="n"/>
+      <c r="E1137" s="20" t="n"/>
+      <c r="F1137" s="20" t="n"/>
+    </row>
+    <row r="1138" ht="20" customHeight="1">
+      <c r="A1138" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1138" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1138" s="20" t="n"/>
+      <c r="D1138" s="20" t="n"/>
+      <c r="E1138" s="20" t="n"/>
+      <c r="F1138" s="20" t="n"/>
+    </row>
+    <row r="1139" ht="45" customHeight="1">
+      <c r="A1139" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1139" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/limpieza-foso-ascensor-san-juan-mekola/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1139" s="20" t="n"/>
+      <c r="D1139" s="20" t="n"/>
+      <c r="E1139" s="20" t="n"/>
+      <c r="F1139" s="20" t="n"/>
+    </row>
+    <row r="1141" ht="30" customHeight="1">
+      <c r="A1141" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 77: EUS-08134</t>
+        </is>
+      </c>
+      <c r="B1141" s="17" t="n"/>
+      <c r="C1141" s="17" t="n"/>
+      <c r="D1141" s="17" t="n"/>
+      <c r="E1141" s="17" t="n"/>
+      <c r="F1141" s="17" t="n"/>
+    </row>
+    <row r="1142" ht="20" customHeight="1">
+      <c r="A1142" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1142" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1142" s="20" t="n"/>
+      <c r="D1142" s="20" t="n"/>
+      <c r="E1142" s="20" t="n"/>
+      <c r="F1142" s="20" t="n"/>
+    </row>
+    <row r="1143" ht="20" customHeight="1">
+      <c r="A1143" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1143" s="19" t="inlineStr">
+        <is>
+          <t>Limpieza sumideros de errebal</t>
+        </is>
+      </c>
+      <c r="C1143" s="20" t="n"/>
+      <c r="D1143" s="20" t="n"/>
+      <c r="E1143" s="20" t="n"/>
+      <c r="F1143" s="20" t="n"/>
+    </row>
+    <row r="1144" ht="20" customHeight="1">
+      <c r="A1144" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1144" s="19" t="inlineStr">
+        <is>
+          <t>EUS-08134</t>
+        </is>
+      </c>
+      <c r="C1144" s="20" t="n"/>
+      <c r="D1144" s="20" t="n"/>
+      <c r="E1144" s="20" t="n"/>
+      <c r="F1144" s="20" t="n"/>
+    </row>
+    <row r="1145" ht="20" customHeight="1">
+      <c r="A1145" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1145" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1145" s="20" t="n"/>
+      <c r="D1145" s="20" t="n"/>
+      <c r="E1145" s="20" t="n"/>
+      <c r="F1145" s="20" t="n"/>
+    </row>
+    <row r="1146" ht="20" customHeight="1">
+      <c r="A1146" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1146" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1146" s="20" t="n"/>
+      <c r="D1146" s="20" t="n"/>
+      <c r="E1146" s="20" t="n"/>
+      <c r="F1146" s="20" t="n"/>
+    </row>
+    <row r="1147" ht="20" customHeight="1">
+      <c r="A1147" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1147" s="19" t="inlineStr"/>
+      <c r="C1147" s="20" t="n"/>
+      <c r="D1147" s="20" t="n"/>
+      <c r="E1147" s="20" t="n"/>
+      <c r="F1147" s="20" t="n"/>
+    </row>
+    <row r="1148" ht="20" customHeight="1">
+      <c r="A1148" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1148" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1148" s="20" t="n"/>
+      <c r="D1148" s="20" t="n"/>
+      <c r="E1148" s="20" t="n"/>
+      <c r="F1148" s="20" t="n"/>
+    </row>
+    <row r="1149" ht="20" customHeight="1">
+      <c r="A1149" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1149" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1149" s="20" t="n"/>
+      <c r="D1149" s="20" t="n"/>
+      <c r="E1149" s="20" t="n"/>
+      <c r="F1149" s="20" t="n"/>
+    </row>
+    <row r="1150" ht="20" customHeight="1">
+      <c r="A1150" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1150" s="19" t="inlineStr"/>
+      <c r="C1150" s="20" t="n"/>
+      <c r="D1150" s="20" t="n"/>
+      <c r="E1150" s="20" t="n"/>
+      <c r="F1150" s="20" t="n"/>
+    </row>
+    <row r="1151" ht="20" customHeight="1">
+      <c r="A1151" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1151" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1151" s="20" t="n"/>
+      <c r="D1151" s="20" t="n"/>
+      <c r="E1151" s="20" t="n"/>
+      <c r="F1151" s="20" t="n"/>
+    </row>
+    <row r="1152" ht="20" customHeight="1">
+      <c r="A1152" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1152" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1152" s="20" t="n"/>
+      <c r="D1152" s="20" t="n"/>
+      <c r="E1152" s="20" t="n"/>
+      <c r="F1152" s="20" t="n"/>
+    </row>
+    <row r="1153" ht="20" customHeight="1">
+      <c r="A1153" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1153" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1153" s="20" t="n"/>
+      <c r="D1153" s="20" t="n"/>
+      <c r="E1153" s="20" t="n"/>
+      <c r="F1153" s="20" t="n"/>
+    </row>
+    <row r="1154" ht="45" customHeight="1">
+      <c r="A1154" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1154" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/limpieza-sumideros-errebal/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1154" s="20" t="n"/>
+      <c r="D1154" s="20" t="n"/>
+      <c r="E1154" s="20" t="n"/>
+      <c r="F1154" s="20" t="n"/>
+    </row>
+    <row r="1156" ht="30" customHeight="1">
+      <c r="A1156" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 78: EUS-92185</t>
+        </is>
+      </c>
+      <c r="B1156" s="17" t="n"/>
+      <c r="C1156" s="17" t="n"/>
+      <c r="D1156" s="17" t="n"/>
+      <c r="E1156" s="17" t="n"/>
+      <c r="F1156" s="17" t="n"/>
+    </row>
+    <row r="1157" ht="20" customHeight="1">
+      <c r="A1157" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1157" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1157" s="20" t="n"/>
+      <c r="D1157" s="20" t="n"/>
+      <c r="E1157" s="20" t="n"/>
+      <c r="F1157" s="20" t="n"/>
+    </row>
+    <row r="1158" ht="45" customHeight="1">
+      <c r="A1158" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1158" s="19" t="inlineStr">
+        <is>
+          <t>Reparación de cableados de circuitos de fuerza y alumbrado que se encuentran requemados y sin aislamiento en el fronton astelena</t>
+        </is>
+      </c>
+      <c r="C1158" s="20" t="n"/>
+      <c r="D1158" s="20" t="n"/>
+      <c r="E1158" s="20" t="n"/>
+      <c r="F1158" s="20" t="n"/>
+    </row>
+    <row r="1159" ht="20" customHeight="1">
+      <c r="A1159" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1159" s="19" t="inlineStr">
+        <is>
+          <t>EUS-92185</t>
+        </is>
+      </c>
+      <c r="C1159" s="20" t="n"/>
+      <c r="D1159" s="20" t="n"/>
+      <c r="E1159" s="20" t="n"/>
+      <c r="F1159" s="20" t="n"/>
+    </row>
+    <row r="1160" ht="20" customHeight="1">
+      <c r="A1160" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1160" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1160" s="20" t="n"/>
+      <c r="D1160" s="20" t="n"/>
+      <c r="E1160" s="20" t="n"/>
+      <c r="F1160" s="20" t="n"/>
+    </row>
+    <row r="1161" ht="20" customHeight="1">
+      <c r="A1161" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1161" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1161" s="20" t="n"/>
+      <c r="D1161" s="20" t="n"/>
+      <c r="E1161" s="20" t="n"/>
+      <c r="F1161" s="20" t="n"/>
+    </row>
+    <row r="1162" ht="20" customHeight="1">
+      <c r="A1162" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1162" s="19" t="inlineStr"/>
+      <c r="C1162" s="20" t="n"/>
+      <c r="D1162" s="20" t="n"/>
+      <c r="E1162" s="20" t="n"/>
+      <c r="F1162" s="20" t="n"/>
+    </row>
+    <row r="1163" ht="20" customHeight="1">
+      <c r="A1163" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1163" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1163" s="20" t="n"/>
+      <c r="D1163" s="20" t="n"/>
+      <c r="E1163" s="20" t="n"/>
+      <c r="F1163" s="20" t="n"/>
+    </row>
+    <row r="1164" ht="20" customHeight="1">
+      <c r="A1164" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1164" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1164" s="20" t="n"/>
+      <c r="D1164" s="20" t="n"/>
+      <c r="E1164" s="20" t="n"/>
+      <c r="F1164" s="20" t="n"/>
+    </row>
+    <row r="1165" ht="20" customHeight="1">
+      <c r="A1165" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1165" s="19" t="inlineStr"/>
+      <c r="C1165" s="20" t="n"/>
+      <c r="D1165" s="20" t="n"/>
+      <c r="E1165" s="20" t="n"/>
+      <c r="F1165" s="20" t="n"/>
+    </row>
+    <row r="1166" ht="20" customHeight="1">
+      <c r="A1166" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1166" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1166" s="20" t="n"/>
+      <c r="D1166" s="20" t="n"/>
+      <c r="E1166" s="20" t="n"/>
+      <c r="F1166" s="20" t="n"/>
+    </row>
+    <row r="1167" ht="20" customHeight="1">
+      <c r="A1167" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1167" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1167" s="20" t="n"/>
+      <c r="D1167" s="20" t="n"/>
+      <c r="E1167" s="20" t="n"/>
+      <c r="F1167" s="20" t="n"/>
+    </row>
+    <row r="1168" ht="20" customHeight="1">
+      <c r="A1168" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1168" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1168" s="20" t="n"/>
+      <c r="D1168" s="20" t="n"/>
+      <c r="E1168" s="20" t="n"/>
+      <c r="F1168" s="20" t="n"/>
+    </row>
+    <row r="1169" ht="45" customHeight="1">
+      <c r="A1169" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1169" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/reparacion-cableados-circuitos-fuerza-y-alumbrado-que-se-encuentran-requemados-y-aislamiento-fronton-astelena/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1169" s="20" t="n"/>
+      <c r="D1169" s="20" t="n"/>
+      <c r="E1169" s="20" t="n"/>
+      <c r="F1169" s="20" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="966">
+  <mergeCells count="1092">
     <mergeCell ref="B679:F679"/>
     <mergeCell ref="B666:F666"/>
     <mergeCell ref="B964:F964"/>
@@ -19665,20 +22077,27 @@
     <mergeCell ref="B532:F532"/>
     <mergeCell ref="B799:F799"/>
     <mergeCell ref="B603:F603"/>
+    <mergeCell ref="B1041:F1041"/>
     <mergeCell ref="B342:F342"/>
     <mergeCell ref="B578:F578"/>
     <mergeCell ref="A541:F541"/>
+    <mergeCell ref="B1148:F1148"/>
+    <mergeCell ref="B1099:F1099"/>
     <mergeCell ref="B515:F515"/>
+    <mergeCell ref="B1128:F1128"/>
     <mergeCell ref="A841:F841"/>
     <mergeCell ref="B158:F158"/>
+    <mergeCell ref="B1094:F1094"/>
     <mergeCell ref="B723:F723"/>
     <mergeCell ref="B6:F6"/>
     <mergeCell ref="B894:F894"/>
     <mergeCell ref="B133:F133"/>
     <mergeCell ref="B959:F959"/>
+    <mergeCell ref="B1130:F1130"/>
     <mergeCell ref="B369:F369"/>
     <mergeCell ref="B667:F667"/>
     <mergeCell ref="B418:F418"/>
+    <mergeCell ref="B1142:F1142"/>
     <mergeCell ref="B356:F356"/>
     <mergeCell ref="B160:F160"/>
     <mergeCell ref="B489:F489"/>
@@ -19693,6 +22112,8 @@
     <mergeCell ref="B1023:F1023"/>
     <mergeCell ref="B433:F433"/>
     <mergeCell ref="B233:F233"/>
+    <mergeCell ref="B1067:F1067"/>
+    <mergeCell ref="B1085:F1085"/>
     <mergeCell ref="B227:F227"/>
     <mergeCell ref="B531:F531"/>
     <mergeCell ref="B591:F591"/>
@@ -19700,15 +22121,18 @@
     <mergeCell ref="B662:F662"/>
     <mergeCell ref="B718:F718"/>
     <mergeCell ref="B889:F889"/>
+    <mergeCell ref="B1131:F1131"/>
     <mergeCell ref="B72:F72"/>
     <mergeCell ref="B954:F954"/>
     <mergeCell ref="B199:F199"/>
     <mergeCell ref="B370:F370"/>
     <mergeCell ref="B1025:F1025"/>
+    <mergeCell ref="B1112:F1112"/>
     <mergeCell ref="B291:F291"/>
     <mergeCell ref="B655:F655"/>
     <mergeCell ref="B974:F974"/>
     <mergeCell ref="B891:F891"/>
+    <mergeCell ref="B1072:F1072"/>
     <mergeCell ref="B70:F70"/>
     <mergeCell ref="B228:F228"/>
     <mergeCell ref="B293:F293"/>
@@ -19733,6 +22157,7 @@
     <mergeCell ref="B217:F217"/>
     <mergeCell ref="B388:F388"/>
     <mergeCell ref="B448:F448"/>
+    <mergeCell ref="B1038:F1038"/>
     <mergeCell ref="B304:F304"/>
     <mergeCell ref="B746:F746"/>
     <mergeCell ref="B546:F546"/>
@@ -19744,9 +22169,11 @@
     <mergeCell ref="B83:F83"/>
     <mergeCell ref="B254:F254"/>
     <mergeCell ref="B909:F909"/>
+    <mergeCell ref="B1105:F1105"/>
     <mergeCell ref="B319:F319"/>
     <mergeCell ref="B490:F490"/>
     <mergeCell ref="B604:F604"/>
+    <mergeCell ref="B1046:F1046"/>
     <mergeCell ref="A61:F61"/>
     <mergeCell ref="B85:F85"/>
     <mergeCell ref="B383:F383"/>
@@ -19754,6 +22181,7 @@
     <mergeCell ref="A346:F346"/>
     <mergeCell ref="B904:F904"/>
     <mergeCell ref="B635:F635"/>
+    <mergeCell ref="A1141:F1141"/>
     <mergeCell ref="B141:F141"/>
     <mergeCell ref="B439:F439"/>
     <mergeCell ref="A136:F136"/>
@@ -19774,8 +22202,10 @@
     <mergeCell ref="B530:F530"/>
     <mergeCell ref="B726:F726"/>
     <mergeCell ref="B962:F962"/>
+    <mergeCell ref="B1133:F1133"/>
     <mergeCell ref="A886:F886"/>
     <mergeCell ref="B505:F505"/>
+    <mergeCell ref="B1060:F1060"/>
     <mergeCell ref="B499:F499"/>
     <mergeCell ref="B299:F299"/>
     <mergeCell ref="B274:F274"/>
@@ -19785,11 +22215,13 @@
     <mergeCell ref="B741:F741"/>
     <mergeCell ref="B461:F461"/>
     <mergeCell ref="B728:F728"/>
+    <mergeCell ref="B1039:F1039"/>
     <mergeCell ref="B249:F249"/>
     <mergeCell ref="A481:F481"/>
     <mergeCell ref="B559:F559"/>
     <mergeCell ref="B243:F243"/>
     <mergeCell ref="B1026:F1026"/>
+    <mergeCell ref="B1075:F1075"/>
     <mergeCell ref="B678:F678"/>
     <mergeCell ref="B363:F363"/>
     <mergeCell ref="B534:F534"/>
@@ -19799,28 +22231,36 @@
     <mergeCell ref="B957:F957"/>
     <mergeCell ref="B373:F373"/>
     <mergeCell ref="B1028:F1028"/>
+    <mergeCell ref="B1055:F1055"/>
     <mergeCell ref="B536:F536"/>
     <mergeCell ref="B834:F834"/>
+    <mergeCell ref="B1143:F1143"/>
     <mergeCell ref="B899:F899"/>
     <mergeCell ref="B752:F752"/>
+    <mergeCell ref="B1070:F1070"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B1115:F1115"/>
     <mergeCell ref="B325:F325"/>
     <mergeCell ref="B154:F154"/>
     <mergeCell ref="A271:F271"/>
     <mergeCell ref="B561:F561"/>
     <mergeCell ref="B754:F754"/>
     <mergeCell ref="B859:F859"/>
+    <mergeCell ref="B1052:F1052"/>
     <mergeCell ref="B981:F981"/>
     <mergeCell ref="B846:F846"/>
     <mergeCell ref="B973:F973"/>
     <mergeCell ref="B389:F389"/>
+    <mergeCell ref="B1044:F1044"/>
     <mergeCell ref="B156:F156"/>
     <mergeCell ref="B327:F327"/>
+    <mergeCell ref="B1144:F1144"/>
     <mergeCell ref="B454:F454"/>
     <mergeCell ref="B625:F625"/>
     <mergeCell ref="B923:F923"/>
     <mergeCell ref="A571:F571"/>
     <mergeCell ref="B612:F612"/>
+    <mergeCell ref="B1054:F1054"/>
     <mergeCell ref="B910:F910"/>
     <mergeCell ref="B22:F22"/>
     <mergeCell ref="B155:F155"/>
@@ -19834,8 +22274,12 @@
     <mergeCell ref="B518:F518"/>
     <mergeCell ref="B562:F562"/>
     <mergeCell ref="B689:F689"/>
+    <mergeCell ref="B1121:F1121"/>
+    <mergeCell ref="B1146:F1146"/>
+    <mergeCell ref="B1123:F1123"/>
     <mergeCell ref="B86:F86"/>
     <mergeCell ref="B912:F912"/>
+    <mergeCell ref="B1083:F1083"/>
     <mergeCell ref="B262:F262"/>
     <mergeCell ref="B887:F887"/>
     <mergeCell ref="B862:F862"/>
@@ -19865,6 +22309,7 @@
     <mergeCell ref="B778:F778"/>
     <mergeCell ref="B978:F978"/>
     <mergeCell ref="B79:F79"/>
+    <mergeCell ref="B1076:F1076"/>
     <mergeCell ref="B41:F41"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B302:F302"/>
@@ -19878,10 +22323,13 @@
     <mergeCell ref="B836:F836"/>
     <mergeCell ref="B81:F81"/>
     <mergeCell ref="B252:F252"/>
+    <mergeCell ref="B1042:F1042"/>
     <mergeCell ref="B366:F366"/>
     <mergeCell ref="B979:F979"/>
     <mergeCell ref="B381:F381"/>
     <mergeCell ref="B552:F552"/>
+    <mergeCell ref="A1111:F1111"/>
+    <mergeCell ref="B1084:F1084"/>
     <mergeCell ref="A976:F976"/>
     <mergeCell ref="B170:F170"/>
     <mergeCell ref="B157:F157"/>
@@ -19914,7 +22362,9 @@
     <mergeCell ref="B92:F92"/>
     <mergeCell ref="B984:F984"/>
     <mergeCell ref="A226:F226"/>
+    <mergeCell ref="B1124:F1124"/>
     <mergeCell ref="B394:F394"/>
+    <mergeCell ref="B1162:F1162"/>
     <mergeCell ref="B692:F692"/>
     <mergeCell ref="A931:F931"/>
     <mergeCell ref="B486:F486"/>
@@ -19926,21 +22376,26 @@
     <mergeCell ref="B265:F265"/>
     <mergeCell ref="B458:F458"/>
     <mergeCell ref="B773:F773"/>
+    <mergeCell ref="B1091:F1091"/>
     <mergeCell ref="A526:F526"/>
     <mergeCell ref="B694:F694"/>
     <mergeCell ref="B786:F786"/>
     <mergeCell ref="B54:F54"/>
     <mergeCell ref="A286:F286"/>
     <mergeCell ref="B125:F125"/>
+    <mergeCell ref="B1073:F1073"/>
     <mergeCell ref="B185:F185"/>
     <mergeCell ref="A826:F826"/>
     <mergeCell ref="B483:F483"/>
+    <mergeCell ref="B1165:F1165"/>
     <mergeCell ref="B581:F581"/>
+    <mergeCell ref="B1048:F1048"/>
     <mergeCell ref="B475:F475"/>
     <mergeCell ref="B768:F768"/>
     <mergeCell ref="B817:F817"/>
     <mergeCell ref="B944:F944"/>
     <mergeCell ref="B56:F56"/>
+    <mergeCell ref="B1102:F1102"/>
     <mergeCell ref="B43:F43"/>
     <mergeCell ref="B176:F176"/>
     <mergeCell ref="B347:F347"/>
@@ -19954,19 +22409,25 @@
     <mergeCell ref="B639:F639"/>
     <mergeCell ref="B710:F710"/>
     <mergeCell ref="B881:F881"/>
+    <mergeCell ref="B1068:F1068"/>
     <mergeCell ref="B868:F868"/>
+    <mergeCell ref="B1117:F1117"/>
     <mergeCell ref="B107:F107"/>
+    <mergeCell ref="B1104:F1104"/>
+    <mergeCell ref="B1160:F1160"/>
     <mergeCell ref="B641:F641"/>
     <mergeCell ref="B57:F57"/>
     <mergeCell ref="B883:F883"/>
     <mergeCell ref="B908:F908"/>
     <mergeCell ref="B171:F171"/>
+    <mergeCell ref="B1168:F1168"/>
     <mergeCell ref="B407:F407"/>
     <mergeCell ref="A646:F646"/>
     <mergeCell ref="B972:F972"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="B463:F463"/>
     <mergeCell ref="B438:F438"/>
+    <mergeCell ref="B1145:F1145"/>
     <mergeCell ref="B359:F359"/>
     <mergeCell ref="B207:F207"/>
     <mergeCell ref="B788:F788"/>
@@ -19979,7 +22440,10 @@
     <mergeCell ref="B934:F934"/>
     <mergeCell ref="B173:F173"/>
     <mergeCell ref="B999:F999"/>
+    <mergeCell ref="B1061:F1061"/>
     <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B1097:F1097"/>
+    <mergeCell ref="B1153:F1153"/>
     <mergeCell ref="A46:F46"/>
     <mergeCell ref="B507:F507"/>
     <mergeCell ref="B62:F62"/>
@@ -19993,9 +22457,13 @@
     <mergeCell ref="B473:F473"/>
     <mergeCell ref="B273:F273"/>
     <mergeCell ref="B857:F857"/>
+    <mergeCell ref="B1063:F1063"/>
+    <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1161:F1161"/>
     <mergeCell ref="B807:F807"/>
     <mergeCell ref="B1000:F1000"/>
     <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B1092:F1092"/>
     <mergeCell ref="B508:F508"/>
     <mergeCell ref="B573:F573"/>
     <mergeCell ref="A961:F961"/>
@@ -20024,7 +22492,9 @@
     <mergeCell ref="B1018:F1018"/>
     <mergeCell ref="B624:F624"/>
     <mergeCell ref="B428:F428"/>
+    <mergeCell ref="B1118:F1118"/>
     <mergeCell ref="B284:F284"/>
+    <mergeCell ref="B1167:F1167"/>
     <mergeCell ref="B222:F222"/>
     <mergeCell ref="B344:F344"/>
     <mergeCell ref="B415:F415"/>
@@ -20035,6 +22505,7 @@
     <mergeCell ref="B123:F123"/>
     <mergeCell ref="B949:F949"/>
     <mergeCell ref="B1011:F1011"/>
+    <mergeCell ref="B1120:F1120"/>
     <mergeCell ref="B50:F50"/>
     <mergeCell ref="B221:F221"/>
     <mergeCell ref="B110:F110"/>
@@ -20051,6 +22522,7 @@
     <mergeCell ref="B802:F802"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="B789:F789"/>
+    <mergeCell ref="B1136:F1136"/>
     <mergeCell ref="B248:F248"/>
     <mergeCell ref="B297:F297"/>
     <mergeCell ref="B813:F813"/>
@@ -20064,13 +22536,17 @@
     <mergeCell ref="B337:F337"/>
     <mergeCell ref="B312:F312"/>
     <mergeCell ref="B579:F579"/>
+    <mergeCell ref="B1089:F1089"/>
     <mergeCell ref="B610:F610"/>
     <mergeCell ref="B877:F877"/>
     <mergeCell ref="B815:F815"/>
     <mergeCell ref="B597:F597"/>
+    <mergeCell ref="B1064:F1064"/>
+    <mergeCell ref="B1113:F1113"/>
     <mergeCell ref="B103:F103"/>
     <mergeCell ref="B78:F78"/>
     <mergeCell ref="B833:F833"/>
+    <mergeCell ref="B1100:F1100"/>
     <mergeCell ref="B205:F205"/>
     <mergeCell ref="B339:F339"/>
     <mergeCell ref="B314:F314"/>
@@ -20079,6 +22555,8 @@
     <mergeCell ref="B808:F808"/>
     <mergeCell ref="B879:F879"/>
     <mergeCell ref="B897:F897"/>
+    <mergeCell ref="B1164:F1164"/>
+    <mergeCell ref="B1158:F1158"/>
     <mergeCell ref="B403:F403"/>
     <mergeCell ref="B574:F574"/>
     <mergeCell ref="B745:F745"/>
@@ -20086,6 +22564,7 @@
     <mergeCell ref="B55:F55"/>
     <mergeCell ref="B1003:F1003"/>
     <mergeCell ref="B169:F169"/>
+    <mergeCell ref="B1166:F1166"/>
     <mergeCell ref="A706:F706"/>
     <mergeCell ref="B7:F7"/>
     <mergeCell ref="B129:F129"/>
@@ -20099,6 +22578,7 @@
     <mergeCell ref="B292:F292"/>
     <mergeCell ref="B492:F492"/>
     <mergeCell ref="B734:F734"/>
+    <mergeCell ref="B1082:F1082"/>
     <mergeCell ref="B528:F528"/>
     <mergeCell ref="B71:F71"/>
     <mergeCell ref="B1019:F1019"/>
@@ -20136,11 +22616,13 @@
     <mergeCell ref="B892:F892"/>
     <mergeCell ref="B53:F53"/>
     <mergeCell ref="A436:F436"/>
+    <mergeCell ref="B1079:F1079"/>
     <mergeCell ref="A121:F121"/>
     <mergeCell ref="B289:F289"/>
     <mergeCell ref="A721:F721"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="B747:F747"/>
+    <mergeCell ref="B1152:F1152"/>
     <mergeCell ref="B668:F668"/>
     <mergeCell ref="B84:F84"/>
     <mergeCell ref="A736:F736"/>
@@ -20151,6 +22633,7 @@
     <mergeCell ref="A1021:F1021"/>
     <mergeCell ref="B434:F434"/>
     <mergeCell ref="B605:F605"/>
+    <mergeCell ref="B1047:F1047"/>
     <mergeCell ref="B142:F142"/>
     <mergeCell ref="B313:F313"/>
     <mergeCell ref="B80:F80"/>
@@ -20163,8 +22646,10 @@
     <mergeCell ref="B305:F305"/>
     <mergeCell ref="B816:F816"/>
     <mergeCell ref="B918:F918"/>
+    <mergeCell ref="B1114:F1114"/>
     <mergeCell ref="B607:F607"/>
     <mergeCell ref="B663:F663"/>
+    <mergeCell ref="B1049:F1049"/>
     <mergeCell ref="B905:F905"/>
     <mergeCell ref="B1032:F1032"/>
     <mergeCell ref="B144:F144"/>
@@ -20172,6 +22657,7 @@
     <mergeCell ref="B442:F442"/>
     <mergeCell ref="B242:F242"/>
     <mergeCell ref="B880:F880"/>
+    <mergeCell ref="B1116:F1116"/>
     <mergeCell ref="B671:F671"/>
     <mergeCell ref="B969:F969"/>
     <mergeCell ref="B907:F907"/>
@@ -20189,12 +22675,15 @@
     <mergeCell ref="B760:F760"/>
     <mergeCell ref="B437:F437"/>
     <mergeCell ref="B852:F852"/>
+    <mergeCell ref="B1119:F1119"/>
     <mergeCell ref="B333:F333"/>
+    <mergeCell ref="B1098:F1098"/>
     <mergeCell ref="B898:F898"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B520:F520"/>
     <mergeCell ref="B958:F958"/>
     <mergeCell ref="B308:F308"/>
+    <mergeCell ref="B1134:F1134"/>
     <mergeCell ref="B854:F854"/>
     <mergeCell ref="B99:F99"/>
     <mergeCell ref="B737:F737"/>
@@ -20211,26 +22700,33 @@
     <mergeCell ref="B239:F239"/>
     <mergeCell ref="B310:F310"/>
     <mergeCell ref="B372:F372"/>
+    <mergeCell ref="B1071:F1071"/>
     <mergeCell ref="B608:F608"/>
+    <mergeCell ref="B1127:F1127"/>
     <mergeCell ref="B595:F595"/>
+    <mergeCell ref="B1037:F1037"/>
     <mergeCell ref="B722:F722"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="A856:F856"/>
     <mergeCell ref="B893:F893"/>
+    <mergeCell ref="B1129:F1129"/>
     <mergeCell ref="B374:F374"/>
     <mergeCell ref="B659:F659"/>
     <mergeCell ref="B830:F830"/>
     <mergeCell ref="A871:F871"/>
     <mergeCell ref="B895:F895"/>
+    <mergeCell ref="A1156:F1156"/>
     <mergeCell ref="B232:F232"/>
     <mergeCell ref="B321:F321"/>
     <mergeCell ref="B215:F215"/>
     <mergeCell ref="B513:F513"/>
     <mergeCell ref="B684:F684"/>
     <mergeCell ref="B982:F982"/>
+    <mergeCell ref="B1053:F1053"/>
     <mergeCell ref="B21:F21"/>
     <mergeCell ref="B847:F847"/>
     <mergeCell ref="B263:F263"/>
+    <mergeCell ref="B1040:F1040"/>
     <mergeCell ref="B152:F152"/>
     <mergeCell ref="B323:F323"/>
     <mergeCell ref="A76:F76"/>
@@ -20283,6 +22779,8 @@
     <mergeCell ref="B309:F309"/>
     <mergeCell ref="A316:F316"/>
     <mergeCell ref="B380:F380"/>
+    <mergeCell ref="B1135:F1135"/>
+    <mergeCell ref="A1081:F1081"/>
     <mergeCell ref="B100:F100"/>
     <mergeCell ref="B336:F336"/>
     <mergeCell ref="B634:F634"/>
@@ -20291,21 +22789,25 @@
     <mergeCell ref="B140:F140"/>
     <mergeCell ref="B115:F115"/>
     <mergeCell ref="B382:F382"/>
+    <mergeCell ref="A1096:F1096"/>
     <mergeCell ref="B680:F680"/>
     <mergeCell ref="A376:F376"/>
     <mergeCell ref="B102:F102"/>
     <mergeCell ref="B674:F674"/>
+    <mergeCell ref="B1137:F1137"/>
     <mergeCell ref="B400:F400"/>
     <mergeCell ref="B698:F698"/>
     <mergeCell ref="B832:F832"/>
     <mergeCell ref="B77:F77"/>
     <mergeCell ref="B903:F903"/>
     <mergeCell ref="B965:F965"/>
+    <mergeCell ref="B1074:F1074"/>
     <mergeCell ref="B440:F440"/>
     <mergeCell ref="B611:F611"/>
     <mergeCell ref="B598:F598"/>
     <mergeCell ref="B402:F402"/>
     <mergeCell ref="B669:F669"/>
+    <mergeCell ref="B1138:F1138"/>
     <mergeCell ref="B377:F377"/>
     <mergeCell ref="A451:F451"/>
     <mergeCell ref="B29:F29"/>
@@ -20315,6 +22817,7 @@
     <mergeCell ref="B756:F756"/>
     <mergeCell ref="B992:F992"/>
     <mergeCell ref="A811:F811"/>
+    <mergeCell ref="B1150:F1150"/>
     <mergeCell ref="B329:F329"/>
     <mergeCell ref="B627:F627"/>
     <mergeCell ref="B49:F49"/>
@@ -20324,10 +22827,12 @@
     <mergeCell ref="B614:F614"/>
     <mergeCell ref="A511:F511"/>
     <mergeCell ref="B785:F785"/>
+    <mergeCell ref="B1056:F1056"/>
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="B850:F850"/>
     <mergeCell ref="B95:F95"/>
     <mergeCell ref="B266:F266"/>
+    <mergeCell ref="B1043:F1043"/>
     <mergeCell ref="B89:F89"/>
     <mergeCell ref="B393:F393"/>
     <mergeCell ref="B453:F453"/>
@@ -20341,6 +22846,7 @@
     <mergeCell ref="B987:F987"/>
     <mergeCell ref="B787:F787"/>
     <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B1058:F1058"/>
     <mergeCell ref="B914:F914"/>
     <mergeCell ref="B197:F197"/>
     <mergeCell ref="B26:F26"/>
@@ -20358,11 +22864,15 @@
     <mergeCell ref="B851:F851"/>
     <mergeCell ref="B845:F845"/>
     <mergeCell ref="B261:F261"/>
+    <mergeCell ref="B1087:F1087"/>
+    <mergeCell ref="B1149:F1149"/>
     <mergeCell ref="B184:F184"/>
+    <mergeCell ref="B1062:F1062"/>
     <mergeCell ref="A301:F301"/>
     <mergeCell ref="B27:F27"/>
     <mergeCell ref="B782:F782"/>
     <mergeCell ref="A331:F331"/>
+    <mergeCell ref="B1069:F1069"/>
     <mergeCell ref="B548:F548"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="A616:F616"/>
@@ -20376,6 +22886,7 @@
     <mergeCell ref="B250:F250"/>
     <mergeCell ref="B927:F927"/>
     <mergeCell ref="B44:F44"/>
+    <mergeCell ref="B1163:F1163"/>
     <mergeCell ref="B408:F408"/>
     <mergeCell ref="B464:F464"/>
     <mergeCell ref="A916:F916"/>
@@ -20407,20 +22918,24 @@
     <mergeCell ref="B281:F281"/>
     <mergeCell ref="B775:F775"/>
     <mergeCell ref="B20:F20"/>
+    <mergeCell ref="A1036:F1036"/>
     <mergeCell ref="B497:F497"/>
     <mergeCell ref="B1033:F1033"/>
     <mergeCell ref="B983:F983"/>
+    <mergeCell ref="A1051:F1051"/>
     <mergeCell ref="B970:F970"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="B355:F355"/>
     <mergeCell ref="B134:F134"/>
     <mergeCell ref="B572:F572"/>
     <mergeCell ref="B759:F759"/>
+    <mergeCell ref="B1057:F1057"/>
     <mergeCell ref="B357:F357"/>
     <mergeCell ref="B995:F995"/>
     <mergeCell ref="B96:F96"/>
     <mergeCell ref="B922:F922"/>
     <mergeCell ref="B167:F167"/>
+    <mergeCell ref="B1093:F1093"/>
     <mergeCell ref="B332:F332"/>
     <mergeCell ref="B503:F503"/>
     <mergeCell ref="B701:F701"/>
@@ -20430,12 +22945,16 @@
     <mergeCell ref="B111:F111"/>
     <mergeCell ref="B617:F617"/>
     <mergeCell ref="B937:F937"/>
+    <mergeCell ref="B1059:F1059"/>
+    <mergeCell ref="B1086:F1086"/>
     <mergeCell ref="B853:F853"/>
     <mergeCell ref="B98:F98"/>
     <mergeCell ref="B986:F986"/>
     <mergeCell ref="B1024:F1024"/>
     <mergeCell ref="B396:F396"/>
     <mergeCell ref="B567:F567"/>
+    <mergeCell ref="B1151:F1151"/>
+    <mergeCell ref="B1157:F1157"/>
     <mergeCell ref="B632:F632"/>
     <mergeCell ref="B803:F803"/>
     <mergeCell ref="B996:F996"/>
@@ -20445,14 +22964,18 @@
     <mergeCell ref="B162:F162"/>
     <mergeCell ref="B267:F267"/>
     <mergeCell ref="B798:F798"/>
+    <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1159:F1159"/>
     <mergeCell ref="B398:F398"/>
     <mergeCell ref="B569:F569"/>
     <mergeCell ref="A466:F466"/>
     <mergeCell ref="B696:F696"/>
     <mergeCell ref="B867:F867"/>
+    <mergeCell ref="A1066:F1066"/>
     <mergeCell ref="B269:F269"/>
     <mergeCell ref="B187:F187"/>
     <mergeCell ref="B485:F485"/>
+    <mergeCell ref="B1154:F1154"/>
     <mergeCell ref="B124:F124"/>
     <mergeCell ref="B251:F251"/>
     <mergeCell ref="B806:F806"/>
@@ -20460,7 +22983,9 @@
     <mergeCell ref="B493:F493"/>
     <mergeCell ref="B216:F216"/>
     <mergeCell ref="B487:F487"/>
+    <mergeCell ref="B1077:F1077"/>
     <mergeCell ref="B343:F343"/>
+    <mergeCell ref="B1169:F1169"/>
     <mergeCell ref="B414:F414"/>
     <mergeCell ref="B474:F474"/>
     <mergeCell ref="B772:F772"/>
@@ -20497,11 +23022,15 @@
     <mergeCell ref="B409:F409"/>
     <mergeCell ref="B580:F580"/>
     <mergeCell ref="B920:F920"/>
+    <mergeCell ref="B1108:F1108"/>
     <mergeCell ref="B711:F711"/>
     <mergeCell ref="B1009:F1009"/>
     <mergeCell ref="B48:F48"/>
+    <mergeCell ref="B1101:F1101"/>
     <mergeCell ref="B582:F582"/>
     <mergeCell ref="B849:F849"/>
+    <mergeCell ref="B1147:F1147"/>
+    <mergeCell ref="B1132:F1132"/>
     <mergeCell ref="B73:F73"/>
     <mergeCell ref="B371:F371"/>
     <mergeCell ref="B638:F638"/>
@@ -20514,6 +23043,7 @@
     <mergeCell ref="A676:F676"/>
     <mergeCell ref="B137:F137"/>
     <mergeCell ref="B379:F379"/>
+    <mergeCell ref="B1106:F1106"/>
     <mergeCell ref="B702:F702"/>
     <mergeCell ref="B677:F677"/>
     <mergeCell ref="B640:F640"/>
@@ -20544,9 +23074,11 @@
     <mergeCell ref="B66:F66"/>
     <mergeCell ref="B326:F326"/>
     <mergeCell ref="B793:F793"/>
+    <mergeCell ref="B1103:F1103"/>
     <mergeCell ref="A406:F406"/>
     <mergeCell ref="B951:F951"/>
     <mergeCell ref="B130:F130"/>
+    <mergeCell ref="B1078:F1078"/>
     <mergeCell ref="A946:F946"/>
     <mergeCell ref="A631:F631"/>
     <mergeCell ref="B117:F117"/>
@@ -20561,6 +23093,8 @@
     <mergeCell ref="B132:F132"/>
     <mergeCell ref="B425:F425"/>
     <mergeCell ref="B430:F430"/>
+    <mergeCell ref="B1107:F1107"/>
+    <mergeCell ref="B1045:F1045"/>
     <mergeCell ref="B119:F119"/>
     <mergeCell ref="B290:F290"/>
     <mergeCell ref="B417:F417"/>
@@ -20570,10 +23104,13 @@
     <mergeCell ref="B824:F824"/>
     <mergeCell ref="B1017:F1017"/>
     <mergeCell ref="B367:F367"/>
+    <mergeCell ref="B1122:F1122"/>
     <mergeCell ref="B427:F427"/>
+    <mergeCell ref="B1139:F1139"/>
     <mergeCell ref="B112:F112"/>
     <mergeCell ref="B283:F283"/>
     <mergeCell ref="B354:F354"/>
+    <mergeCell ref="B1109:F1109"/>
     <mergeCell ref="B348:F348"/>
     <mergeCell ref="B519:F519"/>
     <mergeCell ref="B419:F419"/>
@@ -20589,6 +23126,7 @@
     <mergeCell ref="B648:F648"/>
     <mergeCell ref="B64:F64"/>
     <mergeCell ref="B51:F51"/>
+    <mergeCell ref="A1126:F1126"/>
     <mergeCell ref="B443:F443"/>
     <mergeCell ref="A196:F196"/>
     <mergeCell ref="B237:F237"/>
@@ -20663,6 +23201,15 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1004" r:id="rId67"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1019" r:id="rId68"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1034" r:id="rId69"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1049" r:id="rId70"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1064" r:id="rId71"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1079" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1094" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1109" r:id="rId74"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1124" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1139" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1154" r:id="rId77"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1169" r:id="rId78"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -20674,7 +23221,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -22786,7 +25333,7 @@
     <row r="56" ht="28" customHeight="1">
       <c r="A56" s="6" t="inlineStr">
         <is>
-          <t>EUS-15293</t>
+          <t>EUS-89962</t>
         </is>
       </c>
       <c r="B56" s="6" t="inlineStr">
@@ -22822,7 +25369,7 @@
     <row r="57" ht="28" customHeight="1">
       <c r="A57" s="6" t="inlineStr">
         <is>
-          <t>EUS-60835</t>
+          <t>EUS-51969</t>
         </is>
       </c>
       <c r="B57" s="6" t="inlineStr">
@@ -22858,7 +25405,7 @@
     <row r="58" ht="28" customHeight="1">
       <c r="A58" s="6" t="inlineStr">
         <is>
-          <t>EUS-59232</t>
+          <t>EUS-56284</t>
         </is>
       </c>
       <c r="B58" s="6" t="inlineStr">
@@ -22894,7 +25441,7 @@
     <row r="59" ht="28" customHeight="1">
       <c r="A59" s="6" t="inlineStr">
         <is>
-          <t>EUS-36628</t>
+          <t>EUS-28861</t>
         </is>
       </c>
       <c r="B59" s="6" t="inlineStr">
@@ -22930,7 +25477,7 @@
     <row r="60" ht="28" customHeight="1">
       <c r="A60" s="6" t="inlineStr">
         <is>
-          <t>EUS-18488</t>
+          <t>EUS-17841</t>
         </is>
       </c>
       <c r="B60" s="6" t="inlineStr">
@@ -22966,12 +25513,12 @@
     <row r="61" ht="28" customHeight="1">
       <c r="A61" s="6" t="inlineStr">
         <is>
-          <t>EUS-87234</t>
+          <t>EUS-27002</t>
         </is>
       </c>
       <c r="B61" s="6" t="inlineStr">
         <is>
-          <t>Programa de impulso a las ciudades y territorios inteligente</t>
+          <t>Asesoría Legal - Consultas tramitación de proyectos de energ</t>
         </is>
       </c>
       <c r="C61" s="6" t="inlineStr">
@@ -22987,7 +25534,7 @@
       <c r="E61" s="6" t="inlineStr"/>
       <c r="F61" s="25" t="inlineStr">
         <is>
-          <t>MEDIA</t>
+          <t>ALTA</t>
         </is>
       </c>
       <c r="G61" s="6" t="inlineStr"/>
@@ -23002,12 +25549,12 @@
     <row r="62" ht="28" customHeight="1">
       <c r="A62" s="6" t="inlineStr">
         <is>
-          <t>EUS-73772</t>
+          <t>EUS-18210</t>
         </is>
       </c>
       <c r="B62" s="6" t="inlineStr">
         <is>
-          <t>Formación digital para empleabilidad turística: los fondos N</t>
+          <t>Programa de impulso a las ciudades y territorios inteligente</t>
         </is>
       </c>
       <c r="C62" s="6" t="inlineStr">
@@ -23038,12 +25585,12 @@
     <row r="63" ht="28" customHeight="1">
       <c r="A63" s="6" t="inlineStr">
         <is>
-          <t>EUS-49109</t>
+          <t>EUS-59993</t>
         </is>
       </c>
       <c r="B63" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe. Clúster digital, industrial y espacial. Apoy</t>
+          <t>Formación digital para empleabilidad turística: los fondos N</t>
         </is>
       </c>
       <c r="C63" s="6" t="inlineStr">
@@ -23074,12 +25621,12 @@
     <row r="64" ht="28" customHeight="1">
       <c r="A64" s="6" t="inlineStr">
         <is>
-          <t>EUS-72760</t>
+          <t>EUS-25797</t>
         </is>
       </c>
       <c r="B64" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horizon Europe: ayudas de la línea de energía del clúster 5 </t>
+          <t>Horizon Europe. Clúster digital, industrial y espacial. Apoy</t>
         </is>
       </c>
       <c r="C64" s="6" t="inlineStr">
@@ -23110,12 +25657,12 @@
     <row r="65" ht="28" customHeight="1">
       <c r="A65" s="6" t="inlineStr">
         <is>
-          <t>EUS-28905</t>
+          <t>EUS-12160</t>
         </is>
       </c>
       <c r="B65" s="6" t="inlineStr">
         <is>
-          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instal</t>
+          <t xml:space="preserve">Horizon Europe: ayudas de la línea de energía del clúster 5 </t>
         </is>
       </c>
       <c r="C65" s="6" t="inlineStr">
@@ -23146,12 +25693,12 @@
     <row r="66" ht="28" customHeight="1">
       <c r="A66" s="6" t="inlineStr">
         <is>
-          <t>EUS-54869</t>
+          <t>EUS-77123</t>
         </is>
       </c>
       <c r="B66" s="6" t="inlineStr">
         <is>
-          <t>Subvenciones para innovación en economía circular 2026</t>
+          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instal</t>
         </is>
       </c>
       <c r="C66" s="6" t="inlineStr">
@@ -23182,12 +25729,12 @@
     <row r="67" ht="28" customHeight="1">
       <c r="A67" s="6" t="inlineStr">
         <is>
-          <t>EUS-95967</t>
+          <t>EUS-64792</t>
         </is>
       </c>
       <c r="B67" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones amb</t>
+          <t>Subvenciones para innovación en economía circular 2026</t>
         </is>
       </c>
       <c r="C67" s="6" t="inlineStr">
@@ -23218,12 +25765,12 @@
     <row r="68" ht="28" customHeight="1">
       <c r="A68" s="6" t="inlineStr">
         <is>
-          <t>EUS-17430</t>
+          <t>EUS-00130</t>
         </is>
       </c>
       <c r="B68" s="6" t="inlineStr">
         <is>
-          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfab</t>
+          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones amb</t>
         </is>
       </c>
       <c r="C68" s="6" t="inlineStr">
@@ -23254,12 +25801,12 @@
     <row r="69" ht="28" customHeight="1">
       <c r="A69" s="6" t="inlineStr">
         <is>
-          <t>EUS-18205</t>
+          <t>EUS-83114</t>
         </is>
       </c>
       <c r="B69" s="6" t="inlineStr">
         <is>
-          <t>KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Indust</t>
+          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfab</t>
         </is>
       </c>
       <c r="C69" s="6" t="inlineStr">
@@ -23290,12 +25837,12 @@
     <row r="70" ht="28" customHeight="1">
       <c r="A70" s="6" t="inlineStr">
         <is>
-          <t>EUS-12970</t>
+          <t>EUS-36808</t>
         </is>
       </c>
       <c r="B70" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Asignaciones individualizadas de transporte escolar para el </t>
+          <t>KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Indust</t>
         </is>
       </c>
       <c r="C70" s="6" t="inlineStr">
@@ -23323,8 +25870,332 @@
       <c r="I70" s="6" t="inlineStr"/>
       <c r="J70" s="6" t="inlineStr"/>
     </row>
+    <row r="71" ht="28" customHeight="1">
+      <c r="A71" s="6" t="inlineStr">
+        <is>
+          <t>EUS-28459</t>
+        </is>
+      </c>
+      <c r="B71" s="6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asignaciones individualizadas de transporte escolar para el </t>
+        </is>
+      </c>
+      <c r="C71" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D71" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E71" s="6" t="inlineStr"/>
+      <c r="F71" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G71" s="6" t="inlineStr"/>
+      <c r="H71" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I71" s="6" t="inlineStr"/>
+      <c r="J71" s="6" t="inlineStr"/>
+    </row>
+    <row r="72" ht="28" customHeight="1">
+      <c r="A72" s="6" t="inlineStr">
+        <is>
+          <t>EUS-68968</t>
+        </is>
+      </c>
+      <c r="B72" s="6" t="inlineStr">
+        <is>
+          <t>Mantenimiento preventivo de 10 grúas de techo ubicadas en el</t>
+        </is>
+      </c>
+      <c r="C72" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D72" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E72" s="6" t="inlineStr"/>
+      <c r="F72" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G72" s="6" t="inlineStr"/>
+      <c r="H72" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I72" s="6" t="inlineStr"/>
+      <c r="J72" s="6" t="inlineStr"/>
+    </row>
+    <row r="73" ht="28" customHeight="1">
+      <c r="A73" s="6" t="inlineStr">
+        <is>
+          <t>EUS-40629</t>
+        </is>
+      </c>
+      <c r="B73" s="6" t="inlineStr">
+        <is>
+          <t>Asesoría Legal - Asesoramiento legal contestación borofax So</t>
+        </is>
+      </c>
+      <c r="C73" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D73" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E73" s="6" t="inlineStr"/>
+      <c r="F73" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G73" s="6" t="inlineStr"/>
+      <c r="H73" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I73" s="6" t="inlineStr"/>
+      <c r="J73" s="6" t="inlineStr"/>
+    </row>
+    <row r="74" ht="28" customHeight="1">
+      <c r="A74" s="6" t="inlineStr">
+        <is>
+          <t>EUS-35956</t>
+        </is>
+      </c>
+      <c r="B74" s="6" t="inlineStr">
+        <is>
+          <t>Otras Consultorías/ Servicios - Asesoramiento en la valoraci</t>
+        </is>
+      </c>
+      <c r="C74" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D74" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E74" s="6" t="inlineStr"/>
+      <c r="F74" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G74" s="6" t="inlineStr"/>
+      <c r="H74" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I74" s="6" t="inlineStr"/>
+      <c r="J74" s="6" t="inlineStr"/>
+    </row>
+    <row r="75" ht="28" customHeight="1">
+      <c r="A75" s="6" t="inlineStr">
+        <is>
+          <t>EUS-21012</t>
+        </is>
+      </c>
+      <c r="B75" s="6" t="inlineStr">
+        <is>
+          <t>Otras Consultorías/ Servicios - Asesoramiento en la valoraci</t>
+        </is>
+      </c>
+      <c r="C75" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D75" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E75" s="6" t="inlineStr"/>
+      <c r="F75" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G75" s="6" t="inlineStr"/>
+      <c r="H75" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I75" s="6" t="inlineStr"/>
+      <c r="J75" s="6" t="inlineStr"/>
+    </row>
+    <row r="76" ht="28" customHeight="1">
+      <c r="A76" s="6" t="inlineStr">
+        <is>
+          <t>EUS-80336</t>
+        </is>
+      </c>
+      <c r="B76" s="6" t="inlineStr">
+        <is>
+          <t>Asesoría Legal - Asesoramiento en negociación proyecto plant</t>
+        </is>
+      </c>
+      <c r="C76" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D76" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E76" s="6" t="inlineStr"/>
+      <c r="F76" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G76" s="6" t="inlineStr"/>
+      <c r="H76" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I76" s="6" t="inlineStr"/>
+      <c r="J76" s="6" t="inlineStr"/>
+    </row>
+    <row r="77" ht="28" customHeight="1">
+      <c r="A77" s="6" t="inlineStr">
+        <is>
+          <t>EUS-82751</t>
+        </is>
+      </c>
+      <c r="B77" s="6" t="inlineStr">
+        <is>
+          <t>Limpieza de foso ascensor san juan mekola</t>
+        </is>
+      </c>
+      <c r="C77" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D77" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E77" s="6" t="inlineStr"/>
+      <c r="F77" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G77" s="6" t="inlineStr"/>
+      <c r="H77" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I77" s="6" t="inlineStr"/>
+      <c r="J77" s="6" t="inlineStr"/>
+    </row>
+    <row r="78" ht="28" customHeight="1">
+      <c r="A78" s="6" t="inlineStr">
+        <is>
+          <t>EUS-08134</t>
+        </is>
+      </c>
+      <c r="B78" s="6" t="inlineStr">
+        <is>
+          <t>Limpieza sumideros de errebal</t>
+        </is>
+      </c>
+      <c r="C78" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D78" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E78" s="6" t="inlineStr"/>
+      <c r="F78" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G78" s="6" t="inlineStr"/>
+      <c r="H78" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I78" s="6" t="inlineStr"/>
+      <c r="J78" s="6" t="inlineStr"/>
+    </row>
+    <row r="79" ht="28" customHeight="1">
+      <c r="A79" s="6" t="inlineStr">
+        <is>
+          <t>EUS-92185</t>
+        </is>
+      </c>
+      <c r="B79" s="6" t="inlineStr">
+        <is>
+          <t>Reparación de cableados de circuitos de fuerza y alumbrado q</t>
+        </is>
+      </c>
+      <c r="C79" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D79" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E79" s="6" t="inlineStr"/>
+      <c r="F79" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G79" s="6" t="inlineStr"/>
+      <c r="H79" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I79" s="6" t="inlineStr"/>
+      <c r="J79" s="6" t="inlineStr"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J70"/>
+  <autoFilter ref="A1:J79"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update funding data 2026-02-22
</commit_message>
<xml_diff>
--- a/docs/resultados_convocatorias.xlsx
+++ b/docs/resultados_convocatorias.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Recursos" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen'!$A$4:$M$104</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Seguimiento'!$A$1:$J$99</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen'!$A$4:$M$103</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Seguimiento'!$A$1:$J$98</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -78,13 +78,13 @@
     <font>
       <name val="Leelawadee UI"/>
       <b val="1"/>
-      <color rgb="00DC2626"/>
+      <color rgb="00065F46"/>
       <sz val="10"/>
     </font>
     <font>
       <name val="Leelawadee UI"/>
       <b val="1"/>
-      <color rgb="00065F46"/>
+      <color rgb="00DC2626"/>
       <sz val="10"/>
     </font>
     <font>
@@ -145,11 +145,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00FEF2F2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00DCFCE7"/>
       </patternFill>
     </fill>
@@ -161,6 +156,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="00D1FAE5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FEF2F2"/>
       </patternFill>
     </fill>
     <fill>
@@ -243,14 +243,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="11" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -290,8 +290,8 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -657,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -691,7 +691,7 @@
     <row r="2" ht="22" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Mision Climatica - Neutralidad 2030 - Actualizado: 21/02/2026 07:47 - 98 convocatorias - 34 nuevas</t>
+          <t>Mision Climatica - Neutralidad 2030 - Actualizado: 22/02/2026 07:55 - 97 convocatorias - 30 nuevas</t>
         </is>
       </c>
     </row>
@@ -1198,12 +1198,12 @@
       </c>
       <c r="B13" s="6" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-MSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-SSP</t>
         </is>
       </c>
       <c r="C13" s="6" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
         </is>
       </c>
       <c r="D13" s="6" t="inlineStr">
@@ -1239,7 +1239,7 @@
       </c>
       <c r="K13" s="6" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
         </is>
       </c>
       <c r="L13" s="6" t="inlineStr"/>
@@ -1257,12 +1257,12 @@
       </c>
       <c r="B14" s="6" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-SSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-LSP</t>
         </is>
       </c>
       <c r="C14" s="6" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
         </is>
       </c>
       <c r="D14" s="6" t="inlineStr">
@@ -1298,7 +1298,7 @@
       </c>
       <c r="K14" s="6" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
         </is>
       </c>
       <c r="L14" s="6" t="inlineStr"/>
@@ -1316,12 +1316,12 @@
       </c>
       <c r="B15" s="6" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-LSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-MSP</t>
         </is>
       </c>
       <c r="C15" s="6" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
         </is>
       </c>
       <c r="D15" s="6" t="inlineStr">
@@ -1357,7 +1357,7 @@
       </c>
       <c r="K15" s="6" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
         </is>
       </c>
       <c r="L15" s="6" t="inlineStr"/>
@@ -3789,11 +3789,7 @@
           <t>Expected Outcome:Project results are expected to contribute to the following outcome:Accelerating the commercial availability of Direct Air Capture technologies.  Scope:Projects are expected to aim at</t>
         </is>
       </c>
-      <c r="L54" s="12" t="inlineStr">
-        <is>
-          <t>NUEVA</t>
-        </is>
-      </c>
+      <c r="L54" s="6" t="inlineStr"/>
       <c r="M54" s="9" t="inlineStr">
         <is>
           <t>Ver</t>
@@ -3856,11 +3852,7 @@
           <t>Expected Outcome:Project results are expected to contribute to all of the following expected outcomes:Strengthening of the joint EU-AU Climate Change and Sustainable Energy Collaborative Partnership e</t>
         </is>
       </c>
-      <c r="L55" s="12" t="inlineStr">
-        <is>
-          <t>NUEVA</t>
-        </is>
-      </c>
+      <c r="L55" s="6" t="inlineStr"/>
       <c r="M55" s="9" t="inlineStr">
         <is>
           <t>Ver</t>
@@ -3923,11 +3915,7 @@
           <t>Expected Outcome:Project results are expected to contribute to all of the following expected outcomes:Advance in the realisation of the Strategic Energy Technology (SET) Plan Action of Renewable fuels</t>
         </is>
       </c>
-      <c r="L56" s="12" t="inlineStr">
-        <is>
-          <t>NUEVA</t>
-        </is>
-      </c>
+      <c r="L56" s="6" t="inlineStr"/>
       <c r="M56" s="9" t="inlineStr">
         <is>
           <t>Ver</t>
@@ -3959,7 +3947,7 @@
       <c r="F57" s="6" t="inlineStr"/>
       <c r="G57" s="6" t="inlineStr"/>
       <c r="H57" s="6" t="inlineStr"/>
-      <c r="I57" s="13" t="inlineStr">
+      <c r="I57" s="12" t="inlineStr">
         <is>
           <t>MUY ALTA</t>
         </is>
@@ -4006,7 +3994,7 @@
       <c r="F58" s="6" t="inlineStr"/>
       <c r="G58" s="6" t="inlineStr"/>
       <c r="H58" s="6" t="inlineStr"/>
-      <c r="I58" s="13" t="inlineStr">
+      <c r="I58" s="12" t="inlineStr">
         <is>
           <t>MUY ALTA</t>
         </is>
@@ -4561,7 +4549,7 @@
       </c>
       <c r="B70" s="6" t="inlineStr">
         <is>
-          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="C70" s="6" t="inlineStr">
@@ -4608,7 +4596,7 @@
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
@@ -4695,21 +4683,21 @@
       </c>
     </row>
     <row r="73" ht="28" customHeight="1">
-      <c r="A73" s="14" t="inlineStr">
+      <c r="A73" s="13" t="inlineStr">
         <is>
           <t>🟢 Euskadi</t>
         </is>
       </c>
     </row>
     <row r="74" ht="40" customHeight="1">
-      <c r="A74" s="15" t="inlineStr">
+      <c r="A74" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B74" s="6" t="inlineStr">
         <is>
-          <t>EUS-99821</t>
+          <t>EUS-98933</t>
         </is>
       </c>
       <c r="C74" s="6" t="inlineStr">
@@ -4734,7 +4722,7 @@
           <t>Licitacion Euskadi</t>
         </is>
       </c>
-      <c r="I74" s="13" t="inlineStr">
+      <c r="I74" s="12" t="inlineStr">
         <is>
           <t>MUY ALTA</t>
         </is>
@@ -4745,7 +4733,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L74" s="12" t="inlineStr">
+      <c r="L74" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -4757,14 +4745,14 @@
       </c>
     </row>
     <row r="75" ht="40" customHeight="1">
-      <c r="A75" s="15" t="inlineStr">
+      <c r="A75" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B75" s="6" t="inlineStr">
         <is>
-          <t>EUS-63525</t>
+          <t>EUS-82759</t>
         </is>
       </c>
       <c r="C75" s="6" t="inlineStr">
@@ -4800,7 +4788,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L75" s="12" t="inlineStr">
+      <c r="L75" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -4812,14 +4800,14 @@
       </c>
     </row>
     <row r="76" ht="40" customHeight="1">
-      <c r="A76" s="15" t="inlineStr">
+      <c r="A76" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B76" s="6" t="inlineStr">
         <is>
-          <t>EUS-89917</t>
+          <t>EUS-20999</t>
         </is>
       </c>
       <c r="C76" s="6" t="inlineStr">
@@ -4855,7 +4843,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L76" s="12" t="inlineStr">
+      <c r="L76" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -4867,14 +4855,14 @@
       </c>
     </row>
     <row r="77" ht="40" customHeight="1">
-      <c r="A77" s="15" t="inlineStr">
+      <c r="A77" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>EUS-14531</t>
+          <t>EUS-06061</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
@@ -4910,7 +4898,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L77" s="12" t="inlineStr">
+      <c r="L77" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -4922,14 +4910,14 @@
       </c>
     </row>
     <row r="78" ht="40" customHeight="1">
-      <c r="A78" s="15" t="inlineStr">
+      <c r="A78" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B78" s="6" t="inlineStr">
         <is>
-          <t>EUS-08350</t>
+          <t>EUS-31808</t>
         </is>
       </c>
       <c r="C78" s="6" t="inlineStr">
@@ -4965,7 +4953,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L78" s="12" t="inlineStr">
+      <c r="L78" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -4977,14 +4965,14 @@
       </c>
     </row>
     <row r="79" ht="40" customHeight="1">
-      <c r="A79" s="15" t="inlineStr">
+      <c r="A79" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B79" s="6" t="inlineStr">
         <is>
-          <t>EUS-94562</t>
+          <t>EUS-28729</t>
         </is>
       </c>
       <c r="C79" s="6" t="inlineStr">
@@ -5020,7 +5008,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L79" s="12" t="inlineStr">
+      <c r="L79" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5032,14 +5020,14 @@
       </c>
     </row>
     <row r="80" ht="40" customHeight="1">
-      <c r="A80" s="15" t="inlineStr">
+      <c r="A80" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B80" s="6" t="inlineStr">
         <is>
-          <t>EUS-56734</t>
+          <t>EUS-90487</t>
         </is>
       </c>
       <c r="C80" s="6" t="inlineStr">
@@ -5075,7 +5063,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L80" s="12" t="inlineStr">
+      <c r="L80" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5087,19 +5075,19 @@
       </c>
     </row>
     <row r="81" ht="40" customHeight="1">
-      <c r="A81" s="15" t="inlineStr">
+      <c r="A81" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B81" s="6" t="inlineStr">
         <is>
-          <t>EUS-74809</t>
+          <t>EUS-69558</t>
         </is>
       </c>
       <c r="C81" s="6" t="inlineStr">
         <is>
-          <t>Servicios de Asistencia Técnica para la caracterización de los residuos domésticos y similares de Gipuzkoa en 2026</t>
+          <t xml:space="preserve">FEADER, Fondo Europeo Agrícola de Desarrollo Rural, cofinancia convocatorias de ayudas de Gipuzkoa a explotaciones con limitaciones o desfavorecidas, y a compromisos medioambientales, climáticos y de </t>
         </is>
       </c>
       <c r="D81" s="6" t="inlineStr">
@@ -5116,12 +5104,12 @@
       <c r="G81" s="6" t="inlineStr"/>
       <c r="H81" s="6" t="inlineStr">
         <is>
-          <t>Licitacion Euskadi</t>
-        </is>
-      </c>
-      <c r="I81" s="8" t="inlineStr">
-        <is>
-          <t>ALTA</t>
+          <t>Ayuda/Subvencion Euskadi</t>
+        </is>
+      </c>
+      <c r="I81" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
         </is>
       </c>
       <c r="J81" s="6" t="inlineStr"/>
@@ -5130,7 +5118,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L81" s="12" t="inlineStr">
+      <c r="L81" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5142,19 +5130,19 @@
       </c>
     </row>
     <row r="82" ht="40" customHeight="1">
-      <c r="A82" s="15" t="inlineStr">
+      <c r="A82" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B82" s="6" t="inlineStr">
         <is>
-          <t>EUS-36721</t>
+          <t>EUS-43782</t>
         </is>
       </c>
       <c r="C82" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">FEADER, Fondo Europeo Agrícola de Desarrollo Rural, cofinancia convocatorias de ayudas de Gipuzkoa a explotaciones con limitaciones o desfavorecidas, y a compromisos medioambientales, climáticos y de </t>
+          <t>Digital Europe, Horizon (programas de la UE). Apoyos para consorcios interestatales de I+D+i. IA, robótica, cuántica, computación, ciberseguridad, electrónica, fotónica, TICs e internet avanzadas, esp</t>
         </is>
       </c>
       <c r="D82" s="6" t="inlineStr">
@@ -5185,7 +5173,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L82" s="12" t="inlineStr">
+      <c r="L82" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5197,19 +5185,19 @@
       </c>
     </row>
     <row r="83" ht="40" customHeight="1">
-      <c r="A83" s="15" t="inlineStr">
+      <c r="A83" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B83" s="6" t="inlineStr">
         <is>
-          <t>EUS-88645</t>
+          <t>EUS-07831</t>
         </is>
       </c>
       <c r="C83" s="6" t="inlineStr">
         <is>
-          <t>Digital Europe, Horizon (programas de la UE). Apoyos para consorcios interestatales de I+D+i. IA, robótica, cuántica, computación, ciberseguridad, electrónica, fotónica, TICs e internet avanzadas, esp</t>
+          <t>Salud, cáncer. Programas de Horizon, EIC, IHI. Apoyos para consorcios internacionales de I+D+i. Jornada del Gobierno Vasco y con Enterprise Europe Network y otros socios. Digitalización, dispositivos,</t>
         </is>
       </c>
       <c r="D83" s="6" t="inlineStr">
@@ -5240,7 +5228,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L83" s="12" t="inlineStr">
+      <c r="L83" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5252,19 +5240,19 @@
       </c>
     </row>
     <row r="84" ht="40" customHeight="1">
-      <c r="A84" s="15" t="inlineStr">
+      <c r="A84" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B84" s="6" t="inlineStr">
         <is>
-          <t>EUS-55804</t>
+          <t>EUS-30486</t>
         </is>
       </c>
       <c r="C84" s="6" t="inlineStr">
         <is>
-          <t>Salud, cáncer. Programas de Horizon, EIC, IHI. Apoyos para consorcios internacionales de I+D+i. Jornada del Gobierno Vasco y con Enterprise Europe Network y otros socios. Digitalización, dispositivos,</t>
+          <t>Política Agraria Común de la UE de 2026, y sus ayudas abiertas hasta el 30.4.26: el pilar 1, con el Fondo Europeo Agrícola de Garantía Agraria FEAGA, aborda sostenibilidad de renta, ayuda redistributi</t>
         </is>
       </c>
       <c r="D84" s="6" t="inlineStr">
@@ -5295,7 +5283,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L84" s="12" t="inlineStr">
+      <c r="L84" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5307,19 +5295,19 @@
       </c>
     </row>
     <row r="85" ht="40" customHeight="1">
-      <c r="A85" s="15" t="inlineStr">
+      <c r="A85" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B85" s="6" t="inlineStr">
         <is>
-          <t>EUS-49713</t>
+          <t>EUS-52331</t>
         </is>
       </c>
       <c r="C85" s="6" t="inlineStr">
         <is>
-          <t>Política Agraria Común de la UE de 2026, y sus ayudas abiertas hasta el 30.4.26: el pilar 1, con el Fondo Europeo Agrícola de Garantía Agraria FEAGA, aborda sostenibilidad de renta, ayuda redistributi</t>
+          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
         </is>
       </c>
       <c r="D85" s="6" t="inlineStr">
@@ -5350,7 +5338,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L85" s="12" t="inlineStr">
+      <c r="L85" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5362,19 +5350,19 @@
       </c>
     </row>
     <row r="86" ht="40" customHeight="1">
-      <c r="A86" s="15" t="inlineStr">
+      <c r="A86" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B86" s="6" t="inlineStr">
         <is>
-          <t>EUS-29678</t>
+          <t>EUS-70955</t>
         </is>
       </c>
       <c r="C86" s="6" t="inlineStr">
         <is>
-          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
+          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
         </is>
       </c>
       <c r="D86" s="6" t="inlineStr">
@@ -5405,7 +5393,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L86" s="12" t="inlineStr">
+      <c r="L86" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5417,19 +5405,19 @@
       </c>
     </row>
     <row r="87" ht="40" customHeight="1">
-      <c r="A87" s="15" t="inlineStr">
+      <c r="A87" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B87" s="6" t="inlineStr">
         <is>
-          <t>EUS-12762</t>
+          <t>EUS-28448</t>
         </is>
       </c>
       <c r="C87" s="6" t="inlineStr">
         <is>
-          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
+          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
         </is>
       </c>
       <c r="D87" s="6" t="inlineStr">
@@ -5460,7 +5448,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L87" s="12" t="inlineStr">
+      <c r="L87" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5472,19 +5460,19 @@
       </c>
     </row>
     <row r="88" ht="40" customHeight="1">
-      <c r="A88" s="15" t="inlineStr">
+      <c r="A88" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B88" s="6" t="inlineStr">
         <is>
-          <t>EUS-65368</t>
+          <t>EUS-61284</t>
         </is>
       </c>
       <c r="C88" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
+          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
         </is>
       </c>
       <c r="D88" s="6" t="inlineStr">
@@ -5515,7 +5503,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L88" s="12" t="inlineStr">
+      <c r="L88" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5527,19 +5515,19 @@
       </c>
     </row>
     <row r="89" ht="40" customHeight="1">
-      <c r="A89" s="15" t="inlineStr">
+      <c r="A89" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B89" s="6" t="inlineStr">
         <is>
-          <t>EUS-46726</t>
+          <t>EUS-82808</t>
         </is>
       </c>
       <c r="C89" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
+          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
         </is>
       </c>
       <c r="D89" s="6" t="inlineStr">
@@ -5570,7 +5558,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L89" s="12" t="inlineStr">
+      <c r="L89" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5582,19 +5570,19 @@
       </c>
     </row>
     <row r="90" ht="40" customHeight="1">
-      <c r="A90" s="15" t="inlineStr">
+      <c r="A90" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B90" s="6" t="inlineStr">
         <is>
-          <t>EUS-94309</t>
+          <t>EUS-36705</t>
         </is>
       </c>
       <c r="C90" s="6" t="inlineStr">
         <is>
-          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
+          <t>Subvenciones para innovación en economía circular 2026</t>
         </is>
       </c>
       <c r="D90" s="6" t="inlineStr">
@@ -5625,7 +5613,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L90" s="12" t="inlineStr">
+      <c r="L90" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5637,19 +5625,19 @@
       </c>
     </row>
     <row r="91" ht="40" customHeight="1">
-      <c r="A91" s="15" t="inlineStr">
+      <c r="A91" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>EUS-92798</t>
+          <t>EUS-15893</t>
         </is>
       </c>
       <c r="C91" s="6" t="inlineStr">
         <is>
-          <t>Subvenciones para innovación en economía circular 2026</t>
+          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
         </is>
       </c>
       <c r="D91" s="6" t="inlineStr">
@@ -5680,7 +5668,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L91" s="12" t="inlineStr">
+      <c r="L91" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5692,19 +5680,19 @@
       </c>
     </row>
     <row r="92" ht="40" customHeight="1">
-      <c r="A92" s="15" t="inlineStr">
+      <c r="A92" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B92" s="6" t="inlineStr">
         <is>
-          <t>EUS-33647</t>
+          <t>EUS-56381</t>
         </is>
       </c>
       <c r="C92" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
+          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
         </is>
       </c>
       <c r="D92" s="6" t="inlineStr">
@@ -5735,7 +5723,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L92" s="12" t="inlineStr">
+      <c r="L92" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5747,19 +5735,19 @@
       </c>
     </row>
     <row r="93" ht="40" customHeight="1">
-      <c r="A93" s="15" t="inlineStr">
+      <c r="A93" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B93" s="6" t="inlineStr">
         <is>
-          <t>EUS-37213</t>
+          <t>EUS-49807</t>
         </is>
       </c>
       <c r="C93" s="6" t="inlineStr">
         <is>
-          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
+          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
         </is>
       </c>
       <c r="D93" s="6" t="inlineStr">
@@ -5790,7 +5778,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L93" s="12" t="inlineStr">
+      <c r="L93" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5802,19 +5790,19 @@
       </c>
     </row>
     <row r="94" ht="40" customHeight="1">
-      <c r="A94" s="15" t="inlineStr">
+      <c r="A94" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B94" s="6" t="inlineStr">
         <is>
-          <t>EUS-17024</t>
+          <t>EUS-04869</t>
         </is>
       </c>
       <c r="C94" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
+          <t>Limpieza pozo de bombeo de los garajes de errebal</t>
         </is>
       </c>
       <c r="D94" s="6" t="inlineStr">
@@ -5831,7 +5819,7 @@
       <c r="G94" s="6" t="inlineStr"/>
       <c r="H94" s="6" t="inlineStr">
         <is>
-          <t>Ayuda/Subvencion Euskadi</t>
+          <t>Licitacion Euskadi</t>
         </is>
       </c>
       <c r="I94" s="10" t="inlineStr">
@@ -5845,7 +5833,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L94" s="12" t="inlineStr">
+      <c r="L94" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5857,19 +5845,19 @@
       </c>
     </row>
     <row r="95" ht="40" customHeight="1">
-      <c r="A95" s="15" t="inlineStr">
+      <c r="A95" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B95" s="6" t="inlineStr">
         <is>
-          <t>EUS-94613</t>
+          <t>EUS-58730</t>
         </is>
       </c>
       <c r="C95" s="6" t="inlineStr">
         <is>
-          <t>Limpieza pozo de bombeo de los garajes de errebal</t>
+          <t>Revisión y acondicionamiento de arqueta de pluviales en milaflores</t>
         </is>
       </c>
       <c r="D95" s="6" t="inlineStr">
@@ -5900,7 +5888,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L95" s="12" t="inlineStr">
+      <c r="L95" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5912,19 +5900,19 @@
       </c>
     </row>
     <row r="96" ht="40" customHeight="1">
-      <c r="A96" s="15" t="inlineStr">
+      <c r="A96" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B96" s="6" t="inlineStr">
         <is>
-          <t>EUS-23341</t>
+          <t>EUS-69687</t>
         </is>
       </c>
       <c r="C96" s="6" t="inlineStr">
         <is>
-          <t>Revisión y acondicionamiento de arqueta de pluviales en milaflores</t>
+          <t>servicio de consultoría/educación ambiental para la prestación de la asistencia técnica del pilotaje del programa Agenda 2030 Escolar de Astigarraga</t>
         </is>
       </c>
       <c r="D96" s="6" t="inlineStr">
@@ -5955,7 +5943,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L96" s="12" t="inlineStr">
+      <c r="L96" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -5967,19 +5955,19 @@
       </c>
     </row>
     <row r="97" ht="40" customHeight="1">
-      <c r="A97" s="15" t="inlineStr">
+      <c r="A97" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B97" s="6" t="inlineStr">
         <is>
-          <t>EUS-51873</t>
+          <t>EUS-63751</t>
         </is>
       </c>
       <c r="C97" s="6" t="inlineStr">
         <is>
-          <t>servicio de consultoría/educación ambiental para la prestación de la asistencia técnica del pilotaje del programa Agenda 2030 Escolar de Astigarraga</t>
+          <t>Apagado puntual del alumbrado municipal, con motivo de la celebración del espectáculo de Inauguración de Navidad</t>
         </is>
       </c>
       <c r="D97" s="6" t="inlineStr">
@@ -6010,7 +5998,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L97" s="12" t="inlineStr">
+      <c r="L97" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6022,19 +6010,19 @@
       </c>
     </row>
     <row r="98" ht="40" customHeight="1">
-      <c r="A98" s="15" t="inlineStr">
+      <c r="A98" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B98" s="6" t="inlineStr">
         <is>
-          <t>EUS-28738</t>
+          <t>EUS-50368</t>
         </is>
       </c>
       <c r="C98" s="6" t="inlineStr">
         <is>
-          <t>Apagado puntual del alumbrado municipal, con motivo de la celebración del espectáculo de Inauguración de Navidad</t>
+          <t>Realización de trabajos puntuales de reparación en la ventana de la 3ª planta, sustitución de manilla en la 1ª planta y ajuste de la puerta de entrada en el edificio PIA.</t>
         </is>
       </c>
       <c r="D98" s="6" t="inlineStr">
@@ -6065,7 +6053,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L98" s="12" t="inlineStr">
+      <c r="L98" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6077,19 +6065,19 @@
       </c>
     </row>
     <row r="99" ht="40" customHeight="1">
-      <c r="A99" s="15" t="inlineStr">
+      <c r="A99" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B99" s="6" t="inlineStr">
         <is>
-          <t>EUS-81513</t>
+          <t>EUS-66714</t>
         </is>
       </c>
       <c r="C99" s="6" t="inlineStr">
         <is>
-          <t>Realización de trabajos puntuales de reparación en la ventana de la 3ª planta, sustitución de manilla en la 1ª planta y ajuste de la puerta de entrada en el edificio PIA.</t>
+          <t>Servicio puntual para la configuración y adaptación del software para la recogida de solicitudes de participación en la OPE2022</t>
         </is>
       </c>
       <c r="D99" s="6" t="inlineStr">
@@ -6120,7 +6108,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L99" s="12" t="inlineStr">
+      <c r="L99" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6132,19 +6120,19 @@
       </c>
     </row>
     <row r="100" ht="40" customHeight="1">
-      <c r="A100" s="15" t="inlineStr">
+      <c r="A100" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B100" s="6" t="inlineStr">
         <is>
-          <t>EUS-64768</t>
+          <t>EUS-57664</t>
         </is>
       </c>
       <c r="C100" s="6" t="inlineStr">
         <is>
-          <t>Servicio puntual para la configuración y adaptación del software para la recogida de solicitudes de participación en la OPE2022</t>
+          <t>Suministro de una Columna de Boca de Riego para habilitación de un punto de agua.</t>
         </is>
       </c>
       <c r="D100" s="6" t="inlineStr">
@@ -6175,7 +6163,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L100" s="12" t="inlineStr">
+      <c r="L100" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6187,19 +6175,19 @@
       </c>
     </row>
     <row r="101" ht="40" customHeight="1">
-      <c r="A101" s="15" t="inlineStr">
+      <c r="A101" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B101" s="6" t="inlineStr">
         <is>
-          <t>EUS-29793</t>
+          <t>EUS-90980</t>
         </is>
       </c>
       <c r="C101" s="6" t="inlineStr">
         <is>
-          <t>Suministro de una Columna de Boca de Riego para habilitación de un punto de agua.</t>
+          <t>Servicio puntual de transporte de diverso material corporativo voluminoso con motivo de la celebración del evento DonoSTEAM 2025</t>
         </is>
       </c>
       <c r="D101" s="6" t="inlineStr">
@@ -6230,7 +6218,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L101" s="12" t="inlineStr">
+      <c r="L101" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6242,19 +6230,19 @@
       </c>
     </row>
     <row r="102" ht="40" customHeight="1">
-      <c r="A102" s="15" t="inlineStr">
+      <c r="A102" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B102" s="6" t="inlineStr">
         <is>
-          <t>EUS-50290</t>
+          <t>EUS-55479</t>
         </is>
       </c>
       <c r="C102" s="6" t="inlineStr">
         <is>
-          <t>Servicio puntual de transporte de diverso material corporativo voluminoso con motivo de la celebración del evento DonoSTEAM 2025</t>
+          <t>Suministro puntual de material de seguridad para el edificio PIA. Botas de agua modelo ISSA talla 42</t>
         </is>
       </c>
       <c r="D102" s="6" t="inlineStr">
@@ -6285,7 +6273,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L102" s="12" t="inlineStr">
+      <c r="L102" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6297,19 +6285,19 @@
       </c>
     </row>
     <row r="103" ht="40" customHeight="1">
-      <c r="A103" s="15" t="inlineStr">
+      <c r="A103" s="14" t="inlineStr">
         <is>
           <t>Euskadi</t>
         </is>
       </c>
       <c r="B103" s="6" t="inlineStr">
         <is>
-          <t>EUS-71511</t>
+          <t>EUS-25621</t>
         </is>
       </c>
       <c r="C103" s="6" t="inlineStr">
         <is>
-          <t>Suministro puntual de material de seguridad para el edificio PIA. Botas de agua modelo ISSA talla 42</t>
+          <t xml:space="preserve">Contratación de los servicios de recogida de información mediante encuestas telefónicas para la realización del barómetro ciudadano sobre la percepción social de las políticas de Garantía de Ingresos </t>
         </is>
       </c>
       <c r="D103" s="6" t="inlineStr">
@@ -6340,7 +6328,7 @@
           <t>Gobierno Vasco / Sector Publico Euskadi</t>
         </is>
       </c>
-      <c r="L103" s="12" t="inlineStr">
+      <c r="L103" s="15" t="inlineStr">
         <is>
           <t>NUEVA</t>
         </is>
@@ -6351,63 +6339,8 @@
         </is>
       </c>
     </row>
-    <row r="104" ht="40" customHeight="1">
-      <c r="A104" s="15" t="inlineStr">
-        <is>
-          <t>Euskadi</t>
-        </is>
-      </c>
-      <c r="B104" s="6" t="inlineStr">
-        <is>
-          <t>EUS-47511</t>
-        </is>
-      </c>
-      <c r="C104" s="6" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Contratación de los servicios de recogida de información mediante encuestas telefónicas para la realización del barómetro ciudadano sobre la percepción social de las políticas de Garantía de Ingresos </t>
-        </is>
-      </c>
-      <c r="D104" s="6" t="inlineStr">
-        <is>
-          <t>Euskadi</t>
-        </is>
-      </c>
-      <c r="E104" s="7" t="inlineStr">
-        <is>
-          <t>Open</t>
-        </is>
-      </c>
-      <c r="F104" s="6" t="inlineStr"/>
-      <c r="G104" s="6" t="inlineStr"/>
-      <c r="H104" s="6" t="inlineStr">
-        <is>
-          <t>Licitacion Euskadi</t>
-        </is>
-      </c>
-      <c r="I104" s="10" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="J104" s="6" t="inlineStr"/>
-      <c r="K104" s="6" t="inlineStr">
-        <is>
-          <t>Gobierno Vasco / Sector Publico Euskadi</t>
-        </is>
-      </c>
-      <c r="L104" s="12" t="inlineStr">
-        <is>
-          <t>NUEVA</t>
-        </is>
-      </c>
-      <c r="M104" s="9" t="inlineStr">
-        <is>
-          <t>Ver</t>
-        </is>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A4:M104"/>
+  <autoFilter ref="A4:M103"/>
   <mergeCells count="4">
     <mergeCell ref="A73:M73"/>
     <mergeCell ref="A2:M2"/>
@@ -6512,7 +6445,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M101" r:id="rId95"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M102" r:id="rId96"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M103" r:id="rId97"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M104" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6524,7 +6456,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1469"/>
+  <dimension ref="A1:F1454"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8067,7 +7999,7 @@
     <row r="106" ht="30" customHeight="1">
       <c r="A106" s="16" t="inlineStr">
         <is>
-          <t>FICHA 8: INNOVFUND-2025-NZT-GENERAL-MSP</t>
+          <t>FICHA 8: INNOVFUND-2025-NZT-GENERAL-SSP</t>
         </is>
       </c>
       <c r="B106" s="17" t="n"/>
@@ -8100,7 +8032,7 @@
       </c>
       <c r="B108" s="19" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
         </is>
       </c>
       <c r="C108" s="20" t="n"/>
@@ -8116,7 +8048,7 @@
       </c>
       <c r="B109" s="19" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-MSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-SSP</t>
         </is>
       </c>
       <c r="C109" s="20" t="n"/>
@@ -8228,7 +8160,7 @@
       </c>
       <c r="B116" s="19" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
         </is>
       </c>
       <c r="C116" s="20" t="n"/>
@@ -8276,7 +8208,7 @@
       </c>
       <c r="B119" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/INNOVFUND-2025-NZT-GENERAL-MSP</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/INNOVFUND-2025-NZT-GENERAL-SSP</t>
         </is>
       </c>
       <c r="C119" s="20" t="n"/>
@@ -8287,7 +8219,7 @@
     <row r="121" ht="30" customHeight="1">
       <c r="A121" s="16" t="inlineStr">
         <is>
-          <t>FICHA 9: INNOVFUND-2025-NZT-GENERAL-SSP</t>
+          <t>FICHA 9: INNOVFUND-2025-NZT-GENERAL-LSP</t>
         </is>
       </c>
       <c r="B121" s="17" t="n"/>
@@ -8320,7 +8252,7 @@
       </c>
       <c r="B123" s="19" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
         </is>
       </c>
       <c r="C123" s="20" t="n"/>
@@ -8336,7 +8268,7 @@
       </c>
       <c r="B124" s="19" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-SSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-LSP</t>
         </is>
       </c>
       <c r="C124" s="20" t="n"/>
@@ -8448,7 +8380,7 @@
       </c>
       <c r="B131" s="19" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Small-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
         </is>
       </c>
       <c r="C131" s="20" t="n"/>
@@ -8496,7 +8428,7 @@
       </c>
       <c r="B134" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/INNOVFUND-2025-NZT-GENERAL-SSP</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/INNOVFUND-2025-NZT-GENERAL-LSP</t>
         </is>
       </c>
       <c r="C134" s="20" t="n"/>
@@ -8507,7 +8439,7 @@
     <row r="136" ht="30" customHeight="1">
       <c r="A136" s="16" t="inlineStr">
         <is>
-          <t>FICHA 10: INNOVFUND-2025-NZT-GENERAL-LSP</t>
+          <t>FICHA 10: INNOVFUND-2025-NZT-GENERAL-MSP</t>
         </is>
       </c>
       <c r="B136" s="17" t="n"/>
@@ -8540,7 +8472,7 @@
       </c>
       <c r="B138" s="19" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
         </is>
       </c>
       <c r="C138" s="20" t="n"/>
@@ -8556,7 +8488,7 @@
       </c>
       <c r="B139" s="19" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-LSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-MSP</t>
         </is>
       </c>
       <c r="C139" s="20" t="n"/>
@@ -8668,7 +8600,7 @@
       </c>
       <c r="B146" s="19" t="inlineStr">
         <is>
-          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Large-Scale Projects</t>
+          <t>Innovation Fund 2025 Net Zero Technologies - General decarbonisation - Medium-Scale Projects</t>
         </is>
       </c>
       <c r="C146" s="20" t="n"/>
@@ -8716,7 +8648,7 @@
       </c>
       <c r="B149" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/INNOVFUND-2025-NZT-GENERAL-LSP</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/INNOVFUND-2025-NZT-GENERAL-MSP</t>
         </is>
       </c>
       <c r="C149" s="20" t="n"/>
@@ -20363,7 +20295,7 @@
     <row r="961" ht="30" customHeight="1">
       <c r="A961" s="16" t="inlineStr">
         <is>
-          <t>FICHA 65: 4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>FICHA 65: dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="B961" s="17" t="n"/>
@@ -20412,7 +20344,7 @@
       </c>
       <c r="B964" s="19" t="inlineStr">
         <is>
-          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="C964" s="20" t="n"/>
@@ -20500,7 +20432,7 @@
       </c>
       <c r="B970" s="19" t="inlineStr">
         <is>
-          <t>EC-REGIO/2025/MVP/0036-EXA</t>
+          <t>EC-REGIO/2025/MVP/0023-EXA</t>
         </is>
       </c>
       <c r="C970" s="20" t="n"/>
@@ -20560,7 +20492,7 @@
       </c>
       <c r="B974" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="C974" s="20" t="n"/>
@@ -20571,7 +20503,7 @@
     <row r="976" ht="30" customHeight="1">
       <c r="A976" s="16" t="inlineStr">
         <is>
-          <t>FICHA 66: dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>FICHA 66: 4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="B976" s="17" t="n"/>
@@ -20620,7 +20552,7 @@
       </c>
       <c r="B979" s="19" t="inlineStr">
         <is>
-          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="C979" s="20" t="n"/>
@@ -20708,7 +20640,7 @@
       </c>
       <c r="B985" s="19" t="inlineStr">
         <is>
-          <t>EC-REGIO/2025/MVP/0023-EXA</t>
+          <t>EC-REGIO/2025/MVP/0036-EXA</t>
         </is>
       </c>
       <c r="C985" s="20" t="n"/>
@@ -20768,7 +20700,7 @@
       </c>
       <c r="B989" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="C989" s="20" t="n"/>
@@ -20987,7 +20919,7 @@
     <row r="1006" ht="30" customHeight="1">
       <c r="A1006" s="16" t="inlineStr">
         <is>
-          <t>FICHA 68: EUS-99821</t>
+          <t>FICHA 68: EUS-98933</t>
         </is>
       </c>
       <c r="B1006" s="17" t="n"/>
@@ -21036,7 +20968,7 @@
       </c>
       <c r="B1009" s="19" t="inlineStr">
         <is>
-          <t>EUS-99821</t>
+          <t>EUS-98933</t>
         </is>
       </c>
       <c r="C1009" s="20" t="n"/>
@@ -21199,7 +21131,7 @@
     <row r="1021" ht="30" customHeight="1">
       <c r="A1021" s="16" t="inlineStr">
         <is>
-          <t>FICHA 69: EUS-63525</t>
+          <t>FICHA 69: EUS-82759</t>
         </is>
       </c>
       <c r="B1021" s="17" t="n"/>
@@ -21248,7 +21180,7 @@
       </c>
       <c r="B1024" s="19" t="inlineStr">
         <is>
-          <t>EUS-63525</t>
+          <t>EUS-82759</t>
         </is>
       </c>
       <c r="C1024" s="20" t="n"/>
@@ -21411,7 +21343,7 @@
     <row r="1036" ht="30" customHeight="1">
       <c r="A1036" s="16" t="inlineStr">
         <is>
-          <t>FICHA 70: EUS-89917</t>
+          <t>FICHA 70: EUS-20999</t>
         </is>
       </c>
       <c r="B1036" s="17" t="n"/>
@@ -21460,7 +21392,7 @@
       </c>
       <c r="B1039" s="19" t="inlineStr">
         <is>
-          <t>EUS-89917</t>
+          <t>EUS-20999</t>
         </is>
       </c>
       <c r="C1039" s="20" t="n"/>
@@ -21623,7 +21555,7 @@
     <row r="1051" ht="30" customHeight="1">
       <c r="A1051" s="16" t="inlineStr">
         <is>
-          <t>FICHA 71: EUS-14531</t>
+          <t>FICHA 71: EUS-06061</t>
         </is>
       </c>
       <c r="B1051" s="17" t="n"/>
@@ -21672,7 +21604,7 @@
       </c>
       <c r="B1054" s="19" t="inlineStr">
         <is>
-          <t>EUS-14531</t>
+          <t>EUS-06061</t>
         </is>
       </c>
       <c r="C1054" s="20" t="n"/>
@@ -21835,7 +21767,7 @@
     <row r="1066" ht="30" customHeight="1">
       <c r="A1066" s="16" t="inlineStr">
         <is>
-          <t>FICHA 72: EUS-08350</t>
+          <t>FICHA 72: EUS-31808</t>
         </is>
       </c>
       <c r="B1066" s="17" t="n"/>
@@ -21884,7 +21816,7 @@
       </c>
       <c r="B1069" s="19" t="inlineStr">
         <is>
-          <t>EUS-08350</t>
+          <t>EUS-31808</t>
         </is>
       </c>
       <c r="C1069" s="20" t="n"/>
@@ -22047,7 +21979,7 @@
     <row r="1081" ht="30" customHeight="1">
       <c r="A1081" s="16" t="inlineStr">
         <is>
-          <t>FICHA 73: EUS-94562</t>
+          <t>FICHA 73: EUS-28729</t>
         </is>
       </c>
       <c r="B1081" s="17" t="n"/>
@@ -22096,7 +22028,7 @@
       </c>
       <c r="B1084" s="19" t="inlineStr">
         <is>
-          <t>EUS-94562</t>
+          <t>EUS-28729</t>
         </is>
       </c>
       <c r="C1084" s="20" t="n"/>
@@ -22259,7 +22191,7 @@
     <row r="1096" ht="30" customHeight="1">
       <c r="A1096" s="16" t="inlineStr">
         <is>
-          <t>FICHA 74: EUS-56734</t>
+          <t>FICHA 74: EUS-90487</t>
         </is>
       </c>
       <c r="B1096" s="17" t="n"/>
@@ -22308,7 +22240,7 @@
       </c>
       <c r="B1099" s="19" t="inlineStr">
         <is>
-          <t>EUS-56734</t>
+          <t>EUS-90487</t>
         </is>
       </c>
       <c r="C1099" s="20" t="n"/>
@@ -22471,7 +22403,7 @@
     <row r="1111" ht="30" customHeight="1">
       <c r="A1111" s="16" t="inlineStr">
         <is>
-          <t>FICHA 75: EUS-74809</t>
+          <t>FICHA 75: EUS-69558</t>
         </is>
       </c>
       <c r="B1111" s="17" t="n"/>
@@ -22504,7 +22436,7 @@
       </c>
       <c r="B1113" s="19" t="inlineStr">
         <is>
-          <t>Servicios de Asistencia Técnica para la caracterización de los residuos domésticos y similares de Gipuzkoa en 2026</t>
+          <t xml:space="preserve">FEADER, Fondo Europeo Agrícola de Desarrollo Rural, cofinancia convocatorias de ayudas de Gipuzkoa a explotaciones con limitaciones o desfavorecidas, y a compromisos medioambientales, climáticos y de </t>
         </is>
       </c>
       <c r="C1113" s="20" t="n"/>
@@ -22520,7 +22452,7 @@
       </c>
       <c r="B1114" s="19" t="inlineStr">
         <is>
-          <t>EUS-74809</t>
+          <t>EUS-69558</t>
         </is>
       </c>
       <c r="C1114" s="20" t="n"/>
@@ -22596,7 +22528,7 @@
       </c>
       <c r="B1119" s="19" t="inlineStr">
         <is>
-          <t>Licitacion Euskadi</t>
+          <t>Ayuda/Subvencion Euskadi</t>
         </is>
       </c>
       <c r="C1119" s="20" t="n"/>
@@ -22654,9 +22586,9 @@
           <t>Relevancia Bilbao</t>
         </is>
       </c>
-      <c r="B1123" s="21" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ALTA — </t>
+      <c r="B1123" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
         </is>
       </c>
       <c r="C1123" s="20" t="n"/>
@@ -22672,7 +22604,7 @@
       </c>
       <c r="B1124" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/servicios-asistencia-tecnica-caracterizacion-residuos-domesticos-y-similares-gipuzkoa-2026/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/lgenfnpbgfa260218/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1124" s="20" t="n"/>
@@ -22683,7 +22615,7 @@
     <row r="1126" ht="30" customHeight="1">
       <c r="A1126" s="16" t="inlineStr">
         <is>
-          <t>FICHA 76: EUS-36721</t>
+          <t>FICHA 76: EUS-43782</t>
         </is>
       </c>
       <c r="B1126" s="17" t="n"/>
@@ -22716,7 +22648,7 @@
       </c>
       <c r="B1128" s="19" t="inlineStr">
         <is>
-          <t xml:space="preserve">FEADER, Fondo Europeo Agrícola de Desarrollo Rural, cofinancia convocatorias de ayudas de Gipuzkoa a explotaciones con limitaciones o desfavorecidas, y a compromisos medioambientales, climáticos y de </t>
+          <t>Digital Europe, Horizon (programas de la UE). Apoyos para consorcios interestatales de I+D+i. IA, robótica, cuántica, computación, ciberseguridad, electrónica, fotónica, TICs e internet avanzadas, esp</t>
         </is>
       </c>
       <c r="C1128" s="20" t="n"/>
@@ -22732,7 +22664,7 @@
       </c>
       <c r="B1129" s="19" t="inlineStr">
         <is>
-          <t>EUS-36721</t>
+          <t>EUS-43782</t>
         </is>
       </c>
       <c r="C1129" s="20" t="n"/>
@@ -22884,7 +22816,7 @@
       </c>
       <c r="B1139" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/lgenfnpbgfa260218/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260304digitalhorizoneen/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1139" s="20" t="n"/>
@@ -22895,7 +22827,7 @@
     <row r="1141" ht="30" customHeight="1">
       <c r="A1141" s="16" t="inlineStr">
         <is>
-          <t>FICHA 77: EUS-88645</t>
+          <t>FICHA 77: EUS-07831</t>
         </is>
       </c>
       <c r="B1141" s="17" t="n"/>
@@ -22928,7 +22860,7 @@
       </c>
       <c r="B1143" s="19" t="inlineStr">
         <is>
-          <t>Digital Europe, Horizon (programas de la UE). Apoyos para consorcios interestatales de I+D+i. IA, robótica, cuántica, computación, ciberseguridad, electrónica, fotónica, TICs e internet avanzadas, esp</t>
+          <t>Salud, cáncer. Programas de Horizon, EIC, IHI. Apoyos para consorcios internacionales de I+D+i. Jornada del Gobierno Vasco y con Enterprise Europe Network y otros socios. Digitalización, dispositivos,</t>
         </is>
       </c>
       <c r="C1143" s="20" t="n"/>
@@ -22944,7 +22876,7 @@
       </c>
       <c r="B1144" s="19" t="inlineStr">
         <is>
-          <t>EUS-88645</t>
+          <t>EUS-07831</t>
         </is>
       </c>
       <c r="C1144" s="20" t="n"/>
@@ -23096,7 +23028,7 @@
       </c>
       <c r="B1154" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260304digitalhorizoneen/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260303eicihihorizon/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1154" s="20" t="n"/>
@@ -23107,7 +23039,7 @@
     <row r="1156" ht="30" customHeight="1">
       <c r="A1156" s="16" t="inlineStr">
         <is>
-          <t>FICHA 78: EUS-55804</t>
+          <t>FICHA 78: EUS-30486</t>
         </is>
       </c>
       <c r="B1156" s="17" t="n"/>
@@ -23140,7 +23072,7 @@
       </c>
       <c r="B1158" s="19" t="inlineStr">
         <is>
-          <t>Salud, cáncer. Programas de Horizon, EIC, IHI. Apoyos para consorcios internacionales de I+D+i. Jornada del Gobierno Vasco y con Enterprise Europe Network y otros socios. Digitalización, dispositivos,</t>
+          <t>Política Agraria Común de la UE de 2026, y sus ayudas abiertas hasta el 30.4.26: el pilar 1, con el Fondo Europeo Agrícola de Garantía Agraria FEAGA, aborda sostenibilidad de renta, ayuda redistributi</t>
         </is>
       </c>
       <c r="C1158" s="20" t="n"/>
@@ -23156,7 +23088,7 @@
       </c>
       <c r="B1159" s="19" t="inlineStr">
         <is>
-          <t>EUS-55804</t>
+          <t>EUS-30486</t>
         </is>
       </c>
       <c r="C1159" s="20" t="n"/>
@@ -23308,7 +23240,7 @@
       </c>
       <c r="B1169" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260303eicihihorizon/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260216npblaguntzairekiak/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1169" s="20" t="n"/>
@@ -23319,7 +23251,7 @@
     <row r="1171" ht="30" customHeight="1">
       <c r="A1171" s="16" t="inlineStr">
         <is>
-          <t>FICHA 79: EUS-49713</t>
+          <t>FICHA 79: EUS-52331</t>
         </is>
       </c>
       <c r="B1171" s="17" t="n"/>
@@ -23352,7 +23284,7 @@
       </c>
       <c r="B1173" s="19" t="inlineStr">
         <is>
-          <t>Política Agraria Común de la UE de 2026, y sus ayudas abiertas hasta el 30.4.26: el pilar 1, con el Fondo Europeo Agrícola de Garantía Agraria FEAGA, aborda sostenibilidad de renta, ayuda redistributi</t>
+          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
         </is>
       </c>
       <c r="C1173" s="20" t="n"/>
@@ -23368,7 +23300,7 @@
       </c>
       <c r="B1174" s="19" t="inlineStr">
         <is>
-          <t>EUS-49713</t>
+          <t>EUS-52331</t>
         </is>
       </c>
       <c r="C1174" s="20" t="n"/>
@@ -23520,7 +23452,7 @@
       </c>
       <c r="B1184" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260216npblaguntzairekiak/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260204smartcities/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1184" s="20" t="n"/>
@@ -23531,7 +23463,7 @@
     <row r="1186" ht="30" customHeight="1">
       <c r="A1186" s="16" t="inlineStr">
         <is>
-          <t>FICHA 80: EUS-29678</t>
+          <t>FICHA 80: EUS-70955</t>
         </is>
       </c>
       <c r="B1186" s="17" t="n"/>
@@ -23564,7 +23496,7 @@
       </c>
       <c r="B1188" s="19" t="inlineStr">
         <is>
-          <t>Programa de impulso a las ciudades y territorios inteligentes para el fomento del desarrollo económico y productivo, que podrá ser cofinanciado por el Programa Plurirregional 2021-2027 del Fondo Europ</t>
+          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
         </is>
       </c>
       <c r="C1188" s="20" t="n"/>
@@ -23580,7 +23512,7 @@
       </c>
       <c r="B1189" s="19" t="inlineStr">
         <is>
-          <t>EUS-29678</t>
+          <t>EUS-70955</t>
         </is>
       </c>
       <c r="C1189" s="20" t="n"/>
@@ -23732,7 +23664,7 @@
       </c>
       <c r="B1199" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260204smartcities/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260119nextlanbidedigital/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1199" s="20" t="n"/>
@@ -23743,7 +23675,7 @@
     <row r="1201" ht="30" customHeight="1">
       <c r="A1201" s="16" t="inlineStr">
         <is>
-          <t>FICHA 81: EUS-12762</t>
+          <t>FICHA 81: EUS-28448</t>
         </is>
       </c>
       <c r="B1201" s="17" t="n"/>
@@ -23776,7 +23708,7 @@
       </c>
       <c r="B1203" s="19" t="inlineStr">
         <is>
-          <t>Formación digital para empleabilidad turística: los fondos Next de la UE apoyan una convocatoria de Lanbide y el Gobierno Vasco, de cursos en línea para mejorar las competencias del sector y de sus py</t>
+          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
         </is>
       </c>
       <c r="C1203" s="20" t="n"/>
@@ -23792,7 +23724,7 @@
       </c>
       <c r="B1204" s="19" t="inlineStr">
         <is>
-          <t>EUS-12762</t>
+          <t>EUS-28448</t>
         </is>
       </c>
       <c r="C1204" s="20" t="n"/>
@@ -23944,7 +23876,7 @@
       </c>
       <c r="B1214" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260119nextlanbidedigital/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/250119horizondiginduspaceklust/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1214" s="20" t="n"/>
@@ -23955,7 +23887,7 @@
     <row r="1216" ht="30" customHeight="1">
       <c r="A1216" s="16" t="inlineStr">
         <is>
-          <t>FICHA 82: EUS-65368</t>
+          <t>FICHA 82: EUS-61284</t>
         </is>
       </c>
       <c r="B1216" s="17" t="n"/>
@@ -23988,7 +23920,7 @@
       </c>
       <c r="B1218" s="19" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horizon Europe. Clúster digital, industrial y espacial. Apoyos a proyectos para tecnologías de inteligencia artificial, internet, mundos virtuales, robótica, cuántica, fotónica, materias primas, bajo </t>
+          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
         </is>
       </c>
       <c r="C1218" s="20" t="n"/>
@@ -24004,7 +23936,7 @@
       </c>
       <c r="B1219" s="19" t="inlineStr">
         <is>
-          <t>EUS-65368</t>
+          <t>EUS-61284</t>
         </is>
       </c>
       <c r="C1219" s="20" t="n"/>
@@ -24156,7 +24088,7 @@
       </c>
       <c r="B1229" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/250119horizondiginduspaceklust/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/horizonkluster5hirimisioa/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1229" s="20" t="n"/>
@@ -24167,7 +24099,7 @@
     <row r="1231" ht="30" customHeight="1">
       <c r="A1231" s="16" t="inlineStr">
         <is>
-          <t>FICHA 83: EUS-46726</t>
+          <t>FICHA 83: EUS-82808</t>
         </is>
       </c>
       <c r="B1231" s="17" t="n"/>
@@ -24200,7 +24132,7 @@
       </c>
       <c r="B1233" s="19" t="inlineStr">
         <is>
-          <t>Horizon Europe: ayudas de la línea de energía del clúster 5 y de la Misión Ciudades. Jornada informativa sobre estas y otras iniciativas en colaboración transestatal para la doble transición ecológica</t>
+          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
         </is>
       </c>
       <c r="C1233" s="20" t="n"/>
@@ -24216,7 +24148,7 @@
       </c>
       <c r="B1234" s="19" t="inlineStr">
         <is>
-          <t>EUS-46726</t>
+          <t>EUS-82808</t>
         </is>
       </c>
       <c r="C1234" s="20" t="n"/>
@@ -24368,7 +24300,7 @@
       </c>
       <c r="B1244" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/horizonkluster5hirimisioa/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/azpitek-2026-programa-de-ayudas/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1244" s="20" t="n"/>
@@ -24379,7 +24311,7 @@
     <row r="1246" ht="30" customHeight="1">
       <c r="A1246" s="16" t="inlineStr">
         <is>
-          <t>FICHA 84: EUS-94309</t>
+          <t>FICHA 84: EUS-36705</t>
         </is>
       </c>
       <c r="B1246" s="17" t="n"/>
@@ -24404,7 +24336,7 @@
       <c r="E1247" s="20" t="n"/>
       <c r="F1247" s="20" t="n"/>
     </row>
-    <row r="1248" ht="45" customHeight="1">
+    <row r="1248" ht="20" customHeight="1">
       <c r="A1248" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -24412,7 +24344,7 @@
       </c>
       <c r="B1248" s="19" t="inlineStr">
         <is>
-          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instalación, Renovación y Actualización de Infraestructuras de Investigación</t>
+          <t>Subvenciones para innovación en economía circular 2026</t>
         </is>
       </c>
       <c r="C1248" s="20" t="n"/>
@@ -24428,7 +24360,7 @@
       </c>
       <c r="B1249" s="19" t="inlineStr">
         <is>
-          <t>EUS-94309</t>
+          <t>EUS-36705</t>
         </is>
       </c>
       <c r="C1249" s="20" t="n"/>
@@ -24580,7 +24512,7 @@
       </c>
       <c r="B1259" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/azpitek-2026-programa-de-ayudas/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/subvenciones-para-innovacion-en-economia-circular-2026/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1259" s="20" t="n"/>
@@ -24591,7 +24523,7 @@
     <row r="1261" ht="30" customHeight="1">
       <c r="A1261" s="16" t="inlineStr">
         <is>
-          <t>FICHA 85: EUS-92798</t>
+          <t>FICHA 85: EUS-15893</t>
         </is>
       </c>
       <c r="B1261" s="17" t="n"/>
@@ -24616,7 +24548,7 @@
       <c r="E1262" s="20" t="n"/>
       <c r="F1262" s="20" t="n"/>
     </row>
-    <row r="1263" ht="20" customHeight="1">
+    <row r="1263" ht="45" customHeight="1">
       <c r="A1263" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -24624,7 +24556,7 @@
       </c>
       <c r="B1263" s="19" t="inlineStr">
         <is>
-          <t>Subvenciones para innovación en economía circular 2026</t>
+          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
         </is>
       </c>
       <c r="C1263" s="20" t="n"/>
@@ -24640,7 +24572,7 @@
       </c>
       <c r="B1264" s="19" t="inlineStr">
         <is>
-          <t>EUS-92798</t>
+          <t>EUS-15893</t>
         </is>
       </c>
       <c r="C1264" s="20" t="n"/>
@@ -24792,7 +24724,7 @@
       </c>
       <c r="B1274" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/subvenciones-para-innovacion-en-economia-circular-2026/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/251222horizon2627sprieeni/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1274" s="20" t="n"/>
@@ -24803,7 +24735,7 @@
     <row r="1276" ht="30" customHeight="1">
       <c r="A1276" s="16" t="inlineStr">
         <is>
-          <t>FICHA 86: EUS-33647</t>
+          <t>FICHA 86: EUS-56381</t>
         </is>
       </c>
       <c r="B1276" s="17" t="n"/>
@@ -24836,7 +24768,7 @@
       </c>
       <c r="B1278" s="19" t="inlineStr">
         <is>
-          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones ambientales de la UE, partenariados de economía circular, azul o bio, o a la división alimentaria EIT Food del Instituto Europeo de Tecnología,</t>
+          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
         </is>
       </c>
       <c r="C1278" s="20" t="n"/>
@@ -24852,7 +24784,7 @@
       </c>
       <c r="B1279" s="19" t="inlineStr">
         <is>
-          <t>EUS-33647</t>
+          <t>EUS-56381</t>
         </is>
       </c>
       <c r="C1279" s="20" t="n"/>
@@ -25004,7 +24936,7 @@
       </c>
       <c r="B1289" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/251222horizon2627sprieeni/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/demokraziaezkutua251218/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1289" s="20" t="n"/>
@@ -25015,7 +24947,7 @@
     <row r="1291" ht="30" customHeight="1">
       <c r="A1291" s="16" t="inlineStr">
         <is>
-          <t>FICHA 87: EUS-37213</t>
+          <t>FICHA 87: EUS-49807</t>
         </is>
       </c>
       <c r="B1291" s="17" t="n"/>
@@ -25048,7 +24980,7 @@
       </c>
       <c r="B1293" s="19" t="inlineStr">
         <is>
-          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfabetización mediática y fomento del diálogo y la comprensión en torno a la desinformación digital</t>
+          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
         </is>
       </c>
       <c r="C1293" s="20" t="n"/>
@@ -25064,7 +24996,7 @@
       </c>
       <c r="B1294" s="19" t="inlineStr">
         <is>
-          <t>EUS-37213</t>
+          <t>EUS-49807</t>
         </is>
       </c>
       <c r="C1294" s="20" t="n"/>
@@ -25216,7 +25148,7 @@
       </c>
       <c r="B1304" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/demokraziaezkutua251218/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/ksiberritzalieplus251218/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1304" s="20" t="n"/>
@@ -25227,7 +25159,7 @@
     <row r="1306" ht="30" customHeight="1">
       <c r="A1306" s="16" t="inlineStr">
         <is>
-          <t>FICHA 88: EUS-17024</t>
+          <t>FICHA 88: EUS-04869</t>
         </is>
       </c>
       <c r="B1306" s="17" t="n"/>
@@ -25252,7 +25184,7 @@
       <c r="E1307" s="20" t="n"/>
       <c r="F1307" s="20" t="n"/>
     </row>
-    <row r="1308" ht="45" customHeight="1">
+    <row r="1308" ht="20" customHeight="1">
       <c r="A1308" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -25260,7 +25192,7 @@
       </c>
       <c r="B1308" s="19" t="inlineStr">
         <is>
-          <t xml:space="preserve">KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Industrias Culturales y Creativas para proyectos innovadores en la triple transición tecnológico-digital, energético-climática y socio-sanitaria, </t>
+          <t>Limpieza pozo de bombeo de los garajes de errebal</t>
         </is>
       </c>
       <c r="C1308" s="20" t="n"/>
@@ -25276,7 +25208,7 @@
       </c>
       <c r="B1309" s="19" t="inlineStr">
         <is>
-          <t>EUS-17024</t>
+          <t>EUS-04869</t>
         </is>
       </c>
       <c r="C1309" s="20" t="n"/>
@@ -25352,7 +25284,7 @@
       </c>
       <c r="B1314" s="19" t="inlineStr">
         <is>
-          <t>Ayuda/Subvencion Euskadi</t>
+          <t>Licitacion Euskadi</t>
         </is>
       </c>
       <c r="C1314" s="20" t="n"/>
@@ -25428,7 +25360,7 @@
       </c>
       <c r="B1319" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/ksiberritzalieplus251218/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/limpieza-pozo-bombeo-garajes-errebal/expgeeibar20583/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1319" s="20" t="n"/>
@@ -25439,7 +25371,7 @@
     <row r="1321" ht="30" customHeight="1">
       <c r="A1321" s="16" t="inlineStr">
         <is>
-          <t>FICHA 89: EUS-94613</t>
+          <t>FICHA 89: EUS-58730</t>
         </is>
       </c>
       <c r="B1321" s="17" t="n"/>
@@ -25472,7 +25404,7 @@
       </c>
       <c r="B1323" s="19" t="inlineStr">
         <is>
-          <t>Limpieza pozo de bombeo de los garajes de errebal</t>
+          <t>Revisión y acondicionamiento de arqueta de pluviales en milaflores</t>
         </is>
       </c>
       <c r="C1323" s="20" t="n"/>
@@ -25488,7 +25420,7 @@
       </c>
       <c r="B1324" s="19" t="inlineStr">
         <is>
-          <t>EUS-94613</t>
+          <t>EUS-58730</t>
         </is>
       </c>
       <c r="C1324" s="20" t="n"/>
@@ -25640,7 +25572,7 @@
       </c>
       <c r="B1334" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/limpieza-pozo-bombeo-garajes-errebal/expgeeibar20583/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/revision-y-acondicionamiento-arqueta-pluviales-milaflores/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1334" s="20" t="n"/>
@@ -25651,7 +25583,7 @@
     <row r="1336" ht="30" customHeight="1">
       <c r="A1336" s="16" t="inlineStr">
         <is>
-          <t>FICHA 90: EUS-23341</t>
+          <t>FICHA 90: EUS-69687</t>
         </is>
       </c>
       <c r="B1336" s="17" t="n"/>
@@ -25676,7 +25608,7 @@
       <c r="E1337" s="20" t="n"/>
       <c r="F1337" s="20" t="n"/>
     </row>
-    <row r="1338" ht="20" customHeight="1">
+    <row r="1338" ht="45" customHeight="1">
       <c r="A1338" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -25684,7 +25616,7 @@
       </c>
       <c r="B1338" s="19" t="inlineStr">
         <is>
-          <t>Revisión y acondicionamiento de arqueta de pluviales en milaflores</t>
+          <t>servicio de consultoría/educación ambiental para la prestación de la asistencia técnica del pilotaje del programa Agenda 2030 Escolar de Astigarraga</t>
         </is>
       </c>
       <c r="C1338" s="20" t="n"/>
@@ -25700,7 +25632,7 @@
       </c>
       <c r="B1339" s="19" t="inlineStr">
         <is>
-          <t>EUS-23341</t>
+          <t>EUS-69687</t>
         </is>
       </c>
       <c r="C1339" s="20" t="n"/>
@@ -25852,7 +25784,7 @@
       </c>
       <c r="B1349" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/revision-y-acondicionamiento-arqueta-pluviales-milaflores/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-consultoria-educacion-ambiental-prestacion-asistencia-tecnica-del-pilotaje-del-programa-agenda-2030-escolar-astigarraga/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1349" s="20" t="n"/>
@@ -25863,7 +25795,7 @@
     <row r="1351" ht="30" customHeight="1">
       <c r="A1351" s="16" t="inlineStr">
         <is>
-          <t>FICHA 91: EUS-51873</t>
+          <t>FICHA 91: EUS-63751</t>
         </is>
       </c>
       <c r="B1351" s="17" t="n"/>
@@ -25896,7 +25828,7 @@
       </c>
       <c r="B1353" s="19" t="inlineStr">
         <is>
-          <t>servicio de consultoría/educación ambiental para la prestación de la asistencia técnica del pilotaje del programa Agenda 2030 Escolar de Astigarraga</t>
+          <t>Apagado puntual del alumbrado municipal, con motivo de la celebración del espectáculo de Inauguración de Navidad</t>
         </is>
       </c>
       <c r="C1353" s="20" t="n"/>
@@ -25912,7 +25844,7 @@
       </c>
       <c r="B1354" s="19" t="inlineStr">
         <is>
-          <t>EUS-51873</t>
+          <t>EUS-63751</t>
         </is>
       </c>
       <c r="C1354" s="20" t="n"/>
@@ -26064,7 +25996,7 @@
       </c>
       <c r="B1364" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-consultoria-educacion-ambiental-prestacion-asistencia-tecnica-del-pilotaje-del-programa-agenda-2030-escolar-astigarraga/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/apagado-puntual-del-alumbrado-municipal-motivo-celebracion-del-espectaculo-inauguracion-navidad/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1364" s="20" t="n"/>
@@ -26075,7 +26007,7 @@
     <row r="1366" ht="30" customHeight="1">
       <c r="A1366" s="16" t="inlineStr">
         <is>
-          <t>FICHA 92: EUS-28738</t>
+          <t>FICHA 92: EUS-50368</t>
         </is>
       </c>
       <c r="B1366" s="17" t="n"/>
@@ -26108,7 +26040,7 @@
       </c>
       <c r="B1368" s="19" t="inlineStr">
         <is>
-          <t>Apagado puntual del alumbrado municipal, con motivo de la celebración del espectáculo de Inauguración de Navidad</t>
+          <t>Realización de trabajos puntuales de reparación en la ventana de la 3ª planta, sustitución de manilla en la 1ª planta y ajuste de la puerta de entrada en el edificio PIA.</t>
         </is>
       </c>
       <c r="C1368" s="20" t="n"/>
@@ -26124,7 +26056,7 @@
       </c>
       <c r="B1369" s="19" t="inlineStr">
         <is>
-          <t>EUS-28738</t>
+          <t>EUS-50368</t>
         </is>
       </c>
       <c r="C1369" s="20" t="n"/>
@@ -26276,7 +26208,7 @@
       </c>
       <c r="B1379" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/apagado-puntual-del-alumbrado-municipal-motivo-celebracion-del-espectaculo-inauguracion-navidad/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/realizacion-trabajos-puntuales-reparacion-ventana-3-planta-sustitucion-manilla-1-planta-y-ajuste-puerta-entrada-edificio-pia/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1379" s="20" t="n"/>
@@ -26287,7 +26219,7 @@
     <row r="1381" ht="30" customHeight="1">
       <c r="A1381" s="16" t="inlineStr">
         <is>
-          <t>FICHA 93: EUS-81513</t>
+          <t>FICHA 93: EUS-66714</t>
         </is>
       </c>
       <c r="B1381" s="17" t="n"/>
@@ -26320,7 +26252,7 @@
       </c>
       <c r="B1383" s="19" t="inlineStr">
         <is>
-          <t>Realización de trabajos puntuales de reparación en la ventana de la 3ª planta, sustitución de manilla en la 1ª planta y ajuste de la puerta de entrada en el edificio PIA.</t>
+          <t>Servicio puntual para la configuración y adaptación del software para la recogida de solicitudes de participación en la OPE2022</t>
         </is>
       </c>
       <c r="C1383" s="20" t="n"/>
@@ -26336,7 +26268,7 @@
       </c>
       <c r="B1384" s="19" t="inlineStr">
         <is>
-          <t>EUS-81513</t>
+          <t>EUS-66714</t>
         </is>
       </c>
       <c r="C1384" s="20" t="n"/>
@@ -26488,7 +26420,7 @@
       </c>
       <c r="B1394" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/realizacion-trabajos-puntuales-reparacion-ventana-3-planta-sustitucion-manilla-1-planta-y-ajuste-puerta-entrada-edificio-pia/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-puntual-configuracion-y-adaptacion-del-software-recogida-solicitudes-participacion-ope2022/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1394" s="20" t="n"/>
@@ -26499,7 +26431,7 @@
     <row r="1396" ht="30" customHeight="1">
       <c r="A1396" s="16" t="inlineStr">
         <is>
-          <t>FICHA 94: EUS-64768</t>
+          <t>FICHA 94: EUS-57664</t>
         </is>
       </c>
       <c r="B1396" s="17" t="n"/>
@@ -26532,7 +26464,7 @@
       </c>
       <c r="B1398" s="19" t="inlineStr">
         <is>
-          <t>Servicio puntual para la configuración y adaptación del software para la recogida de solicitudes de participación en la OPE2022</t>
+          <t>Suministro de una Columna de Boca de Riego para habilitación de un punto de agua.</t>
         </is>
       </c>
       <c r="C1398" s="20" t="n"/>
@@ -26548,7 +26480,7 @@
       </c>
       <c r="B1399" s="19" t="inlineStr">
         <is>
-          <t>EUS-64768</t>
+          <t>EUS-57664</t>
         </is>
       </c>
       <c r="C1399" s="20" t="n"/>
@@ -26700,7 +26632,7 @@
       </c>
       <c r="B1409" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-puntual-configuracion-y-adaptacion-del-software-recogida-solicitudes-participacion-ope2022/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/suministro-columna-boca-riego-habilitacion-punto-agua/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1409" s="20" t="n"/>
@@ -26711,7 +26643,7 @@
     <row r="1411" ht="30" customHeight="1">
       <c r="A1411" s="16" t="inlineStr">
         <is>
-          <t>FICHA 95: EUS-29793</t>
+          <t>FICHA 95: EUS-90980</t>
         </is>
       </c>
       <c r="B1411" s="17" t="n"/>
@@ -26744,7 +26676,7 @@
       </c>
       <c r="B1413" s="19" t="inlineStr">
         <is>
-          <t>Suministro de una Columna de Boca de Riego para habilitación de un punto de agua.</t>
+          <t>Servicio puntual de transporte de diverso material corporativo voluminoso con motivo de la celebración del evento DonoSTEAM 2025</t>
         </is>
       </c>
       <c r="C1413" s="20" t="n"/>
@@ -26760,7 +26692,7 @@
       </c>
       <c r="B1414" s="19" t="inlineStr">
         <is>
-          <t>EUS-29793</t>
+          <t>EUS-90980</t>
         </is>
       </c>
       <c r="C1414" s="20" t="n"/>
@@ -26912,7 +26844,7 @@
       </c>
       <c r="B1424" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/suministro-columna-boca-riego-habilitacion-punto-agua/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-puntual-transporte-diverso-material-corporativo-voluminoso-motivo-celebracion-del-evento-donosteam-2025/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1424" s="20" t="n"/>
@@ -26923,7 +26855,7 @@
     <row r="1426" ht="30" customHeight="1">
       <c r="A1426" s="16" t="inlineStr">
         <is>
-          <t>FICHA 96: EUS-50290</t>
+          <t>FICHA 96: EUS-55479</t>
         </is>
       </c>
       <c r="B1426" s="17" t="n"/>
@@ -26956,7 +26888,7 @@
       </c>
       <c r="B1428" s="19" t="inlineStr">
         <is>
-          <t>Servicio puntual de transporte de diverso material corporativo voluminoso con motivo de la celebración del evento DonoSTEAM 2025</t>
+          <t>Suministro puntual de material de seguridad para el edificio PIA. Botas de agua modelo ISSA talla 42</t>
         </is>
       </c>
       <c r="C1428" s="20" t="n"/>
@@ -26972,7 +26904,7 @@
       </c>
       <c r="B1429" s="19" t="inlineStr">
         <is>
-          <t>EUS-50290</t>
+          <t>EUS-55479</t>
         </is>
       </c>
       <c r="C1429" s="20" t="n"/>
@@ -27124,7 +27056,7 @@
       </c>
       <c r="B1439" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-puntual-transporte-diverso-material-corporativo-voluminoso-motivo-celebracion-del-evento-donosteam-2025/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/suministro-puntual-material-seguridad-edificio-pia-botas-agua-modelo-issa-talla-42/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1439" s="20" t="n"/>
@@ -27135,7 +27067,7 @@
     <row r="1441" ht="30" customHeight="1">
       <c r="A1441" s="16" t="inlineStr">
         <is>
-          <t>FICHA 97: EUS-71511</t>
+          <t>FICHA 97: EUS-25621</t>
         </is>
       </c>
       <c r="B1441" s="17" t="n"/>
@@ -27168,7 +27100,7 @@
       </c>
       <c r="B1443" s="19" t="inlineStr">
         <is>
-          <t>Suministro puntual de material de seguridad para el edificio PIA. Botas de agua modelo ISSA talla 42</t>
+          <t xml:space="preserve">Contratación de los servicios de recogida de información mediante encuestas telefónicas para la realización del barómetro ciudadano sobre la percepción social de las políticas de Garantía de Ingresos </t>
         </is>
       </c>
       <c r="C1443" s="20" t="n"/>
@@ -27184,7 +27116,7 @@
       </c>
       <c r="B1444" s="19" t="inlineStr">
         <is>
-          <t>EUS-71511</t>
+          <t>EUS-25621</t>
         </is>
       </c>
       <c r="C1444" s="20" t="n"/>
@@ -27336,7 +27268,7 @@
       </c>
       <c r="B1454" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/suministro-puntual-material-seguridad-edificio-pia-botas-agua-modelo-issa-talla-42/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/contratacion-servicios-recogida-informacion-mediante-encuestas-telefonicas-realizacion-del-barometro-ciudadano-percepcion-social-politicas-garantia-ingresos-y-inclusion-cae/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1454" s="20" t="n"/>
@@ -27344,220 +27276,8 @@
       <c r="E1454" s="20" t="n"/>
       <c r="F1454" s="20" t="n"/>
     </row>
-    <row r="1456" ht="30" customHeight="1">
-      <c r="A1456" s="16" t="inlineStr">
-        <is>
-          <t>FICHA 98: EUS-47511</t>
-        </is>
-      </c>
-      <c r="B1456" s="17" t="n"/>
-      <c r="C1456" s="17" t="n"/>
-      <c r="D1456" s="17" t="n"/>
-      <c r="E1456" s="17" t="n"/>
-      <c r="F1456" s="17" t="n"/>
-    </row>
-    <row r="1457" ht="20" customHeight="1">
-      <c r="A1457" s="18" t="inlineStr">
-        <is>
-          <t>Fuente</t>
-        </is>
-      </c>
-      <c r="B1457" s="19" t="inlineStr">
-        <is>
-          <t>🟢 Euskadi</t>
-        </is>
-      </c>
-      <c r="C1457" s="20" t="n"/>
-      <c r="D1457" s="20" t="n"/>
-      <c r="E1457" s="20" t="n"/>
-      <c r="F1457" s="20" t="n"/>
-    </row>
-    <row r="1458" ht="45" customHeight="1">
-      <c r="A1458" s="18" t="inlineStr">
-        <is>
-          <t>Titulo</t>
-        </is>
-      </c>
-      <c r="B1458" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Contratación de los servicios de recogida de información mediante encuestas telefónicas para la realización del barómetro ciudadano sobre la percepción social de las políticas de Garantía de Ingresos </t>
-        </is>
-      </c>
-      <c r="C1458" s="20" t="n"/>
-      <c r="D1458" s="20" t="n"/>
-      <c r="E1458" s="20" t="n"/>
-      <c r="F1458" s="20" t="n"/>
-    </row>
-    <row r="1459" ht="20" customHeight="1">
-      <c r="A1459" s="18" t="inlineStr">
-        <is>
-          <t>ID</t>
-        </is>
-      </c>
-      <c r="B1459" s="19" t="inlineStr">
-        <is>
-          <t>EUS-47511</t>
-        </is>
-      </c>
-      <c r="C1459" s="20" t="n"/>
-      <c r="D1459" s="20" t="n"/>
-      <c r="E1459" s="20" t="n"/>
-      <c r="F1459" s="20" t="n"/>
-    </row>
-    <row r="1460" ht="20" customHeight="1">
-      <c r="A1460" s="18" t="inlineStr">
-        <is>
-          <t>Programa</t>
-        </is>
-      </c>
-      <c r="B1460" s="19" t="inlineStr">
-        <is>
-          <t>Euskadi</t>
-        </is>
-      </c>
-      <c r="C1460" s="20" t="n"/>
-      <c r="D1460" s="20" t="n"/>
-      <c r="E1460" s="20" t="n"/>
-      <c r="F1460" s="20" t="n"/>
-    </row>
-    <row r="1461" ht="20" customHeight="1">
-      <c r="A1461" s="18" t="inlineStr">
-        <is>
-          <t>Estado</t>
-        </is>
-      </c>
-      <c r="B1461" s="19" t="inlineStr">
-        <is>
-          <t>Open</t>
-        </is>
-      </c>
-      <c r="C1461" s="20" t="n"/>
-      <c r="D1461" s="20" t="n"/>
-      <c r="E1461" s="20" t="n"/>
-      <c r="F1461" s="20" t="n"/>
-    </row>
-    <row r="1462" ht="20" customHeight="1">
-      <c r="A1462" s="18" t="inlineStr">
-        <is>
-          <t>Deadline</t>
-        </is>
-      </c>
-      <c r="B1462" s="19" t="inlineStr"/>
-      <c r="C1462" s="20" t="n"/>
-      <c r="D1462" s="20" t="n"/>
-      <c r="E1462" s="20" t="n"/>
-      <c r="F1462" s="20" t="n"/>
-    </row>
-    <row r="1463" ht="20" customHeight="1">
-      <c r="A1463" s="18" t="inlineStr">
-        <is>
-          <t>Presupuesto (EUR)</t>
-        </is>
-      </c>
-      <c r="B1463" s="19" t="inlineStr">
-        <is>
-          <t>No disponible</t>
-        </is>
-      </c>
-      <c r="C1463" s="20" t="n"/>
-      <c r="D1463" s="20" t="n"/>
-      <c r="E1463" s="20" t="n"/>
-      <c r="F1463" s="20" t="n"/>
-    </row>
-    <row r="1464" ht="20" customHeight="1">
-      <c r="A1464" s="18" t="inlineStr">
-        <is>
-          <t>Tipo de Accion</t>
-        </is>
-      </c>
-      <c r="B1464" s="19" t="inlineStr">
-        <is>
-          <t>Licitacion Euskadi</t>
-        </is>
-      </c>
-      <c r="C1464" s="20" t="n"/>
-      <c r="D1464" s="20" t="n"/>
-      <c r="E1464" s="20" t="n"/>
-      <c r="F1464" s="20" t="n"/>
-    </row>
-    <row r="1465" ht="20" customHeight="1">
-      <c r="A1465" s="18" t="inlineStr">
-        <is>
-          <t>Call ID</t>
-        </is>
-      </c>
-      <c r="B1465" s="19" t="inlineStr"/>
-      <c r="C1465" s="20" t="n"/>
-      <c r="D1465" s="20" t="n"/>
-      <c r="E1465" s="20" t="n"/>
-      <c r="F1465" s="20" t="n"/>
-    </row>
-    <row r="1466" ht="20" customHeight="1">
-      <c r="A1466" s="18" t="inlineStr">
-        <is>
-          <t>Descripcion</t>
-        </is>
-      </c>
-      <c r="B1466" s="19" t="inlineStr">
-        <is>
-          <t>Gobierno Vasco / Sector Publico Euskadi</t>
-        </is>
-      </c>
-      <c r="C1466" s="20" t="n"/>
-      <c r="D1466" s="20" t="n"/>
-      <c r="E1466" s="20" t="n"/>
-      <c r="F1466" s="20" t="n"/>
-    </row>
-    <row r="1467" ht="20" customHeight="1">
-      <c r="A1467" s="18" t="inlineStr">
-        <is>
-          <t>Tags</t>
-        </is>
-      </c>
-      <c r="B1467" s="19" t="inlineStr">
-        <is>
-          <t>energia</t>
-        </is>
-      </c>
-      <c r="C1467" s="20" t="n"/>
-      <c r="D1467" s="20" t="n"/>
-      <c r="E1467" s="20" t="n"/>
-      <c r="F1467" s="20" t="n"/>
-    </row>
-    <row r="1468" ht="20" customHeight="1">
-      <c r="A1468" s="18" t="inlineStr">
-        <is>
-          <t>Relevancia Bilbao</t>
-        </is>
-      </c>
-      <c r="B1468" s="19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MEDIA — </t>
-        </is>
-      </c>
-      <c r="C1468" s="20" t="n"/>
-      <c r="D1468" s="20" t="n"/>
-      <c r="E1468" s="20" t="n"/>
-      <c r="F1468" s="20" t="n"/>
-    </row>
-    <row r="1469" ht="45" customHeight="1">
-      <c r="A1469" s="18" t="inlineStr">
-        <is>
-          <t>Enlace al portal</t>
-        </is>
-      </c>
-      <c r="B1469" s="22" t="inlineStr">
-        <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/contratacion-servicios-recogida-informacion-mediante-encuestas-telefonicas-realizacion-del-barometro-ciudadano-percepcion-social-politicas-garantia-ingresos-y-inclusion-cae/web01-tramite/es/</t>
-        </is>
-      </c>
-      <c r="C1469" s="20" t="n"/>
-      <c r="D1469" s="20" t="n"/>
-      <c r="E1469" s="20" t="n"/>
-      <c r="F1469" s="20" t="n"/>
-    </row>
   </sheetData>
-  <mergeCells count="1372">
+  <mergeCells count="1358">
     <mergeCell ref="B679:F679"/>
     <mergeCell ref="B1010:F1010"/>
     <mergeCell ref="B276:F276"/>
@@ -27815,13 +27535,11 @@
     <mergeCell ref="B1163:F1163"/>
     <mergeCell ref="B408:F408"/>
     <mergeCell ref="A916:F916"/>
-    <mergeCell ref="B1461:F1461"/>
     <mergeCell ref="B619:F619"/>
     <mergeCell ref="B279:F279"/>
     <mergeCell ref="B410:F410"/>
     <mergeCell ref="B733:F733"/>
     <mergeCell ref="B708:F708"/>
-    <mergeCell ref="B1463:F1463"/>
     <mergeCell ref="B1031:F1031"/>
     <mergeCell ref="B281:F281"/>
     <mergeCell ref="B1033:F1033"/>
@@ -27871,14 +27589,11 @@
     <mergeCell ref="B379:F379"/>
     <mergeCell ref="B702:F702"/>
     <mergeCell ref="B677:F677"/>
-    <mergeCell ref="B1465:F1465"/>
-    <mergeCell ref="B1459:F1459"/>
     <mergeCell ref="B704:F704"/>
     <mergeCell ref="B1002:F1002"/>
     <mergeCell ref="B399:F399"/>
     <mergeCell ref="B1004:F1004"/>
     <mergeCell ref="B1302:F1302"/>
-    <mergeCell ref="B1460:F1460"/>
     <mergeCell ref="A946:F946"/>
     <mergeCell ref="A631:F631"/>
     <mergeCell ref="B117:F117"/>
@@ -28107,7 +27822,6 @@
     <mergeCell ref="B260:F260"/>
     <mergeCell ref="A496:F496"/>
     <mergeCell ref="B1346:F1346"/>
-    <mergeCell ref="B1458:F1458"/>
     <mergeCell ref="A796:F796"/>
     <mergeCell ref="B309:F309"/>
     <mergeCell ref="A316:F316"/>
@@ -28179,7 +27893,6 @@
     <mergeCell ref="B396:F396"/>
     <mergeCell ref="B267:F267"/>
     <mergeCell ref="B1159:F1159"/>
-    <mergeCell ref="B1457:F1457"/>
     <mergeCell ref="B398:F398"/>
     <mergeCell ref="B1451:F1451"/>
     <mergeCell ref="B696:F696"/>
@@ -28364,7 +28077,6 @@
     <mergeCell ref="B1354:F1354"/>
     <mergeCell ref="B284:F284"/>
     <mergeCell ref="B415:F415"/>
-    <mergeCell ref="B1468:F1468"/>
     <mergeCell ref="B713:F713"/>
     <mergeCell ref="B1011:F1011"/>
     <mergeCell ref="B110:F110"/>
@@ -28415,11 +28127,9 @@
     <mergeCell ref="B378:F378"/>
     <mergeCell ref="A1321:F1321"/>
     <mergeCell ref="B386:F386"/>
-    <mergeCell ref="B1464:F1464"/>
     <mergeCell ref="B1439:F1439"/>
     <mergeCell ref="B740:F740"/>
     <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B1467:F1467"/>
     <mergeCell ref="B437:F437"/>
     <mergeCell ref="B852:F852"/>
     <mergeCell ref="B10:F10"/>
@@ -28699,7 +28409,6 @@
     <mergeCell ref="B1160:F1160"/>
     <mergeCell ref="B1377:F1377"/>
     <mergeCell ref="B1168:F1168"/>
-    <mergeCell ref="B1466:F1466"/>
     <mergeCell ref="B407:F407"/>
     <mergeCell ref="A646:F646"/>
     <mergeCell ref="B1379:F1379"/>
@@ -28749,7 +28458,6 @@
     <mergeCell ref="B1158:F1158"/>
     <mergeCell ref="B403:F403"/>
     <mergeCell ref="B745:F745"/>
-    <mergeCell ref="B1462:F1462"/>
     <mergeCell ref="B1166:F1166"/>
     <mergeCell ref="B1278:F1278"/>
     <mergeCell ref="B7:F7"/>
@@ -28803,7 +28511,6 @@
     <mergeCell ref="B1274:F1274"/>
     <mergeCell ref="B215:F215"/>
     <mergeCell ref="B513:F513"/>
-    <mergeCell ref="A1456:F1456"/>
     <mergeCell ref="B847:F847"/>
     <mergeCell ref="B244:F244"/>
     <mergeCell ref="B819:F819"/>
@@ -28882,7 +28589,6 @@
     <mergeCell ref="B867:F867"/>
     <mergeCell ref="B1296:F1296"/>
     <mergeCell ref="A1351:F1351"/>
-    <mergeCell ref="B1469:F1469"/>
     <mergeCell ref="B251:F251"/>
     <mergeCell ref="B1014:F1014"/>
     <mergeCell ref="B1008:F1008"/>
@@ -29029,7 +28735,6 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1424" r:id="rId95"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1439" r:id="rId96"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1454" r:id="rId97"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1469" r:id="rId98"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -29041,7 +28746,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J99"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -29393,7 +29098,7 @@
     <row r="9" ht="28" customHeight="1">
       <c r="A9" s="6" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-MSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-SSP</t>
         </is>
       </c>
       <c r="B9" s="6" t="inlineStr">
@@ -29433,7 +29138,7 @@
     <row r="10" ht="28" customHeight="1">
       <c r="A10" s="6" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-SSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-LSP</t>
         </is>
       </c>
       <c r="B10" s="6" t="inlineStr">
@@ -29473,7 +29178,7 @@
     <row r="11" ht="28" customHeight="1">
       <c r="A11" s="6" t="inlineStr">
         <is>
-          <t>INNOVFUND-2025-NZT-GENERAL-LSP</t>
+          <t>INNOVFUND-2025-NZT-GENERAL-MSP</t>
         </is>
       </c>
       <c r="B11" s="6" t="inlineStr">
@@ -31569,7 +31274,7 @@
     <row r="66" ht="28" customHeight="1">
       <c r="A66" s="6" t="inlineStr">
         <is>
-          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="B66" s="6" t="inlineStr">
@@ -31601,7 +31306,7 @@
     <row r="67" ht="28" customHeight="1">
       <c r="A67" s="6" t="inlineStr">
         <is>
-          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="B67" s="6" t="inlineStr">
@@ -31665,7 +31370,7 @@
     <row r="69" ht="28" customHeight="1">
       <c r="A69" s="6" t="inlineStr">
         <is>
-          <t>EUS-99821</t>
+          <t>EUS-98933</t>
         </is>
       </c>
       <c r="B69" s="6" t="inlineStr">
@@ -31701,7 +31406,7 @@
     <row r="70" ht="28" customHeight="1">
       <c r="A70" s="6" t="inlineStr">
         <is>
-          <t>EUS-63525</t>
+          <t>EUS-82759</t>
         </is>
       </c>
       <c r="B70" s="6" t="inlineStr">
@@ -31737,7 +31442,7 @@
     <row r="71" ht="28" customHeight="1">
       <c r="A71" s="6" t="inlineStr">
         <is>
-          <t>EUS-89917</t>
+          <t>EUS-20999</t>
         </is>
       </c>
       <c r="B71" s="6" t="inlineStr">
@@ -31773,7 +31478,7 @@
     <row r="72" ht="28" customHeight="1">
       <c r="A72" s="6" t="inlineStr">
         <is>
-          <t>EUS-14531</t>
+          <t>EUS-06061</t>
         </is>
       </c>
       <c r="B72" s="6" t="inlineStr">
@@ -31809,7 +31514,7 @@
     <row r="73" ht="28" customHeight="1">
       <c r="A73" s="6" t="inlineStr">
         <is>
-          <t>EUS-08350</t>
+          <t>EUS-31808</t>
         </is>
       </c>
       <c r="B73" s="6" t="inlineStr">
@@ -31845,7 +31550,7 @@
     <row r="74" ht="28" customHeight="1">
       <c r="A74" s="6" t="inlineStr">
         <is>
-          <t>EUS-94562</t>
+          <t>EUS-28729</t>
         </is>
       </c>
       <c r="B74" s="6" t="inlineStr">
@@ -31881,7 +31586,7 @@
     <row r="75" ht="28" customHeight="1">
       <c r="A75" s="6" t="inlineStr">
         <is>
-          <t>EUS-56734</t>
+          <t>EUS-90487</t>
         </is>
       </c>
       <c r="B75" s="6" t="inlineStr">
@@ -31917,12 +31622,12 @@
     <row r="76" ht="28" customHeight="1">
       <c r="A76" s="6" t="inlineStr">
         <is>
-          <t>EUS-74809</t>
+          <t>EUS-69558</t>
         </is>
       </c>
       <c r="B76" s="6" t="inlineStr">
         <is>
-          <t>Servicios de Asistencia Técnica para la caracterización de l</t>
+          <t>FEADER, Fondo Europeo Agrícola de Desarrollo Rural, cofinanc</t>
         </is>
       </c>
       <c r="C76" s="6" t="inlineStr">
@@ -31938,7 +31643,7 @@
       <c r="E76" s="6" t="inlineStr"/>
       <c r="F76" s="25" t="inlineStr">
         <is>
-          <t>ALTA</t>
+          <t>MEDIA</t>
         </is>
       </c>
       <c r="G76" s="6" t="inlineStr"/>
@@ -31953,12 +31658,12 @@
     <row r="77" ht="28" customHeight="1">
       <c r="A77" s="6" t="inlineStr">
         <is>
-          <t>EUS-36721</t>
+          <t>EUS-43782</t>
         </is>
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>FEADER, Fondo Europeo Agrícola de Desarrollo Rural, cofinanc</t>
+          <t>Digital Europe, Horizon (programas de la UE). Apoyos para co</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
@@ -31989,12 +31694,12 @@
     <row r="78" ht="28" customHeight="1">
       <c r="A78" s="6" t="inlineStr">
         <is>
-          <t>EUS-88645</t>
+          <t>EUS-07831</t>
         </is>
       </c>
       <c r="B78" s="6" t="inlineStr">
         <is>
-          <t>Digital Europe, Horizon (programas de la UE). Apoyos para co</t>
+          <t>Salud, cáncer. Programas de Horizon, EIC, IHI. Apoyos para c</t>
         </is>
       </c>
       <c r="C78" s="6" t="inlineStr">
@@ -32025,12 +31730,12 @@
     <row r="79" ht="28" customHeight="1">
       <c r="A79" s="6" t="inlineStr">
         <is>
-          <t>EUS-55804</t>
+          <t>EUS-30486</t>
         </is>
       </c>
       <c r="B79" s="6" t="inlineStr">
         <is>
-          <t>Salud, cáncer. Programas de Horizon, EIC, IHI. Apoyos para c</t>
+          <t>Política Agraria Común de la UE de 2026, y sus ayudas abiert</t>
         </is>
       </c>
       <c r="C79" s="6" t="inlineStr">
@@ -32061,12 +31766,12 @@
     <row r="80" ht="28" customHeight="1">
       <c r="A80" s="6" t="inlineStr">
         <is>
-          <t>EUS-49713</t>
+          <t>EUS-52331</t>
         </is>
       </c>
       <c r="B80" s="6" t="inlineStr">
         <is>
-          <t>Política Agraria Común de la UE de 2026, y sus ayudas abiert</t>
+          <t>Programa de impulso a las ciudades y territorios inteligente</t>
         </is>
       </c>
       <c r="C80" s="6" t="inlineStr">
@@ -32097,12 +31802,12 @@
     <row r="81" ht="28" customHeight="1">
       <c r="A81" s="6" t="inlineStr">
         <is>
-          <t>EUS-29678</t>
+          <t>EUS-70955</t>
         </is>
       </c>
       <c r="B81" s="6" t="inlineStr">
         <is>
-          <t>Programa de impulso a las ciudades y territorios inteligente</t>
+          <t>Formación digital para empleabilidad turística: los fondos N</t>
         </is>
       </c>
       <c r="C81" s="6" t="inlineStr">
@@ -32133,12 +31838,12 @@
     <row r="82" ht="28" customHeight="1">
       <c r="A82" s="6" t="inlineStr">
         <is>
-          <t>EUS-12762</t>
+          <t>EUS-28448</t>
         </is>
       </c>
       <c r="B82" s="6" t="inlineStr">
         <is>
-          <t>Formación digital para empleabilidad turística: los fondos N</t>
+          <t>Horizon Europe. Clúster digital, industrial y espacial. Apoy</t>
         </is>
       </c>
       <c r="C82" s="6" t="inlineStr">
@@ -32169,12 +31874,12 @@
     <row r="83" ht="28" customHeight="1">
       <c r="A83" s="6" t="inlineStr">
         <is>
-          <t>EUS-65368</t>
+          <t>EUS-61284</t>
         </is>
       </c>
       <c r="B83" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe. Clúster digital, industrial y espacial. Apoy</t>
+          <t xml:space="preserve">Horizon Europe: ayudas de la línea de energía del clúster 5 </t>
         </is>
       </c>
       <c r="C83" s="6" t="inlineStr">
@@ -32205,12 +31910,12 @@
     <row r="84" ht="28" customHeight="1">
       <c r="A84" s="6" t="inlineStr">
         <is>
-          <t>EUS-46726</t>
+          <t>EUS-82808</t>
         </is>
       </c>
       <c r="B84" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Horizon Europe: ayudas de la línea de energía del clúster 5 </t>
+          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instal</t>
         </is>
       </c>
       <c r="C84" s="6" t="inlineStr">
@@ -32241,12 +31946,12 @@
     <row r="85" ht="28" customHeight="1">
       <c r="A85" s="6" t="inlineStr">
         <is>
-          <t>EUS-94309</t>
+          <t>EUS-36705</t>
         </is>
       </c>
       <c r="B85" s="6" t="inlineStr">
         <is>
-          <t>Azpitek 2026: Programa de Ayudas para la Adquisición, Instal</t>
+          <t>Subvenciones para innovación en economía circular 2026</t>
         </is>
       </c>
       <c r="C85" s="6" t="inlineStr">
@@ -32277,12 +31982,12 @@
     <row r="86" ht="28" customHeight="1">
       <c r="A86" s="6" t="inlineStr">
         <is>
-          <t>EUS-92798</t>
+          <t>EUS-15893</t>
         </is>
       </c>
       <c r="B86" s="6" t="inlineStr">
         <is>
-          <t>Subvenciones para innovación en economía circular 2026</t>
+          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones amb</t>
         </is>
       </c>
       <c r="C86" s="6" t="inlineStr">
@@ -32313,12 +32018,12 @@
     <row r="87" ht="28" customHeight="1">
       <c r="A87" s="6" t="inlineStr">
         <is>
-          <t>EUS-33647</t>
+          <t>EUS-56381</t>
         </is>
       </c>
       <c r="B87" s="6" t="inlineStr">
         <is>
-          <t>Horizon Europe 2026-27: convocatorias ligadas a misiones amb</t>
+          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfab</t>
         </is>
       </c>
       <c r="C87" s="6" t="inlineStr">
@@ -32349,12 +32054,12 @@
     <row r="88" ht="28" customHeight="1">
       <c r="A88" s="6" t="inlineStr">
         <is>
-          <t>EUS-37213</t>
+          <t>EUS-49807</t>
         </is>
       </c>
       <c r="B88" s="6" t="inlineStr">
         <is>
-          <t>Escudo Europeo de la Democracia: ayudas a proyectos de alfab</t>
+          <t>KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Indust</t>
         </is>
       </c>
       <c r="C88" s="6" t="inlineStr">
@@ -32385,12 +32090,12 @@
     <row r="89" ht="28" customHeight="1">
       <c r="A89" s="6" t="inlineStr">
         <is>
-          <t>EUS-17024</t>
+          <t>EUS-04869</t>
         </is>
       </c>
       <c r="B89" s="6" t="inlineStr">
         <is>
-          <t>KSI Berritzaile Plus: ayudas del Gobierno Vasco a las Indust</t>
+          <t>Limpieza pozo de bombeo de los garajes de errebal</t>
         </is>
       </c>
       <c r="C89" s="6" t="inlineStr">
@@ -32421,12 +32126,12 @@
     <row r="90" ht="28" customHeight="1">
       <c r="A90" s="6" t="inlineStr">
         <is>
-          <t>EUS-94613</t>
+          <t>EUS-58730</t>
         </is>
       </c>
       <c r="B90" s="6" t="inlineStr">
         <is>
-          <t>Limpieza pozo de bombeo de los garajes de errebal</t>
+          <t>Revisión y acondicionamiento de arqueta de pluviales en mila</t>
         </is>
       </c>
       <c r="C90" s="6" t="inlineStr">
@@ -32457,12 +32162,12 @@
     <row r="91" ht="28" customHeight="1">
       <c r="A91" s="6" t="inlineStr">
         <is>
-          <t>EUS-23341</t>
+          <t>EUS-69687</t>
         </is>
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>Revisión y acondicionamiento de arqueta de pluviales en mila</t>
+          <t>servicio de consultoría/educación ambiental para la prestaci</t>
         </is>
       </c>
       <c r="C91" s="6" t="inlineStr">
@@ -32493,12 +32198,12 @@
     <row r="92" ht="28" customHeight="1">
       <c r="A92" s="6" t="inlineStr">
         <is>
-          <t>EUS-51873</t>
+          <t>EUS-63751</t>
         </is>
       </c>
       <c r="B92" s="6" t="inlineStr">
         <is>
-          <t>servicio de consultoría/educación ambiental para la prestaci</t>
+          <t>Apagado puntual del alumbrado municipal, con motivo de la ce</t>
         </is>
       </c>
       <c r="C92" s="6" t="inlineStr">
@@ -32529,12 +32234,12 @@
     <row r="93" ht="28" customHeight="1">
       <c r="A93" s="6" t="inlineStr">
         <is>
-          <t>EUS-28738</t>
+          <t>EUS-50368</t>
         </is>
       </c>
       <c r="B93" s="6" t="inlineStr">
         <is>
-          <t>Apagado puntual del alumbrado municipal, con motivo de la ce</t>
+          <t>Realización de trabajos puntuales de reparación en la ventan</t>
         </is>
       </c>
       <c r="C93" s="6" t="inlineStr">
@@ -32565,12 +32270,12 @@
     <row r="94" ht="28" customHeight="1">
       <c r="A94" s="6" t="inlineStr">
         <is>
-          <t>EUS-81513</t>
+          <t>EUS-66714</t>
         </is>
       </c>
       <c r="B94" s="6" t="inlineStr">
         <is>
-          <t>Realización de trabajos puntuales de reparación en la ventan</t>
+          <t>Servicio puntual para la configuración y adaptación del soft</t>
         </is>
       </c>
       <c r="C94" s="6" t="inlineStr">
@@ -32601,12 +32306,12 @@
     <row r="95" ht="28" customHeight="1">
       <c r="A95" s="6" t="inlineStr">
         <is>
-          <t>EUS-64768</t>
+          <t>EUS-57664</t>
         </is>
       </c>
       <c r="B95" s="6" t="inlineStr">
         <is>
-          <t>Servicio puntual para la configuración y adaptación del soft</t>
+          <t>Suministro de una Columna de Boca de Riego para habilitación</t>
         </is>
       </c>
       <c r="C95" s="6" t="inlineStr">
@@ -32637,12 +32342,12 @@
     <row r="96" ht="28" customHeight="1">
       <c r="A96" s="6" t="inlineStr">
         <is>
-          <t>EUS-29793</t>
+          <t>EUS-90980</t>
         </is>
       </c>
       <c r="B96" s="6" t="inlineStr">
         <is>
-          <t>Suministro de una Columna de Boca de Riego para habilitación</t>
+          <t>Servicio puntual de transporte de diverso material corporati</t>
         </is>
       </c>
       <c r="C96" s="6" t="inlineStr">
@@ -32673,12 +32378,12 @@
     <row r="97" ht="28" customHeight="1">
       <c r="A97" s="6" t="inlineStr">
         <is>
-          <t>EUS-50290</t>
+          <t>EUS-55479</t>
         </is>
       </c>
       <c r="B97" s="6" t="inlineStr">
         <is>
-          <t>Servicio puntual de transporte de diverso material corporati</t>
+          <t>Suministro puntual de material de seguridad para el edificio</t>
         </is>
       </c>
       <c r="C97" s="6" t="inlineStr">
@@ -32709,12 +32414,12 @@
     <row r="98" ht="28" customHeight="1">
       <c r="A98" s="6" t="inlineStr">
         <is>
-          <t>EUS-71511</t>
+          <t>EUS-25621</t>
         </is>
       </c>
       <c r="B98" s="6" t="inlineStr">
         <is>
-          <t>Suministro puntual de material de seguridad para el edificio</t>
+          <t>Contratación de los servicios de recogida de información med</t>
         </is>
       </c>
       <c r="C98" s="6" t="inlineStr">
@@ -32742,44 +32447,8 @@
       <c r="I98" s="6" t="inlineStr"/>
       <c r="J98" s="6" t="inlineStr"/>
     </row>
-    <row r="99" ht="28" customHeight="1">
-      <c r="A99" s="6" t="inlineStr">
-        <is>
-          <t>EUS-47511</t>
-        </is>
-      </c>
-      <c r="B99" s="6" t="inlineStr">
-        <is>
-          <t>Contratación de los servicios de recogida de información med</t>
-        </is>
-      </c>
-      <c r="C99" s="6" t="inlineStr">
-        <is>
-          <t>Euskadi</t>
-        </is>
-      </c>
-      <c r="D99" s="6" t="inlineStr">
-        <is>
-          <t>Open</t>
-        </is>
-      </c>
-      <c r="E99" s="6" t="inlineStr"/>
-      <c r="F99" s="25" t="inlineStr">
-        <is>
-          <t>MEDIA</t>
-        </is>
-      </c>
-      <c r="G99" s="6" t="inlineStr"/>
-      <c r="H99" s="6" t="inlineStr">
-        <is>
-          <t>Por revisar</t>
-        </is>
-      </c>
-      <c r="I99" s="6" t="inlineStr"/>
-      <c r="J99" s="6" t="inlineStr"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:J99"/>
+  <autoFilter ref="A1:J98"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update funding data 2026-02-25
</commit_message>
<xml_diff>
--- a/docs/resultados_convocatorias.xlsx
+++ b/docs/resultados_convocatorias.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Recursos" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen'!$A$4:$M$96</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Seguimiento'!$A$1:$J$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Resumen'!$A$4:$M$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Seguimiento'!$A$1:$J$92</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -657,7 +657,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
@@ -691,7 +691,7 @@
     <row r="2" ht="22" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Mision Climatica - Neutralidad 2030 - Actualizado: 24/02/2026 08:09 - 90 convocatorias - 23 nuevas</t>
+          <t>Mision Climatica - Neutralidad 2030 - Actualizado: 25/02/2026 08:10 - 91 convocatorias - 24 nuevas</t>
         </is>
       </c>
     </row>
@@ -4549,7 +4549,7 @@
       </c>
       <c r="B70" s="6" t="inlineStr">
         <is>
-          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="C70" s="6" t="inlineStr">
@@ -4596,7 +4596,7 @@
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
@@ -4697,12 +4697,12 @@
       </c>
       <c r="B74" s="6" t="inlineStr">
         <is>
-          <t>EUS-01513</t>
+          <t>EUS-37980</t>
         </is>
       </c>
       <c r="C74" s="6" t="inlineStr">
         <is>
-          <t>Mantenimiento de cubiertas en los centros de Bilbao Kirolak</t>
+          <t>Ayudas a proyectos al amparo de la estrategia de desarrollo local participativo (EDLP), aprobada al grupo de acción local del sector pesquero (GALP) para el desarrollo sostenible de las zonas de pesca</t>
         </is>
       </c>
       <c r="D74" s="6" t="inlineStr">
@@ -4719,12 +4719,12 @@
       <c r="G74" s="6" t="inlineStr"/>
       <c r="H74" s="6" t="inlineStr">
         <is>
-          <t>Licitacion Euskadi</t>
-        </is>
-      </c>
-      <c r="I74" s="12" t="inlineStr">
-        <is>
-          <t>MUY ALTA</t>
+          <t>Ayuda/Subvencion Euskadi</t>
+        </is>
+      </c>
+      <c r="I74" s="8" t="inlineStr">
+        <is>
+          <t>ALTA</t>
         </is>
       </c>
       <c r="J74" s="6" t="inlineStr"/>
@@ -4752,12 +4752,12 @@
       </c>
       <c r="B75" s="6" t="inlineStr">
         <is>
-          <t>EUS-46570</t>
+          <t>EUS-88998</t>
         </is>
       </c>
       <c r="C75" s="6" t="inlineStr">
         <is>
-          <t>Ayudas a proyectos al amparo de la estrategia de desarrollo local participativo (EDLP), aprobada al grupo de acción local del sector pesquero (GALP) para el desarrollo sostenible de las zonas de pesca</t>
+          <t>ReSourceEU y materias primas críticas: la UE sigue tramitando convocatorias para favorecer proyectos otorgándoles carácter estratégico, de la mano del Banco Europeo de Inversiones, de cara a ámbitos c</t>
         </is>
       </c>
       <c r="D75" s="6" t="inlineStr">
@@ -4807,12 +4807,12 @@
       </c>
       <c r="B76" s="6" t="inlineStr">
         <is>
-          <t>EUS-20748</t>
+          <t>EUS-22037</t>
         </is>
       </c>
       <c r="C76" s="6" t="inlineStr">
         <is>
-          <t>ReSourceEU y materias primas críticas: la UE sigue tramitando convocatorias para favorecer proyectos otorgándoles carácter estratégico, de la mano del Banco Europeo de Inversiones, de cara a ámbitos c</t>
+          <t>Ciudades sostenibles: los Premios Capital Verde Europea y Hoja Verde de 2028 abren su convocatoria hasta el 01.04.26 para ciudades de más de 100.000 y de más de 20.000 habitantes, climáticamente resil</t>
         </is>
       </c>
       <c r="D76" s="6" t="inlineStr">
@@ -4862,12 +4862,12 @@
       </c>
       <c r="B77" s="6" t="inlineStr">
         <is>
-          <t>EUS-33329</t>
+          <t>EUS-96198</t>
         </is>
       </c>
       <c r="C77" s="6" t="inlineStr">
         <is>
-          <t>Ciudades sostenibles: los Premios Capital Verde Europea y Hoja Verde de 2028 abren su convocatoria hasta el 01.04.26 para ciudades de más de 100.000 y de más de 20.000 habitantes, climáticamente resil</t>
+          <t>Presolicitud para programa de ayudas a empresas que realicen inversiones productivas que permitan diversificar líneas de negocio, productos, servicios y mercados, con un enfoque en el crecimiento sost</t>
         </is>
       </c>
       <c r="D77" s="6" t="inlineStr">
@@ -4917,12 +4917,12 @@
       </c>
       <c r="B78" s="6" t="inlineStr">
         <is>
-          <t>EUS-46971</t>
+          <t>EUS-18212</t>
         </is>
       </c>
       <c r="C78" s="6" t="inlineStr">
         <is>
-          <t>Presolicitud para programa de ayudas a empresas que realicen inversiones productivas que permitan diversificar líneas de negocio, productos, servicios y mercados, con un enfoque en el crecimiento sost</t>
+          <t>Servicio integral de gestión operativa de movilidad que de soporte al plan operativo de movilidad y transporte en las Finales de Rugby EPCR 2026</t>
         </is>
       </c>
       <c r="D78" s="6" t="inlineStr">
@@ -4939,7 +4939,7 @@
       <c r="G78" s="6" t="inlineStr"/>
       <c r="H78" s="6" t="inlineStr">
         <is>
-          <t>Ayuda/Subvencion Euskadi</t>
+          <t>Licitacion Euskadi</t>
         </is>
       </c>
       <c r="I78" s="8" t="inlineStr">
@@ -4972,7 +4972,7 @@
       </c>
       <c r="B79" s="6" t="inlineStr">
         <is>
-          <t>EUS-23727</t>
+          <t>EUS-35207</t>
         </is>
       </c>
       <c r="C79" s="6" t="inlineStr">
@@ -5027,7 +5027,7 @@
       </c>
       <c r="B80" s="6" t="inlineStr">
         <is>
-          <t>EUS-63736</t>
+          <t>EUS-04351</t>
         </is>
       </c>
       <c r="C80" s="6" t="inlineStr">
@@ -5082,7 +5082,7 @@
       </c>
       <c r="B81" s="6" t="inlineStr">
         <is>
-          <t>EUS-38314</t>
+          <t>EUS-41297</t>
         </is>
       </c>
       <c r="C81" s="6" t="inlineStr">
@@ -5137,7 +5137,7 @@
       </c>
       <c r="B82" s="6" t="inlineStr">
         <is>
-          <t>EUS-43135</t>
+          <t>EUS-78717</t>
         </is>
       </c>
       <c r="C82" s="6" t="inlineStr">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="B83" s="6" t="inlineStr">
         <is>
-          <t>EUS-00654</t>
+          <t>EUS-25588</t>
         </is>
       </c>
       <c r="C83" s="6" t="inlineStr">
@@ -5247,7 +5247,7 @@
       </c>
       <c r="B84" s="6" t="inlineStr">
         <is>
-          <t>EUS-24940</t>
+          <t>EUS-33200</t>
         </is>
       </c>
       <c r="C84" s="6" t="inlineStr">
@@ -5302,7 +5302,7 @@
       </c>
       <c r="B85" s="6" t="inlineStr">
         <is>
-          <t>EUS-30791</t>
+          <t>EUS-47048</t>
         </is>
       </c>
       <c r="C85" s="6" t="inlineStr">
@@ -5357,7 +5357,7 @@
       </c>
       <c r="B86" s="6" t="inlineStr">
         <is>
-          <t>EUS-01008</t>
+          <t>EUS-74734</t>
         </is>
       </c>
       <c r="C86" s="6" t="inlineStr">
@@ -5412,7 +5412,7 @@
       </c>
       <c r="B87" s="6" t="inlineStr">
         <is>
-          <t>EUS-10663</t>
+          <t>EUS-60281</t>
         </is>
       </c>
       <c r="C87" s="6" t="inlineStr">
@@ -5467,7 +5467,7 @@
       </c>
       <c r="B88" s="6" t="inlineStr">
         <is>
-          <t>EUS-56941</t>
+          <t>EUS-54283</t>
         </is>
       </c>
       <c r="C88" s="6" t="inlineStr">
@@ -5522,7 +5522,7 @@
       </c>
       <c r="B89" s="6" t="inlineStr">
         <is>
-          <t>EUS-01208</t>
+          <t>EUS-10026</t>
         </is>
       </c>
       <c r="C89" s="6" t="inlineStr">
@@ -5577,7 +5577,7 @@
       </c>
       <c r="B90" s="6" t="inlineStr">
         <is>
-          <t>EUS-00233</t>
+          <t>EUS-35931</t>
         </is>
       </c>
       <c r="C90" s="6" t="inlineStr">
@@ -5632,7 +5632,7 @@
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>EUS-15421</t>
+          <t>EUS-44255</t>
         </is>
       </c>
       <c r="C91" s="6" t="inlineStr">
@@ -5687,7 +5687,7 @@
       </c>
       <c r="B92" s="6" t="inlineStr">
         <is>
-          <t>EUS-74016</t>
+          <t>EUS-75900</t>
         </is>
       </c>
       <c r="C92" s="6" t="inlineStr">
@@ -5742,12 +5742,12 @@
       </c>
       <c r="B93" s="6" t="inlineStr">
         <is>
-          <t>EUS-57526</t>
+          <t>EUS-96234</t>
         </is>
       </c>
       <c r="C93" s="6" t="inlineStr">
         <is>
-          <t>ejecución de cuneta en acera de kosta kalea para canalizar las aguas, posterior colocación de baldosa negra</t>
+          <t>Reparación de fuga de agua en la acometida den centro escolar CEPA Donostia HHI (Julio Urquijo) de Donostia</t>
         </is>
       </c>
       <c r="D93" s="6" t="inlineStr">
@@ -5797,12 +5797,12 @@
       </c>
       <c r="B94" s="6" t="inlineStr">
         <is>
-          <t>EUS-99494</t>
+          <t>EUS-89077</t>
         </is>
       </c>
       <c r="C94" s="6" t="inlineStr">
         <is>
-          <t>evitar y redirigir las aguas, así como eliminar las eflorescencias en la acera de kandido saseta</t>
+          <t>Mantenimiento integral de las instalaciones de alumbrado público exterior, navideño, ornamental de ferias y fiestas y semáforos</t>
         </is>
       </c>
       <c r="D94" s="6" t="inlineStr">
@@ -5852,12 +5852,12 @@
       </c>
       <c r="B95" s="6" t="inlineStr">
         <is>
-          <t>EUS-68529</t>
+          <t>EUS-75154</t>
         </is>
       </c>
       <c r="C95" s="6" t="inlineStr">
         <is>
-          <t>proyecto de nuevo edificio de mercado municipal en la parcela de damarri</t>
+          <t>Auscultación geotécnica de la red de infraestructuras viarias de la Diputación Foral de Gipuzkoa (1-O-54/2025)</t>
         </is>
       </c>
       <c r="D95" s="6" t="inlineStr">
@@ -5907,12 +5907,12 @@
       </c>
       <c r="B96" s="6" t="inlineStr">
         <is>
-          <t>EUS-03547</t>
+          <t>EUS-74501</t>
         </is>
       </c>
       <c r="C96" s="6" t="inlineStr">
         <is>
-          <t>renovación de 2 calderas en los vestuarios de la playa</t>
+          <t>Servicio de limpieza viaria</t>
         </is>
       </c>
       <c r="D96" s="6" t="inlineStr">
@@ -5954,8 +5954,63 @@
         </is>
       </c>
     </row>
+    <row r="97" ht="40" customHeight="1">
+      <c r="A97" s="14" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="B97" s="6" t="inlineStr">
+        <is>
+          <t>EUS-26650</t>
+        </is>
+      </c>
+      <c r="C97" s="6" t="inlineStr">
+        <is>
+          <t>Ofrecer los servicios de gestión de reservas, utilización, mantenimiento, y  limpieza del albergue Santiagomendi, así como el servicio de organización de actividades naturales en el medio ambiente.</t>
+        </is>
+      </c>
+      <c r="D97" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="E97" s="7" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="F97" s="6" t="inlineStr"/>
+      <c r="G97" s="6" t="inlineStr"/>
+      <c r="H97" s="6" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="I97" s="10" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="J97" s="6" t="inlineStr"/>
+      <c r="K97" s="6" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="L97" s="15" t="inlineStr">
+        <is>
+          <t>NUEVA</t>
+        </is>
+      </c>
+      <c r="M97" s="9" t="inlineStr">
+        <is>
+          <t>Ver</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A4:M96"/>
+  <autoFilter ref="A4:M97"/>
   <mergeCells count="4">
     <mergeCell ref="A73:M73"/>
     <mergeCell ref="A2:M2"/>
@@ -6053,6 +6108,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M94" r:id="rId88"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M95" r:id="rId89"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M96" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="M97" r:id="rId91"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6064,7 +6120,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1349"/>
+  <dimension ref="A1:F1364"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -19903,7 +19959,7 @@
     <row r="961" ht="30" customHeight="1">
       <c r="A961" s="16" t="inlineStr">
         <is>
-          <t>FICHA 65: 4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>FICHA 65: dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="B961" s="17" t="n"/>
@@ -19952,7 +20008,7 @@
       </c>
       <c r="B964" s="19" t="inlineStr">
         <is>
-          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="C964" s="20" t="n"/>
@@ -20040,7 +20096,7 @@
       </c>
       <c r="B970" s="19" t="inlineStr">
         <is>
-          <t>EC-REGIO/2025/MVP/0036-EXA</t>
+          <t>EC-REGIO/2025/MVP/0023-EXA</t>
         </is>
       </c>
       <c r="C970" s="20" t="n"/>
@@ -20100,7 +20156,7 @@
       </c>
       <c r="B974" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="C974" s="20" t="n"/>
@@ -20111,7 +20167,7 @@
     <row r="976" ht="30" customHeight="1">
       <c r="A976" s="16" t="inlineStr">
         <is>
-          <t>FICHA 66: dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>FICHA 66: 4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="B976" s="17" t="n"/>
@@ -20160,7 +20216,7 @@
       </c>
       <c r="B979" s="19" t="inlineStr">
         <is>
-          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="C979" s="20" t="n"/>
@@ -20248,7 +20304,7 @@
       </c>
       <c r="B985" s="19" t="inlineStr">
         <is>
-          <t>EC-REGIO/2025/MVP/0023-EXA</t>
+          <t>EC-REGIO/2025/MVP/0036-EXA</t>
         </is>
       </c>
       <c r="C985" s="20" t="n"/>
@@ -20308,7 +20364,7 @@
       </c>
       <c r="B989" s="22" t="inlineStr">
         <is>
-          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>https://ec.europa.eu/info/funding-tenders/opportunities/portal/screen/opportunities/topic-details/4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="C989" s="20" t="n"/>
@@ -20527,7 +20583,7 @@
     <row r="1006" ht="30" customHeight="1">
       <c r="A1006" s="16" t="inlineStr">
         <is>
-          <t>FICHA 68: EUS-01513</t>
+          <t>FICHA 68: EUS-37980</t>
         </is>
       </c>
       <c r="B1006" s="17" t="n"/>
@@ -20552,7 +20608,7 @@
       <c r="E1007" s="20" t="n"/>
       <c r="F1007" s="20" t="n"/>
     </row>
-    <row r="1008" ht="20" customHeight="1">
+    <row r="1008" ht="45" customHeight="1">
       <c r="A1008" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -20560,7 +20616,7 @@
       </c>
       <c r="B1008" s="19" t="inlineStr">
         <is>
-          <t>Mantenimiento de cubiertas en los centros de Bilbao Kirolak</t>
+          <t>Ayudas a proyectos al amparo de la estrategia de desarrollo local participativo (EDLP), aprobada al grupo de acción local del sector pesquero (GALP) para el desarrollo sostenible de las zonas de pesca</t>
         </is>
       </c>
       <c r="C1008" s="20" t="n"/>
@@ -20576,7 +20632,7 @@
       </c>
       <c r="B1009" s="19" t="inlineStr">
         <is>
-          <t>EUS-01513</t>
+          <t>EUS-37980</t>
         </is>
       </c>
       <c r="C1009" s="20" t="n"/>
@@ -20652,7 +20708,7 @@
       </c>
       <c r="B1014" s="19" t="inlineStr">
         <is>
-          <t>Licitacion Euskadi</t>
+          <t>Ayuda/Subvencion Euskadi</t>
         </is>
       </c>
       <c r="C1014" s="20" t="n"/>
@@ -20710,9 +20766,9 @@
           <t>Relevancia Bilbao</t>
         </is>
       </c>
-      <c r="B1018" s="23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">MUY ALTA — </t>
+      <c r="B1018" s="21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ALTA — </t>
         </is>
       </c>
       <c r="C1018" s="20" t="n"/>
@@ -20728,7 +20784,7 @@
       </c>
       <c r="B1019" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/mantenimiento-cubiertas-centros-bilbao-kirolak/expjaso685080/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/ayudas-al-amparo-de-la-estrategia-de-desarrollo-local-participativo-2026/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1019" s="20" t="n"/>
@@ -20739,7 +20795,7 @@
     <row r="1021" ht="30" customHeight="1">
       <c r="A1021" s="16" t="inlineStr">
         <is>
-          <t>FICHA 69: EUS-46570</t>
+          <t>FICHA 69: EUS-88998</t>
         </is>
       </c>
       <c r="B1021" s="17" t="n"/>
@@ -20772,7 +20828,7 @@
       </c>
       <c r="B1023" s="19" t="inlineStr">
         <is>
-          <t>Ayudas a proyectos al amparo de la estrategia de desarrollo local participativo (EDLP), aprobada al grupo de acción local del sector pesquero (GALP) para el desarrollo sostenible de las zonas de pesca</t>
+          <t>ReSourceEU y materias primas críticas: la UE sigue tramitando convocatorias para favorecer proyectos otorgándoles carácter estratégico, de la mano del Banco Europeo de Inversiones, de cara a ámbitos c</t>
         </is>
       </c>
       <c r="C1023" s="20" t="n"/>
@@ -20788,7 +20844,7 @@
       </c>
       <c r="B1024" s="19" t="inlineStr">
         <is>
-          <t>EUS-46570</t>
+          <t>EUS-88998</t>
         </is>
       </c>
       <c r="C1024" s="20" t="n"/>
@@ -20940,7 +20996,7 @@
       </c>
       <c r="B1034" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/ayudas-al-amparo-de-la-estrategia-de-desarrollo-local-participativo-2026/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260119resourceeumateriaes/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1034" s="20" t="n"/>
@@ -20951,7 +21007,7 @@
     <row r="1036" ht="30" customHeight="1">
       <c r="A1036" s="16" t="inlineStr">
         <is>
-          <t>FICHA 70: EUS-20748</t>
+          <t>FICHA 70: EUS-22037</t>
         </is>
       </c>
       <c r="B1036" s="17" t="n"/>
@@ -20984,7 +21040,7 @@
       </c>
       <c r="B1038" s="19" t="inlineStr">
         <is>
-          <t>ReSourceEU y materias primas críticas: la UE sigue tramitando convocatorias para favorecer proyectos otorgándoles carácter estratégico, de la mano del Banco Europeo de Inversiones, de cara a ámbitos c</t>
+          <t>Ciudades sostenibles: los Premios Capital Verde Europea y Hoja Verde de 2028 abren su convocatoria hasta el 01.04.26 para ciudades de más de 100.000 y de más de 20.000 habitantes, climáticamente resil</t>
         </is>
       </c>
       <c r="C1038" s="20" t="n"/>
@@ -21000,7 +21056,7 @@
       </c>
       <c r="B1039" s="19" t="inlineStr">
         <is>
-          <t>EUS-20748</t>
+          <t>EUS-22037</t>
         </is>
       </c>
       <c r="C1039" s="20" t="n"/>
@@ -21152,7 +21208,7 @@
       </c>
       <c r="B1049" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/260119resourceeumateriaes/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2026/hiriburutahostoberdea2826/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1049" s="20" t="n"/>
@@ -21163,7 +21219,7 @@
     <row r="1051" ht="30" customHeight="1">
       <c r="A1051" s="16" t="inlineStr">
         <is>
-          <t>FICHA 71: EUS-33329</t>
+          <t>FICHA 71: EUS-96198</t>
         </is>
       </c>
       <c r="B1051" s="17" t="n"/>
@@ -21196,7 +21252,7 @@
       </c>
       <c r="B1053" s="19" t="inlineStr">
         <is>
-          <t>Ciudades sostenibles: los Premios Capital Verde Europea y Hoja Verde de 2028 abren su convocatoria hasta el 01.04.26 para ciudades de más de 100.000 y de más de 20.000 habitantes, climáticamente resil</t>
+          <t>Presolicitud para programa de ayudas a empresas que realicen inversiones productivas que permitan diversificar líneas de negocio, productos, servicios y mercados, con un enfoque en el crecimiento sost</t>
         </is>
       </c>
       <c r="C1053" s="20" t="n"/>
@@ -21212,7 +21268,7 @@
       </c>
       <c r="B1054" s="19" t="inlineStr">
         <is>
-          <t>EUS-33329</t>
+          <t>EUS-96198</t>
         </is>
       </c>
       <c r="C1054" s="20" t="n"/>
@@ -21364,7 +21420,7 @@
       </c>
       <c r="B1064" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2026/hiriburutahostoberdea2826/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/ayuda_subvencion/2025/presolicitud-dibertsifika-2026/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1064" s="20" t="n"/>
@@ -21375,7 +21431,7 @@
     <row r="1066" ht="30" customHeight="1">
       <c r="A1066" s="16" t="inlineStr">
         <is>
-          <t>FICHA 72: EUS-46971</t>
+          <t>FICHA 72: EUS-18212</t>
         </is>
       </c>
       <c r="B1066" s="17" t="n"/>
@@ -21408,7 +21464,7 @@
       </c>
       <c r="B1068" s="19" t="inlineStr">
         <is>
-          <t>Presolicitud para programa de ayudas a empresas que realicen inversiones productivas que permitan diversificar líneas de negocio, productos, servicios y mercados, con un enfoque en el crecimiento sost</t>
+          <t>Servicio integral de gestión operativa de movilidad que de soporte al plan operativo de movilidad y transporte en las Finales de Rugby EPCR 2026</t>
         </is>
       </c>
       <c r="C1068" s="20" t="n"/>
@@ -21424,7 +21480,7 @@
       </c>
       <c r="B1069" s="19" t="inlineStr">
         <is>
-          <t>EUS-46971</t>
+          <t>EUS-18212</t>
         </is>
       </c>
       <c r="C1069" s="20" t="n"/>
@@ -21500,7 +21556,7 @@
       </c>
       <c r="B1074" s="19" t="inlineStr">
         <is>
-          <t>Ayuda/Subvencion Euskadi</t>
+          <t>Licitacion Euskadi</t>
         </is>
       </c>
       <c r="C1074" s="20" t="n"/>
@@ -21576,7 +21632,7 @@
       </c>
       <c r="B1079" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/ayuda_subvencion/2025/presolicitud-dibertsifika-2026/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-integral-gestion-operativa-movilidad-que-soporte-al-plan-operativo-movilidad-y-transporte-finales-rugby-epcr-2026/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1079" s="20" t="n"/>
@@ -21587,7 +21643,7 @@
     <row r="1081" ht="30" customHeight="1">
       <c r="A1081" s="16" t="inlineStr">
         <is>
-          <t>FICHA 73: EUS-23727</t>
+          <t>FICHA 73: EUS-35207</t>
         </is>
       </c>
       <c r="B1081" s="17" t="n"/>
@@ -21636,7 +21692,7 @@
       </c>
       <c r="B1084" s="19" t="inlineStr">
         <is>
-          <t>EUS-23727</t>
+          <t>EUS-35207</t>
         </is>
       </c>
       <c r="C1084" s="20" t="n"/>
@@ -21799,7 +21855,7 @@
     <row r="1096" ht="30" customHeight="1">
       <c r="A1096" s="16" t="inlineStr">
         <is>
-          <t>FICHA 74: EUS-63736</t>
+          <t>FICHA 74: EUS-04351</t>
         </is>
       </c>
       <c r="B1096" s="17" t="n"/>
@@ -21848,7 +21904,7 @@
       </c>
       <c r="B1099" s="19" t="inlineStr">
         <is>
-          <t>EUS-63736</t>
+          <t>EUS-04351</t>
         </is>
       </c>
       <c r="C1099" s="20" t="n"/>
@@ -22011,7 +22067,7 @@
     <row r="1111" ht="30" customHeight="1">
       <c r="A1111" s="16" t="inlineStr">
         <is>
-          <t>FICHA 75: EUS-38314</t>
+          <t>FICHA 75: EUS-41297</t>
         </is>
       </c>
       <c r="B1111" s="17" t="n"/>
@@ -22060,7 +22116,7 @@
       </c>
       <c r="B1114" s="19" t="inlineStr">
         <is>
-          <t>EUS-38314</t>
+          <t>EUS-41297</t>
         </is>
       </c>
       <c r="C1114" s="20" t="n"/>
@@ -22223,7 +22279,7 @@
     <row r="1126" ht="30" customHeight="1">
       <c r="A1126" s="16" t="inlineStr">
         <is>
-          <t>FICHA 76: EUS-43135</t>
+          <t>FICHA 76: EUS-78717</t>
         </is>
       </c>
       <c r="B1126" s="17" t="n"/>
@@ -22272,7 +22328,7 @@
       </c>
       <c r="B1129" s="19" t="inlineStr">
         <is>
-          <t>EUS-43135</t>
+          <t>EUS-78717</t>
         </is>
       </c>
       <c r="C1129" s="20" t="n"/>
@@ -22435,7 +22491,7 @@
     <row r="1141" ht="30" customHeight="1">
       <c r="A1141" s="16" t="inlineStr">
         <is>
-          <t>FICHA 77: EUS-00654</t>
+          <t>FICHA 77: EUS-25588</t>
         </is>
       </c>
       <c r="B1141" s="17" t="n"/>
@@ -22484,7 +22540,7 @@
       </c>
       <c r="B1144" s="19" t="inlineStr">
         <is>
-          <t>EUS-00654</t>
+          <t>EUS-25588</t>
         </is>
       </c>
       <c r="C1144" s="20" t="n"/>
@@ -22647,7 +22703,7 @@
     <row r="1156" ht="30" customHeight="1">
       <c r="A1156" s="16" t="inlineStr">
         <is>
-          <t>FICHA 78: EUS-24940</t>
+          <t>FICHA 78: EUS-33200</t>
         </is>
       </c>
       <c r="B1156" s="17" t="n"/>
@@ -22696,7 +22752,7 @@
       </c>
       <c r="B1159" s="19" t="inlineStr">
         <is>
-          <t>EUS-24940</t>
+          <t>EUS-33200</t>
         </is>
       </c>
       <c r="C1159" s="20" t="n"/>
@@ -22859,7 +22915,7 @@
     <row r="1171" ht="30" customHeight="1">
       <c r="A1171" s="16" t="inlineStr">
         <is>
-          <t>FICHA 79: EUS-30791</t>
+          <t>FICHA 79: EUS-47048</t>
         </is>
       </c>
       <c r="B1171" s="17" t="n"/>
@@ -22908,7 +22964,7 @@
       </c>
       <c r="B1174" s="19" t="inlineStr">
         <is>
-          <t>EUS-30791</t>
+          <t>EUS-47048</t>
         </is>
       </c>
       <c r="C1174" s="20" t="n"/>
@@ -23071,7 +23127,7 @@
     <row r="1186" ht="30" customHeight="1">
       <c r="A1186" s="16" t="inlineStr">
         <is>
-          <t>FICHA 80: EUS-01008</t>
+          <t>FICHA 80: EUS-74734</t>
         </is>
       </c>
       <c r="B1186" s="17" t="n"/>
@@ -23120,7 +23176,7 @@
       </c>
       <c r="B1189" s="19" t="inlineStr">
         <is>
-          <t>EUS-01008</t>
+          <t>EUS-74734</t>
         </is>
       </c>
       <c r="C1189" s="20" t="n"/>
@@ -23283,7 +23339,7 @@
     <row r="1201" ht="30" customHeight="1">
       <c r="A1201" s="16" t="inlineStr">
         <is>
-          <t>FICHA 81: EUS-10663</t>
+          <t>FICHA 81: EUS-60281</t>
         </is>
       </c>
       <c r="B1201" s="17" t="n"/>
@@ -23332,7 +23388,7 @@
       </c>
       <c r="B1204" s="19" t="inlineStr">
         <is>
-          <t>EUS-10663</t>
+          <t>EUS-60281</t>
         </is>
       </c>
       <c r="C1204" s="20" t="n"/>
@@ -23495,7 +23551,7 @@
     <row r="1216" ht="30" customHeight="1">
       <c r="A1216" s="16" t="inlineStr">
         <is>
-          <t>FICHA 82: EUS-56941</t>
+          <t>FICHA 82: EUS-54283</t>
         </is>
       </c>
       <c r="B1216" s="17" t="n"/>
@@ -23544,7 +23600,7 @@
       </c>
       <c r="B1219" s="19" t="inlineStr">
         <is>
-          <t>EUS-56941</t>
+          <t>EUS-54283</t>
         </is>
       </c>
       <c r="C1219" s="20" t="n"/>
@@ -23707,7 +23763,7 @@
     <row r="1231" ht="30" customHeight="1">
       <c r="A1231" s="16" t="inlineStr">
         <is>
-          <t>FICHA 83: EUS-01208</t>
+          <t>FICHA 83: EUS-10026</t>
         </is>
       </c>
       <c r="B1231" s="17" t="n"/>
@@ -23756,7 +23812,7 @@
       </c>
       <c r="B1234" s="19" t="inlineStr">
         <is>
-          <t>EUS-01208</t>
+          <t>EUS-10026</t>
         </is>
       </c>
       <c r="C1234" s="20" t="n"/>
@@ -23919,7 +23975,7 @@
     <row r="1246" ht="30" customHeight="1">
       <c r="A1246" s="16" t="inlineStr">
         <is>
-          <t>FICHA 84: EUS-00233</t>
+          <t>FICHA 84: EUS-35931</t>
         </is>
       </c>
       <c r="B1246" s="17" t="n"/>
@@ -23968,7 +24024,7 @@
       </c>
       <c r="B1249" s="19" t="inlineStr">
         <is>
-          <t>EUS-00233</t>
+          <t>EUS-35931</t>
         </is>
       </c>
       <c r="C1249" s="20" t="n"/>
@@ -24131,7 +24187,7 @@
     <row r="1261" ht="30" customHeight="1">
       <c r="A1261" s="16" t="inlineStr">
         <is>
-          <t>FICHA 85: EUS-15421</t>
+          <t>FICHA 85: EUS-44255</t>
         </is>
       </c>
       <c r="B1261" s="17" t="n"/>
@@ -24180,7 +24236,7 @@
       </c>
       <c r="B1264" s="19" t="inlineStr">
         <is>
-          <t>EUS-15421</t>
+          <t>EUS-44255</t>
         </is>
       </c>
       <c r="C1264" s="20" t="n"/>
@@ -24343,7 +24399,7 @@
     <row r="1276" ht="30" customHeight="1">
       <c r="A1276" s="16" t="inlineStr">
         <is>
-          <t>FICHA 86: EUS-74016</t>
+          <t>FICHA 86: EUS-75900</t>
         </is>
       </c>
       <c r="B1276" s="17" t="n"/>
@@ -24392,7 +24448,7 @@
       </c>
       <c r="B1279" s="19" t="inlineStr">
         <is>
-          <t>EUS-74016</t>
+          <t>EUS-75900</t>
         </is>
       </c>
       <c r="C1279" s="20" t="n"/>
@@ -24555,7 +24611,7 @@
     <row r="1291" ht="30" customHeight="1">
       <c r="A1291" s="16" t="inlineStr">
         <is>
-          <t>FICHA 87: EUS-57526</t>
+          <t>FICHA 87: EUS-96234</t>
         </is>
       </c>
       <c r="B1291" s="17" t="n"/>
@@ -24588,7 +24644,7 @@
       </c>
       <c r="B1293" s="19" t="inlineStr">
         <is>
-          <t>ejecución de cuneta en acera de kosta kalea para canalizar las aguas, posterior colocación de baldosa negra</t>
+          <t>Reparación de fuga de agua en la acometida den centro escolar CEPA Donostia HHI (Julio Urquijo) de Donostia</t>
         </is>
       </c>
       <c r="C1293" s="20" t="n"/>
@@ -24604,7 +24660,7 @@
       </c>
       <c r="B1294" s="19" t="inlineStr">
         <is>
-          <t>EUS-57526</t>
+          <t>EUS-96234</t>
         </is>
       </c>
       <c r="C1294" s="20" t="n"/>
@@ -24756,7 +24812,7 @@
       </c>
       <c r="B1304" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/ejecucion-cuneta-acera-kosta-kalea-canalizar-aguas-posterior-colocacion-baldosa-negra/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/reparacion-fuga-agua-acometida-den-centro-escolar-cepa-donostia-hhi-julio-urquijo-donostia/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1304" s="20" t="n"/>
@@ -24767,7 +24823,7 @@
     <row r="1306" ht="30" customHeight="1">
       <c r="A1306" s="16" t="inlineStr">
         <is>
-          <t>FICHA 88: EUS-99494</t>
+          <t>FICHA 88: EUS-89077</t>
         </is>
       </c>
       <c r="B1306" s="17" t="n"/>
@@ -24800,7 +24856,7 @@
       </c>
       <c r="B1308" s="19" t="inlineStr">
         <is>
-          <t>evitar y redirigir las aguas, así como eliminar las eflorescencias en la acera de kandido saseta</t>
+          <t>Mantenimiento integral de las instalaciones de alumbrado público exterior, navideño, ornamental de ferias y fiestas y semáforos</t>
         </is>
       </c>
       <c r="C1308" s="20" t="n"/>
@@ -24816,7 +24872,7 @@
       </c>
       <c r="B1309" s="19" t="inlineStr">
         <is>
-          <t>EUS-99494</t>
+          <t>EUS-89077</t>
         </is>
       </c>
       <c r="C1309" s="20" t="n"/>
@@ -24968,7 +25024,7 @@
       </c>
       <c r="B1319" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/evitar-y-redirigir-aguas-asi-como-eliminar-eflorescencias-acera-kandido-saseta/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/mantenimiento-integral-instalaciones-alumbrado-publico-exterior-navideno-ornamental-ferias-y-fiestas-y-semaforos/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1319" s="20" t="n"/>
@@ -24979,7 +25035,7 @@
     <row r="1321" ht="30" customHeight="1">
       <c r="A1321" s="16" t="inlineStr">
         <is>
-          <t>FICHA 89: EUS-68529</t>
+          <t>FICHA 89: EUS-75154</t>
         </is>
       </c>
       <c r="B1321" s="17" t="n"/>
@@ -25004,7 +25060,7 @@
       <c r="E1322" s="20" t="n"/>
       <c r="F1322" s="20" t="n"/>
     </row>
-    <row r="1323" ht="20" customHeight="1">
+    <row r="1323" ht="45" customHeight="1">
       <c r="A1323" s="18" t="inlineStr">
         <is>
           <t>Titulo</t>
@@ -25012,7 +25068,7 @@
       </c>
       <c r="B1323" s="19" t="inlineStr">
         <is>
-          <t>proyecto de nuevo edificio de mercado municipal en la parcela de damarri</t>
+          <t>Auscultación geotécnica de la red de infraestructuras viarias de la Diputación Foral de Gipuzkoa (1-O-54/2025)</t>
         </is>
       </c>
       <c r="C1323" s="20" t="n"/>
@@ -25028,7 +25084,7 @@
       </c>
       <c r="B1324" s="19" t="inlineStr">
         <is>
-          <t>EUS-68529</t>
+          <t>EUS-75154</t>
         </is>
       </c>
       <c r="C1324" s="20" t="n"/>
@@ -25180,7 +25236,7 @@
       </c>
       <c r="B1334" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/proyecto-nuevo-edificio-mercado-municipal-parcela-damarri/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/auscultacion-geotecnica-red-infraestructuras-viarias-diputacion-foral-gipuzkoa-1-o-54-2025/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1334" s="20" t="n"/>
@@ -25191,7 +25247,7 @@
     <row r="1336" ht="30" customHeight="1">
       <c r="A1336" s="16" t="inlineStr">
         <is>
-          <t>FICHA 90: EUS-03547</t>
+          <t>FICHA 90: EUS-74501</t>
         </is>
       </c>
       <c r="B1336" s="17" t="n"/>
@@ -25224,7 +25280,7 @@
       </c>
       <c r="B1338" s="19" t="inlineStr">
         <is>
-          <t>renovación de 2 calderas en los vestuarios de la playa</t>
+          <t>Servicio de limpieza viaria</t>
         </is>
       </c>
       <c r="C1338" s="20" t="n"/>
@@ -25240,7 +25296,7 @@
       </c>
       <c r="B1339" s="19" t="inlineStr">
         <is>
-          <t>EUS-03547</t>
+          <t>EUS-74501</t>
         </is>
       </c>
       <c r="C1339" s="20" t="n"/>
@@ -25392,7 +25448,7 @@
       </c>
       <c r="B1349" s="22" t="inlineStr">
         <is>
-          <t>https://www.euskadi.eus/anuncio_contratacion/renovacion-2-calderas-vestuarios-playa/web01-tramite/es/</t>
+          <t>https://www.euskadi.eus/anuncio_contratacion/servicio-limpieza-viaria/expgebizkaia3327143/web01-tramite/es/</t>
         </is>
       </c>
       <c r="C1349" s="20" t="n"/>
@@ -25400,8 +25456,220 @@
       <c r="E1349" s="20" t="n"/>
       <c r="F1349" s="20" t="n"/>
     </row>
+    <row r="1351" ht="30" customHeight="1">
+      <c r="A1351" s="16" t="inlineStr">
+        <is>
+          <t>FICHA 91: EUS-26650</t>
+        </is>
+      </c>
+      <c r="B1351" s="17" t="n"/>
+      <c r="C1351" s="17" t="n"/>
+      <c r="D1351" s="17" t="n"/>
+      <c r="E1351" s="17" t="n"/>
+      <c r="F1351" s="17" t="n"/>
+    </row>
+    <row r="1352" ht="20" customHeight="1">
+      <c r="A1352" s="18" t="inlineStr">
+        <is>
+          <t>Fuente</t>
+        </is>
+      </c>
+      <c r="B1352" s="19" t="inlineStr">
+        <is>
+          <t>🟢 Euskadi</t>
+        </is>
+      </c>
+      <c r="C1352" s="20" t="n"/>
+      <c r="D1352" s="20" t="n"/>
+      <c r="E1352" s="20" t="n"/>
+      <c r="F1352" s="20" t="n"/>
+    </row>
+    <row r="1353" ht="45" customHeight="1">
+      <c r="A1353" s="18" t="inlineStr">
+        <is>
+          <t>Titulo</t>
+        </is>
+      </c>
+      <c r="B1353" s="19" t="inlineStr">
+        <is>
+          <t>Ofrecer los servicios de gestión de reservas, utilización, mantenimiento, y  limpieza del albergue Santiagomendi, así como el servicio de organización de actividades naturales en el medio ambiente.</t>
+        </is>
+      </c>
+      <c r="C1353" s="20" t="n"/>
+      <c r="D1353" s="20" t="n"/>
+      <c r="E1353" s="20" t="n"/>
+      <c r="F1353" s="20" t="n"/>
+    </row>
+    <row r="1354" ht="20" customHeight="1">
+      <c r="A1354" s="18" t="inlineStr">
+        <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1354" s="19" t="inlineStr">
+        <is>
+          <t>EUS-26650</t>
+        </is>
+      </c>
+      <c r="C1354" s="20" t="n"/>
+      <c r="D1354" s="20" t="n"/>
+      <c r="E1354" s="20" t="n"/>
+      <c r="F1354" s="20" t="n"/>
+    </row>
+    <row r="1355" ht="20" customHeight="1">
+      <c r="A1355" s="18" t="inlineStr">
+        <is>
+          <t>Programa</t>
+        </is>
+      </c>
+      <c r="B1355" s="19" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="C1355" s="20" t="n"/>
+      <c r="D1355" s="20" t="n"/>
+      <c r="E1355" s="20" t="n"/>
+      <c r="F1355" s="20" t="n"/>
+    </row>
+    <row r="1356" ht="20" customHeight="1">
+      <c r="A1356" s="18" t="inlineStr">
+        <is>
+          <t>Estado</t>
+        </is>
+      </c>
+      <c r="B1356" s="19" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="C1356" s="20" t="n"/>
+      <c r="D1356" s="20" t="n"/>
+      <c r="E1356" s="20" t="n"/>
+      <c r="F1356" s="20" t="n"/>
+    </row>
+    <row r="1357" ht="20" customHeight="1">
+      <c r="A1357" s="18" t="inlineStr">
+        <is>
+          <t>Deadline</t>
+        </is>
+      </c>
+      <c r="B1357" s="19" t="inlineStr"/>
+      <c r="C1357" s="20" t="n"/>
+      <c r="D1357" s="20" t="n"/>
+      <c r="E1357" s="20" t="n"/>
+      <c r="F1357" s="20" t="n"/>
+    </row>
+    <row r="1358" ht="20" customHeight="1">
+      <c r="A1358" s="18" t="inlineStr">
+        <is>
+          <t>Presupuesto (EUR)</t>
+        </is>
+      </c>
+      <c r="B1358" s="19" t="inlineStr">
+        <is>
+          <t>No disponible</t>
+        </is>
+      </c>
+      <c r="C1358" s="20" t="n"/>
+      <c r="D1358" s="20" t="n"/>
+      <c r="E1358" s="20" t="n"/>
+      <c r="F1358" s="20" t="n"/>
+    </row>
+    <row r="1359" ht="20" customHeight="1">
+      <c r="A1359" s="18" t="inlineStr">
+        <is>
+          <t>Tipo de Accion</t>
+        </is>
+      </c>
+      <c r="B1359" s="19" t="inlineStr">
+        <is>
+          <t>Licitacion Euskadi</t>
+        </is>
+      </c>
+      <c r="C1359" s="20" t="n"/>
+      <c r="D1359" s="20" t="n"/>
+      <c r="E1359" s="20" t="n"/>
+      <c r="F1359" s="20" t="n"/>
+    </row>
+    <row r="1360" ht="20" customHeight="1">
+      <c r="A1360" s="18" t="inlineStr">
+        <is>
+          <t>Call ID</t>
+        </is>
+      </c>
+      <c r="B1360" s="19" t="inlineStr"/>
+      <c r="C1360" s="20" t="n"/>
+      <c r="D1360" s="20" t="n"/>
+      <c r="E1360" s="20" t="n"/>
+      <c r="F1360" s="20" t="n"/>
+    </row>
+    <row r="1361" ht="20" customHeight="1">
+      <c r="A1361" s="18" t="inlineStr">
+        <is>
+          <t>Descripcion</t>
+        </is>
+      </c>
+      <c r="B1361" s="19" t="inlineStr">
+        <is>
+          <t>Gobierno Vasco / Sector Publico Euskadi</t>
+        </is>
+      </c>
+      <c r="C1361" s="20" t="n"/>
+      <c r="D1361" s="20" t="n"/>
+      <c r="E1361" s="20" t="n"/>
+      <c r="F1361" s="20" t="n"/>
+    </row>
+    <row r="1362" ht="20" customHeight="1">
+      <c r="A1362" s="18" t="inlineStr">
+        <is>
+          <t>Tags</t>
+        </is>
+      </c>
+      <c r="B1362" s="19" t="inlineStr">
+        <is>
+          <t>energia</t>
+        </is>
+      </c>
+      <c r="C1362" s="20" t="n"/>
+      <c r="D1362" s="20" t="n"/>
+      <c r="E1362" s="20" t="n"/>
+      <c r="F1362" s="20" t="n"/>
+    </row>
+    <row r="1363" ht="20" customHeight="1">
+      <c r="A1363" s="18" t="inlineStr">
+        <is>
+          <t>Relevancia Bilbao</t>
+        </is>
+      </c>
+      <c r="B1363" s="19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">MEDIA — </t>
+        </is>
+      </c>
+      <c r="C1363" s="20" t="n"/>
+      <c r="D1363" s="20" t="n"/>
+      <c r="E1363" s="20" t="n"/>
+      <c r="F1363" s="20" t="n"/>
+    </row>
+    <row r="1364" ht="45" customHeight="1">
+      <c r="A1364" s="18" t="inlineStr">
+        <is>
+          <t>Enlace al portal</t>
+        </is>
+      </c>
+      <c r="B1364" s="22" t="inlineStr">
+        <is>
+          <t>https://www.euskadi.eus/anuncio_contratacion/ofrecer-servicios-gestion-reservas-utilizacion-mantenimiento-y-limpieza-del-albergue-santiagomendi-asi-como-servicio-organizacion-actividades-naturales-medio-ambiente/web01-tramite/es/</t>
+        </is>
+      </c>
+      <c r="C1364" s="20" t="n"/>
+      <c r="D1364" s="20" t="n"/>
+      <c r="E1364" s="20" t="n"/>
+      <c r="F1364" s="20" t="n"/>
+    </row>
   </sheetData>
-  <mergeCells count="1260">
+  <mergeCells count="1274">
     <mergeCell ref="B679:F679"/>
     <mergeCell ref="B1010:F1010"/>
     <mergeCell ref="B276:F276"/>
@@ -25596,9 +25864,11 @@
     <mergeCell ref="B593:F593"/>
     <mergeCell ref="B1022:F1022"/>
     <mergeCell ref="B1198:F1198"/>
+    <mergeCell ref="B1356:F1356"/>
     <mergeCell ref="B595:F595"/>
     <mergeCell ref="B893:F893"/>
     <mergeCell ref="B1322:F1322"/>
+    <mergeCell ref="B1358:F1358"/>
     <mergeCell ref="B895:F895"/>
     <mergeCell ref="B321:F321"/>
     <mergeCell ref="B1040:F1040"/>
@@ -25650,17 +25920,21 @@
     <mergeCell ref="B281:F281"/>
     <mergeCell ref="B1033:F1033"/>
     <mergeCell ref="B1333:F1333"/>
+    <mergeCell ref="B1362:F1362"/>
     <mergeCell ref="B759:F759"/>
     <mergeCell ref="B1057:F1057"/>
     <mergeCell ref="B1093:F1093"/>
+    <mergeCell ref="B1364:F1364"/>
     <mergeCell ref="B332:F332"/>
     <mergeCell ref="B937:F937"/>
     <mergeCell ref="B1059:F1059"/>
     <mergeCell ref="B1086:F1086"/>
+    <mergeCell ref="B1357:F1357"/>
     <mergeCell ref="B632:F632"/>
     <mergeCell ref="B175:F175"/>
     <mergeCell ref="B790:F790"/>
     <mergeCell ref="B1088:F1088"/>
+    <mergeCell ref="B1359:F1359"/>
     <mergeCell ref="A1291:F1291"/>
     <mergeCell ref="B806:F806"/>
     <mergeCell ref="B1077:F1077"/>
@@ -25744,6 +26018,7 @@
     <mergeCell ref="B83:F83"/>
     <mergeCell ref="B85:F85"/>
     <mergeCell ref="B383:F383"/>
+    <mergeCell ref="B1355:F1355"/>
     <mergeCell ref="B141:F141"/>
     <mergeCell ref="B439:F439"/>
     <mergeCell ref="B985:F985"/>
@@ -25807,6 +26082,7 @@
     <mergeCell ref="B883:F883"/>
     <mergeCell ref="B1208:F1208"/>
     <mergeCell ref="B207:F207"/>
+    <mergeCell ref="B1353:F1353"/>
     <mergeCell ref="B636:F636"/>
     <mergeCell ref="B296:F296"/>
     <mergeCell ref="B934:F934"/>
@@ -26089,6 +26365,7 @@
     <mergeCell ref="B277:F277"/>
     <mergeCell ref="B575:F575"/>
     <mergeCell ref="B873:F873"/>
+    <mergeCell ref="B1363:F1363"/>
     <mergeCell ref="A1111:F1111"/>
     <mergeCell ref="B170:F170"/>
     <mergeCell ref="B328:F328"/>
@@ -26139,6 +26416,7 @@
     <mergeCell ref="B1018:F1018"/>
     <mergeCell ref="B624:F624"/>
     <mergeCell ref="B1316:F1316"/>
+    <mergeCell ref="B1354:F1354"/>
     <mergeCell ref="B284:F284"/>
     <mergeCell ref="B415:F415"/>
     <mergeCell ref="B713:F713"/>
@@ -26393,6 +26671,7 @@
     <mergeCell ref="A481:F481"/>
     <mergeCell ref="B1026:F1026"/>
     <mergeCell ref="B1324:F1324"/>
+    <mergeCell ref="B1360:F1360"/>
     <mergeCell ref="B599:F599"/>
     <mergeCell ref="B1028:F1028"/>
     <mergeCell ref="B1055:F1055"/>
@@ -26408,6 +26687,7 @@
     <mergeCell ref="B923:F923"/>
     <mergeCell ref="B1054:F1054"/>
     <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B1352:F1352"/>
     <mergeCell ref="B320:F320"/>
     <mergeCell ref="B1083:F1083"/>
     <mergeCell ref="B38:F38"/>
@@ -26463,6 +26743,7 @@
     <mergeCell ref="B792:F792"/>
     <mergeCell ref="B1063:F1063"/>
     <mergeCell ref="B1090:F1090"/>
+    <mergeCell ref="B1361:F1361"/>
     <mergeCell ref="B1221:F1221"/>
     <mergeCell ref="B39:F39"/>
     <mergeCell ref="B1092:F1092"/>
@@ -26619,6 +26900,7 @@
     <mergeCell ref="A466:F466"/>
     <mergeCell ref="B867:F867"/>
     <mergeCell ref="B1296:F1296"/>
+    <mergeCell ref="A1351:F1351"/>
     <mergeCell ref="B251:F251"/>
     <mergeCell ref="B1014:F1014"/>
     <mergeCell ref="B1008:F1008"/>
@@ -26754,6 +27036,7 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1319" r:id="rId88"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1334" r:id="rId89"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1349" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B1364" r:id="rId91"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -26765,7 +27048,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J91"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -29293,7 +29576,7 @@
     <row r="66" ht="28" customHeight="1">
       <c r="A66" s="6" t="inlineStr">
         <is>
-          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
+          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
         </is>
       </c>
       <c r="B66" s="6" t="inlineStr">
@@ -29325,7 +29608,7 @@
     <row r="67" ht="28" customHeight="1">
       <c r="A67" s="6" t="inlineStr">
         <is>
-          <t>dc0033a0-cb94-44ed-8102-0fd0a386989e-EXA</t>
+          <t>4b45d249-5739-4bf7-9595-a4715b73c2f6-EXA</t>
         </is>
       </c>
       <c r="B67" s="6" t="inlineStr">
@@ -29389,12 +29672,12 @@
     <row r="69" ht="28" customHeight="1">
       <c r="A69" s="6" t="inlineStr">
         <is>
-          <t>EUS-01513</t>
+          <t>EUS-37980</t>
         </is>
       </c>
       <c r="B69" s="6" t="inlineStr">
         <is>
-          <t>Mantenimiento de cubiertas en los centros de Bilbao Kirolak</t>
+          <t xml:space="preserve">Ayudas a proyectos al amparo de la estrategia de desarrollo </t>
         </is>
       </c>
       <c r="C69" s="6" t="inlineStr">
@@ -29410,7 +29693,7 @@
       <c r="E69" s="6" t="inlineStr"/>
       <c r="F69" s="25" t="inlineStr">
         <is>
-          <t>MUY ALTA</t>
+          <t>ALTA</t>
         </is>
       </c>
       <c r="G69" s="6" t="inlineStr"/>
@@ -29425,12 +29708,12 @@
     <row r="70" ht="28" customHeight="1">
       <c r="A70" s="6" t="inlineStr">
         <is>
-          <t>EUS-46570</t>
+          <t>EUS-88998</t>
         </is>
       </c>
       <c r="B70" s="6" t="inlineStr">
         <is>
-          <t xml:space="preserve">Ayudas a proyectos al amparo de la estrategia de desarrollo </t>
+          <t>ReSourceEU y materias primas críticas: la UE sigue tramitand</t>
         </is>
       </c>
       <c r="C70" s="6" t="inlineStr">
@@ -29461,12 +29744,12 @@
     <row r="71" ht="28" customHeight="1">
       <c r="A71" s="6" t="inlineStr">
         <is>
-          <t>EUS-20748</t>
+          <t>EUS-22037</t>
         </is>
       </c>
       <c r="B71" s="6" t="inlineStr">
         <is>
-          <t>ReSourceEU y materias primas críticas: la UE sigue tramitand</t>
+          <t>Ciudades sostenibles: los Premios Capital Verde Europea y Ho</t>
         </is>
       </c>
       <c r="C71" s="6" t="inlineStr">
@@ -29497,12 +29780,12 @@
     <row r="72" ht="28" customHeight="1">
       <c r="A72" s="6" t="inlineStr">
         <is>
-          <t>EUS-33329</t>
+          <t>EUS-96198</t>
         </is>
       </c>
       <c r="B72" s="6" t="inlineStr">
         <is>
-          <t>Ciudades sostenibles: los Premios Capital Verde Europea y Ho</t>
+          <t>Presolicitud para programa de ayudas a empresas que realicen</t>
         </is>
       </c>
       <c r="C72" s="6" t="inlineStr">
@@ -29533,12 +29816,12 @@
     <row r="73" ht="28" customHeight="1">
       <c r="A73" s="6" t="inlineStr">
         <is>
-          <t>EUS-46971</t>
+          <t>EUS-18212</t>
         </is>
       </c>
       <c r="B73" s="6" t="inlineStr">
         <is>
-          <t>Presolicitud para programa de ayudas a empresas que realicen</t>
+          <t>Servicio integral de gestión operativa de movilidad que de s</t>
         </is>
       </c>
       <c r="C73" s="6" t="inlineStr">
@@ -29569,7 +29852,7 @@
     <row r="74" ht="28" customHeight="1">
       <c r="A74" s="6" t="inlineStr">
         <is>
-          <t>EUS-23727</t>
+          <t>EUS-35207</t>
         </is>
       </c>
       <c r="B74" s="6" t="inlineStr">
@@ -29605,7 +29888,7 @@
     <row r="75" ht="28" customHeight="1">
       <c r="A75" s="6" t="inlineStr">
         <is>
-          <t>EUS-63736</t>
+          <t>EUS-04351</t>
         </is>
       </c>
       <c r="B75" s="6" t="inlineStr">
@@ -29641,7 +29924,7 @@
     <row r="76" ht="28" customHeight="1">
       <c r="A76" s="6" t="inlineStr">
         <is>
-          <t>EUS-38314</t>
+          <t>EUS-41297</t>
         </is>
       </c>
       <c r="B76" s="6" t="inlineStr">
@@ -29677,7 +29960,7 @@
     <row r="77" ht="28" customHeight="1">
       <c r="A77" s="6" t="inlineStr">
         <is>
-          <t>EUS-43135</t>
+          <t>EUS-78717</t>
         </is>
       </c>
       <c r="B77" s="6" t="inlineStr">
@@ -29713,7 +29996,7 @@
     <row r="78" ht="28" customHeight="1">
       <c r="A78" s="6" t="inlineStr">
         <is>
-          <t>EUS-00654</t>
+          <t>EUS-25588</t>
         </is>
       </c>
       <c r="B78" s="6" t="inlineStr">
@@ -29749,7 +30032,7 @@
     <row r="79" ht="28" customHeight="1">
       <c r="A79" s="6" t="inlineStr">
         <is>
-          <t>EUS-24940</t>
+          <t>EUS-33200</t>
         </is>
       </c>
       <c r="B79" s="6" t="inlineStr">
@@ -29785,7 +30068,7 @@
     <row r="80" ht="28" customHeight="1">
       <c r="A80" s="6" t="inlineStr">
         <is>
-          <t>EUS-30791</t>
+          <t>EUS-47048</t>
         </is>
       </c>
       <c r="B80" s="6" t="inlineStr">
@@ -29821,7 +30104,7 @@
     <row r="81" ht="28" customHeight="1">
       <c r="A81" s="6" t="inlineStr">
         <is>
-          <t>EUS-01008</t>
+          <t>EUS-74734</t>
         </is>
       </c>
       <c r="B81" s="6" t="inlineStr">
@@ -29857,7 +30140,7 @@
     <row r="82" ht="28" customHeight="1">
       <c r="A82" s="6" t="inlineStr">
         <is>
-          <t>EUS-10663</t>
+          <t>EUS-60281</t>
         </is>
       </c>
       <c r="B82" s="6" t="inlineStr">
@@ -29893,7 +30176,7 @@
     <row r="83" ht="28" customHeight="1">
       <c r="A83" s="6" t="inlineStr">
         <is>
-          <t>EUS-56941</t>
+          <t>EUS-54283</t>
         </is>
       </c>
       <c r="B83" s="6" t="inlineStr">
@@ -29929,7 +30212,7 @@
     <row r="84" ht="28" customHeight="1">
       <c r="A84" s="6" t="inlineStr">
         <is>
-          <t>EUS-01208</t>
+          <t>EUS-10026</t>
         </is>
       </c>
       <c r="B84" s="6" t="inlineStr">
@@ -29965,7 +30248,7 @@
     <row r="85" ht="28" customHeight="1">
       <c r="A85" s="6" t="inlineStr">
         <is>
-          <t>EUS-00233</t>
+          <t>EUS-35931</t>
         </is>
       </c>
       <c r="B85" s="6" t="inlineStr">
@@ -30001,7 +30284,7 @@
     <row r="86" ht="28" customHeight="1">
       <c r="A86" s="6" t="inlineStr">
         <is>
-          <t>EUS-15421</t>
+          <t>EUS-44255</t>
         </is>
       </c>
       <c r="B86" s="6" t="inlineStr">
@@ -30037,7 +30320,7 @@
     <row r="87" ht="28" customHeight="1">
       <c r="A87" s="6" t="inlineStr">
         <is>
-          <t>EUS-74016</t>
+          <t>EUS-75900</t>
         </is>
       </c>
       <c r="B87" s="6" t="inlineStr">
@@ -30073,12 +30356,12 @@
     <row r="88" ht="28" customHeight="1">
       <c r="A88" s="6" t="inlineStr">
         <is>
-          <t>EUS-57526</t>
+          <t>EUS-96234</t>
         </is>
       </c>
       <c r="B88" s="6" t="inlineStr">
         <is>
-          <t>ejecución de cuneta en acera de kosta kalea para canalizar l</t>
+          <t>Reparación de fuga de agua en la acometida den centro escola</t>
         </is>
       </c>
       <c r="C88" s="6" t="inlineStr">
@@ -30109,12 +30392,12 @@
     <row r="89" ht="28" customHeight="1">
       <c r="A89" s="6" t="inlineStr">
         <is>
-          <t>EUS-99494</t>
+          <t>EUS-89077</t>
         </is>
       </c>
       <c r="B89" s="6" t="inlineStr">
         <is>
-          <t>evitar y redirigir las aguas, así como eliminar las efloresc</t>
+          <t>Mantenimiento integral de las instalaciones de alumbrado púb</t>
         </is>
       </c>
       <c r="C89" s="6" t="inlineStr">
@@ -30145,12 +30428,12 @@
     <row r="90" ht="28" customHeight="1">
       <c r="A90" s="6" t="inlineStr">
         <is>
-          <t>EUS-68529</t>
+          <t>EUS-75154</t>
         </is>
       </c>
       <c r="B90" s="6" t="inlineStr">
         <is>
-          <t>proyecto de nuevo edificio de mercado municipal en la parcel</t>
+          <t>Auscultación geotécnica de la red de infraestructuras viaria</t>
         </is>
       </c>
       <c r="C90" s="6" t="inlineStr">
@@ -30181,12 +30464,12 @@
     <row r="91" ht="28" customHeight="1">
       <c r="A91" s="6" t="inlineStr">
         <is>
-          <t>EUS-03547</t>
+          <t>EUS-74501</t>
         </is>
       </c>
       <c r="B91" s="6" t="inlineStr">
         <is>
-          <t>renovación de 2 calderas en los vestuarios de la playa</t>
+          <t>Servicio de limpieza viaria</t>
         </is>
       </c>
       <c r="C91" s="6" t="inlineStr">
@@ -30214,8 +30497,44 @@
       <c r="I91" s="6" t="inlineStr"/>
       <c r="J91" s="6" t="inlineStr"/>
     </row>
+    <row r="92" ht="28" customHeight="1">
+      <c r="A92" s="6" t="inlineStr">
+        <is>
+          <t>EUS-26650</t>
+        </is>
+      </c>
+      <c r="B92" s="6" t="inlineStr">
+        <is>
+          <t>Ofrecer los servicios de gestión de reservas, utilización, m</t>
+        </is>
+      </c>
+      <c r="C92" s="6" t="inlineStr">
+        <is>
+          <t>Euskadi</t>
+        </is>
+      </c>
+      <c r="D92" s="6" t="inlineStr">
+        <is>
+          <t>Open</t>
+        </is>
+      </c>
+      <c r="E92" s="6" t="inlineStr"/>
+      <c r="F92" s="25" t="inlineStr">
+        <is>
+          <t>MEDIA</t>
+        </is>
+      </c>
+      <c r="G92" s="6" t="inlineStr"/>
+      <c r="H92" s="6" t="inlineStr">
+        <is>
+          <t>Por revisar</t>
+        </is>
+      </c>
+      <c r="I92" s="6" t="inlineStr"/>
+      <c r="J92" s="6" t="inlineStr"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J91"/>
+  <autoFilter ref="A1:J92"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>

</xml_diff>